<commit_message>
trained on full train data
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -42,11 +42,22 @@
 Trained on datasubset</t>
   </si>
   <si>
-    <t xml:space="preserve">Epoch 1 finished | Train Loss: 0.452 | Valid Loss: 0.271 | Combined metric: 0.574 | Dice: 0.179 (LB 0.505, SB 0.236, S 0.236) | Hausdorff: 0.162 (LB 0.153, SB 0.095, S 0.239)
-Epoch 2 finished | Train Loss: 0.167 | Valid Loss: 0.280 | Combined metric: 0.540 | Dice: 0.205 (LB 0.499, SB 0.285, S 0.147) | Hausdorff: 0.237 (LB 0.194, SB 0.160, S 0.357)
-Epoch 3 finished | Train Loss: 0.114 | Valid Loss: 0.181 | Combined metric: 0.616 | Dice: 0.241 (LB 0.622, SB 0.207, S 0.561) | Hausdorff: 0.135 (LB 0.174, SB 0.099, S 0.131)
-Epoch 4 finished | Train Loss: 0.091 | Valid Loss: 0.167 | Combined metric: 0.636 | Dice: 0.255 (LB 0.648, SB 0.265, S 0.578) | Hausdorff: 0.110 (LB 0.126, SB 0.132, S 0.072)
-Epoch 5 finished | Train Loss: 0.079 | Valid Loss: 0.170 | Combined metric: 0.646 | Dice: 0.253 (LB 0.649, SB 0.237, S 0.605) | Hausdorff: 0.091 (LB 0.083, SB 0.089, S 0.101)</t>
+    <t xml:space="preserve">Epoch 1 | Train Loss: 0.452 | Valid Loss: 0.271 | Combined metric: 0.574 | Dice: 0.179 (LB 0.505, SB 0.236, S 0.236) | Hausdorff: 0.162 (LB 0.153, SB 0.095, S 0.239)
+Epoch 2 | Train Loss: 0.167 | Valid Loss: 0.280 | Combined metric: 0.540 | Dice: 0.205 (LB 0.499, SB 0.285, S 0.147) | Hausdorff: 0.237 (LB 0.194, SB 0.160, S 0.357)
+Epoch 3 | Train Loss: 0.114 | Valid Loss: 0.181 | Combined metric: 0.616 | Dice: 0.241 (LB 0.622, SB 0.207, S 0.561) | Hausdorff: 0.135 (LB 0.174, SB 0.099, S 0.131)
+Epoch 4 | Train Loss: 0.091 | Valid Loss: 0.167 | Combined metric: 0.636 | Dice: 0.255 (LB 0.648, SB 0.265, S 0.578) | Hausdorff: 0.110 (LB 0.126, SB 0.132, S 0.072)
+Epoch 5 | Train Loss: 0.079 | Valid Loss: 0.170 | Combined metric: 0.646 | Dice: 0.253 (LB 0.649, SB 0.237, S 0.605) | Hausdorff: 0.091 (LB 0.083, SB 0.089, S 0.101)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unet Efficientnet-b1 
+Trained on full train data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 1 | Train Loss: 0.203 | Valid Loss: 0.123 | Combined metric: 0.654 | Dice: 0.292 (LB 0.675, SB 0.506, S 0.660) | Hausdorff: 0.104 (LB 0.093, SB 0.164, S 0.054)
+Epoch 2 | Train Loss: 0.108 | Valid Loss: 0.114 | Combined metric: 0.671 | Dice: 0.304 (LB 0.688, SB 0.566, S 0.693) | Hausdorff: 0.084 (LB 0.108, SB 0.073, S 0.071)
+Epoch 3 | Train Loss: 0.096 | Valid Loss: 0.110 | Combined metric: 0.653 | Dice: 0.304 (LB 0.612, SB 0.565, S 0.694) | Hausdorff: 0.115 (LB 0.214, SB 0.076, S 0.054)
+Epoch 4 | Train Loss: 0.087 | Valid Loss: 0.115 | Combined metric: 0.668 | Dice: 0.300 (LB 0.687, SB 0.524, S 0.670) | Hausdorff: 0.087 (LB 0.109, SB 0.096, S 0.057)
+Epoch 5 | Train Loss: 0.081 | Valid Loss: 0.107 | Combined metric: 0.689 | Dice: 0.311 (LB 0.703, SB 0.581, S 0.728) | Hausdorff: 0.060 (LB 0.068, SB 0.065, S 0.047)</t>
   </si>
 </sst>
 </file>
@@ -266,10 +277,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -314,6 +325,23 @@
         <v>0.75162</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.689</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.82808</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.81848</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
precreate masks and train with 224x224
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -39,25 +39,87 @@
   </si>
   <si>
     <t xml:space="preserve">Unet Efficientnet-b1 
-Trained on datasubset</t>
+Trained on datasubset
+(288x288)</t>
   </si>
   <si>
     <t xml:space="preserve">Epoch 1 | Train Loss: 0.452 | Valid Loss: 0.271 | Combined metric: 0.574 | Dice: 0.179 (LB 0.505, SB 0.236, S 0.236) | Hausdorff: 0.162 (LB 0.153, SB 0.095, S 0.239)
 Epoch 2 | Train Loss: 0.167 | Valid Loss: 0.280 | Combined metric: 0.540 | Dice: 0.205 (LB 0.499, SB 0.285, S 0.147) | Hausdorff: 0.237 (LB 0.194, SB 0.160, S 0.357)
 Epoch 3 | Train Loss: 0.114 | Valid Loss: 0.181 | Combined metric: 0.616 | Dice: 0.241 (LB 0.622, SB 0.207, S 0.561) | Hausdorff: 0.135 (LB 0.174, SB 0.099, S 0.131)
 Epoch 4 | Train Loss: 0.091 | Valid Loss: 0.167 | Combined metric: 0.636 | Dice: 0.255 (LB 0.648, SB 0.265, S 0.578) | Hausdorff: 0.110 (LB 0.126, SB 0.132, S 0.072)
-Epoch 5 | Train Loss: 0.079 | Valid Loss: 0.170 | Combined metric: 0.646 | Dice: 0.253 (LB 0.649, SB 0.237, S 0.605) | Hausdorff: 0.091 (LB 0.083, SB 0.089, S 0.101)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unet Efficientnet-b1 
-Trained on full train data</t>
+Epoch 5 | Train Loss: 0.079 | Valid Loss: 0.170 | Combined metric: 0.646 | Dice: 0.253 (LB 0.649, SB 0.237, S 0.605) | Hausdorff: 0.091 (LB 0.083, SB 0.089, S 0.101)
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Unet Efficientnet-b1 
+Trained on full train data
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(288x288)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Epoch 1 | Train Loss: 0.203 | Valid Loss: 0.123 | Combined metric: 0.654 | Dice: 0.292 (LB 0.675, SB 0.506, S 0.660) | Hausdorff: 0.104 (LB 0.093, SB 0.164, S 0.054)
 Epoch 2 | Train Loss: 0.108 | Valid Loss: 0.114 | Combined metric: 0.671 | Dice: 0.304 (LB 0.688, SB 0.566, S 0.693) | Hausdorff: 0.084 (LB 0.108, SB 0.073, S 0.071)
 Epoch 3 | Train Loss: 0.096 | Valid Loss: 0.110 | Combined metric: 0.653 | Dice: 0.304 (LB 0.612, SB 0.565, S 0.694) | Hausdorff: 0.115 (LB 0.214, SB 0.076, S 0.054)
 Epoch 4 | Train Loss: 0.087 | Valid Loss: 0.115 | Combined metric: 0.668 | Dice: 0.300 (LB 0.687, SB 0.524, S 0.670) | Hausdorff: 0.087 (LB 0.109, SB 0.096, S 0.057)
-Epoch 5 | Train Loss: 0.081 | Valid Loss: 0.107 | Combined metric: 0.689 | Dice: 0.311 (LB 0.703, SB 0.581, S 0.728) | Hausdorff: 0.060 (LB 0.068, SB 0.065, S 0.047)</t>
+Epoch 5 | Train Loss: 0.081 | Valid Loss: 0.107 | Combined metric: 0.689 | Dice: 0.311 (LB 0.703, SB 0.581, S 0.728) | Hausdorff: 0.060 (LB 0.068, SB 0.065, S 0.047)
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Unet Efficientnet-b1 
+Trained on full train data
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(256x256)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 1 | Train Loss: 0.211 | Valid Loss: 0.139 | Combined metric: 0.658 | Dice: 0.291 (LB 0.588, SB 0.433, S 0.600) | Hausdorff: 0.097 (LB 0.105, SB 0.111, S 0.075)
+Epoch 2 | Train Loss: 0.110 | Valid Loss: 0.129 | Combined metric: 0.657 | Dice: 0.285 (LB 0.650, SB 0.486, S 0.654) | Hausdorff: 0.095 (LB 0.130, SB 0.097, S 0.056)
+Epoch 3 | Train Loss: 0.098 | Valid Loss: 0.124 | Combined metric: 0.609 | Dice: 0.297 (LB 0.583, SB 0.393, S 0.611) | Hausdorff: 0.183 (LB 0.217, SB 0.231, S 0.100)
+Epoch 4 | Train Loss: 0.089 | Valid Loss: 0.122 | Combined metric: 0.677 | Dice: 0.297 (LB 0.687, SB 0.558, S 0.651) | Hausdorff: 0.070 (LB 0.068, SB 0.069, S 0.071)
+Epoch 5 | Train Loss: 0.083 | Valid Loss: 0.109 | Combined metric: 0.668 | Dice: 0.306 (LB 0.686, SB 0.569, S 0.685) | Hausdorff: 0.090 (LB 0.097, SB 0.119, S 0.055)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unet Efficientnet-b1 
+Trained on full train data
+(224x224)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 1 | Train Loss: 0.210 | Valid Loss: 0.125 | Combined metric: 0.662 | Dice: 0.295 (LB 0.659, SB 0.527, S 0.623) | Hausdorff: 0.093 (LB 0.140, SB 0.072, S 0.068)
+Epoch 2 | Train Loss: 0.111 | Valid Loss: 0.126 | Combined metric: 0.666 | Dice: 0.294 (LB 0.663, SB 0.545, S 0.615) | Hausdorff: 0.085 (LB 0.076, SB 0.115, S 0.065)
+Epoch 3 | Train Loss: 0.098 | Valid Loss: 0.115 | Combined metric: 0.682 | Dice: 0.303 (LB 0.691, SB 0.565, S 0.690) | Hausdorff: 0.066 (LB 0.078, SB 0.070, S 0.050)
+Epoch 4 | Train Loss: 0.088 | Valid Loss: 0.127 | Combined metric: 0.660 | Dice: 0.282 (LB 0.660, SB 0.520, S 0.659) | Hausdorff: 0.088 (LB 0.060, SB 0.136, S 0.068)
+Epoch 5 | Train Loss: 0.085 | Valid Loss: 0.109 | Combined metric: 0.682 | Dice: 0.315 (LB 0.687, SB 0.564, S 0.699) | Hausdorff: 0.073 (LB 0.075, SB 0.102, S 0.041)
+</t>
   </si>
 </sst>
 </file>
@@ -67,11 +129,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -90,6 +153,12 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -137,20 +206,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -277,69 +354,103 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="141.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="141.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.23"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>0.646</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0.76843</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>0.75162</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0.689</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.82808</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>0.81848</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.668</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.8153</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.80775</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0.682</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0.82298</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.81752</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pad if needed  test submission results
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -51,25 +51,9 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Unet Efficientnet-b1 
+    <t xml:space="preserve">Unet Efficientnet-b1 
 Trained on full train data
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(288x288)</t>
-    </r>
+(288x288)</t>
   </si>
   <si>
     <t xml:space="preserve">Epoch 1 | Train Loss: 0.203 | Valid Loss: 0.123 | Combined metric: 0.654 | Dice: 0.292 (LB 0.675, SB 0.506, S 0.660) | Hausdorff: 0.104 (LB 0.093, SB 0.164, S 0.054)
@@ -80,25 +64,9 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Unet Efficientnet-b1 
+    <t xml:space="preserve">Unet Efficientnet-b1 
 Trained on full train data
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(256x256)</t>
-    </r>
+(256x256)</t>
   </si>
   <si>
     <t xml:space="preserve">Epoch 1 | Train Loss: 0.211 | Valid Loss: 0.139 | Combined metric: 0.658 | Dice: 0.291 (LB 0.588, SB 0.433, S 0.600) | Hausdorff: 0.097 (LB 0.105, SB 0.111, S 0.075)
@@ -120,6 +88,18 @@
 Epoch 4 | Train Loss: 0.088 | Valid Loss: 0.127 | Combined metric: 0.660 | Dice: 0.282 (LB 0.660, SB 0.520, S 0.659) | Hausdorff: 0.088 (LB 0.060, SB 0.136, S 0.068)
 Epoch 5 | Train Loss: 0.085 | Valid Loss: 0.109 | Combined metric: 0.682 | Dice: 0.315 (LB 0.687, SB 0.564, S 0.699) | Hausdorff: 0.073 (LB 0.075, SB 0.102, S 0.041)
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unet Efficientnet-b1 
+Trained on full train data
+(padif needed + 224x224 resize)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 1 | Train Loss: 0.213 | Valid Loss: 0.126 | Combined metric: 0.664 | Dice: 0.298 (LB 0.649, SB 0.492, S 0.633) | Hausdorff: 0.092 (LB 0.103, SB 0.091, S 0.081)
+Epoch 2 | Train Loss: 0.113 | Valid Loss: 0.136 | Combined metric: 0.659 | Dice: 0.272 (LB 0.663, SB 0.495, S 0.594) | Hausdorff: 0.083 (LB 0.096, SB 0.086, S 0.066)
+Epoch 3 | Train Loss: 0.098 | Valid Loss: 0.124 | Combined metric: 0.648 | Dice: 0.286 (LB 0.668, SB 0.513, S 0.651) | Hausdorff: 0.111 (LB 0.123, SB 0.111, S 0.099)
+Epoch 4 | Train Loss: 0.089 | Valid Loss: 0.140 | Combined metric: 0.650 | Dice: 0.269 (LB 0.619, SB 0.482, S 0.592) | Hausdorff: 0.095 (LB 0.103, SB 0.075, S 0.108)
+Epoch 5 | Train Loss: 0.086 | Valid Loss: 0.116 | Combined metric: 0.685 | Dice: 0.302 (LB 0.662, SB 0.563, S 0.706) | Hausdorff: 0.059 (LB 0.074, SB 0.063, S 0.040)</t>
   </si>
 </sst>
 </file>
@@ -129,7 +109,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -158,11 +138,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,7 +181,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -224,10 +199,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -354,10 +325,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -432,12 +403,12 @@
       <c r="D4" s="1" t="n">
         <v>0.8153</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>0.80775</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -449,8 +420,25 @@
       <c r="D5" s="1" t="n">
         <v>0.82298</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>0.81752</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0.685</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0.79655</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.78819</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scores from training on different folds
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -100,6 +100,75 @@
 Epoch 3 | Train Loss: 0.098 | Valid Loss: 0.124 | Combined metric: 0.648 | Dice: 0.286 (LB 0.668, SB 0.513, S 0.651) | Hausdorff: 0.111 (LB 0.123, SB 0.111, S 0.099)
 Epoch 4 | Train Loss: 0.089 | Valid Loss: 0.140 | Combined metric: 0.650 | Dice: 0.269 (LB 0.619, SB 0.482, S 0.592) | Hausdorff: 0.095 (LB 0.103, SB 0.075, S 0.108)
 Epoch 5 | Train Loss: 0.086 | Valid Loss: 0.116 | Combined metric: 0.685 | Dice: 0.302 (LB 0.662, SB 0.563, S 0.706) | Hausdorff: 0.059 (LB 0.074, SB 0.063, S 0.040)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unet Efficientnet-b1 
+Trained on full train data
+(224x224)
+Batch size 64, with AMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 1 | Train Loss: 0.258 | Valid Loss: 0.166 | Combined metric: 0.661 | Dice: 0.289 (LB 0.627, SB 0.504, S 0.567) | Hausdorff: 0.092 (LB 0.108, SB 0.082, S 0.085)
+Epoch 2 | Train Loss: 0.107 | Valid Loss: 0.176 | Combined metric: 0.615 | Dice: 0.270 (LB 0.513, SB 0.522, S 0.595) | Hausdorff: 0.155 (LB 0.304, SB 0.109, S 0.051)
+Epoch 3 | Train Loss: 0.093 | Valid Loss: 0.162 | Combined metric: 0.628 | Dice: 0.272 (LB 0.614, SB 0.467, S 0.627) | Hausdorff: 0.135 (LB 0.175, SB 0.085, S 0.145)
+Epoch 4 | Train Loss: 0.086 | Valid Loss: 0.140 | Combined metric: 0.656 | Dice: 0.305 (LB 0.657, SB 0.549, S 0.645) | Hausdorff: 0.110 (LB 0.174, SB 0.074, S 0.082)
+Epoch 5 | Train Loss: 0.078 | Valid Loss: 0.139 | Combined metric: 0.675 | Dice: 0.303 (LB 0.670, SB 0.532, S 0.682) | Hausdorff: 0.076 (LB 0.096, SB 0.080, S 0.053)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unet Efficientnet-b1 
+Trained on full train data
+(224x224)
+Batch size 64, with AMP
+Fold 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 1 | Train Loss: 0.252 | Valid Loss: 0.186 | Combined metric: 0.647 | Dice: 0.228 (LB 0.587, SB 0.450, S 0.613) | Hausdorff: 0.074 (LB 0.081, SB 0.068, S 0.073)
+Epoch 2 | Train Loss: 0.106 | Valid Loss: 0.200 | Combined metric: 0.629 | Dice: 0.221 (LB 0.570, SB 0.395, S 0.590) | Hausdorff: 0.099 (LB 0.082, SB 0.072, S 0.144)
+Epoch 3 | Train Loss: 0.091 | Valid Loss: 0.235 | Combined metric: 0.567 | Dice: 0.205 (LB 0.216, SB 0.467, S 0.611) | Hausdorff: 0.191 (LB 0.331, SB 0.195, S 0.048)
+Epoch 4 | Train Loss: 0.083 | Valid Loss: 0.159 | Combined metric: 0.654 | Dice: 0.249 (LB 0.643, SB 0.519, S 0.662) | Hausdorff: 0.076 (LB 0.076, SB 0.088, S 0.065)
+Epoch 5 | Train Loss: 0.076 | Valid Loss: 0.165 | Combined metric: 0.646 | Dice: 0.251 (LB 0.615, SB 0.504, S 0.624) | Hausdorff: 0.090 (LB 0.112, SB 0.090, S 0.069)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unet Efficientnet-b1 
+Trained on full train data
+(224x224)
+Batch size 64, with AMP
+Fold 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 1 | Train Loss: 0.260 | Valid Loss: 0.151 | Combined metric: 0.650 | Dice: 0.286 (LB 0.638, SB 0.499, S 0.649) | Hausdorff: 0.108 (LB 0.113, SB 0.123, S 0.087)
+Epoch 2 | Train Loss: 0.106 | Valid Loss: 0.142 | Combined metric: 0.675 | Dice: 0.298 (LB 0.648, SB 0.535, S 0.663) | Hausdorff: 0.074 (LB 0.100, SB 0.083, S 0.039)
+Epoch 3 | Train Loss: 0.092 | Valid Loss: 0.128 | Combined metric: 0.673 | Dice: 0.303 (LB 0.701, SB 0.576, S 0.693) | Hausdorff: 0.081 (LB 0.075, SB 0.087, S 0.080)
+Epoch 4 | Train Loss: 0.084 | Valid Loss: 0.135 | Combined metric: 0.680 | Dice: 0.302 (LB 0.670, SB 0.545, S 0.692) | Hausdorff: 0.068 (LB 0.078, SB 0.079, S 0.048)
+Epoch 5 | Train Loss: 0.077 | Valid Loss: 0.155 | Combined metric: 0.672 | Dice: 0.276 (LB 0.638, SB 0.534, S 0.695) | Hausdorff: 0.064 (LB 0.054, SB 0.068, S 0.069)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unet Efficientnet-b1 
+Trained on full train data
+(224x224)
+Batch size 64, with AMP
+Fold 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 1 | Train Loss: 0.248 | Valid Loss: 0.189 | Combined metric: 0.593 | Dice: 0.244 (LB 0.587, SB 0.463, S 0.399) | Hausdorff: 0.175 (LB 0.176, SB 0.125, S 0.222)
+Epoch 2 | Train Loss: 0.104 | Valid Loss: 0.176 | Combined metric: 0.652 | Dice: 0.263 (LB 0.641, SB 0.491, S 0.579) | Hausdorff: 0.088 (LB 0.095, SB 0.124, S 0.046)
+Epoch 3 | Train Loss: 0.090 | Valid Loss: 0.155 | Combined metric: 0.633 | Dice: 0.273 (LB 0.657, SB 0.485, S 0.651) | Hausdorff: 0.126 (LB 0.120, SB 0.177, S 0.083)
+Epoch 4 | Train Loss: 0.080 | Valid Loss: 0.154 | Combined metric: 0.657 | Dice: 0.282 (LB 0.662, SB 0.532, S 0.639) | Hausdorff: 0.093 (LB 0.095, SB 0.111, S 0.073)
+Epoch 5 | Train Loss: 0.074 | Valid Loss: 0.160 | Combined metric: 0.639 | Dice: 0.279 (LB 0.641, SB 0.521, S 0.614) | Hausdorff: 0.121 (LB 0.154, SB 0.086, S 0.123)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unet Efficientnet-b1 
+Trained on full train data
+(224x224)
+Batch size 64, with AMP
+Fold 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 1 | Train Loss: 0.261 | Valid Loss: 0.165 | Combined metric: 0.664 | Dice: 0.289 (LB 0.651, SB 0.494, S 0.615) | Hausdorff: 0.086 (LB 0.075, SB 0.073, S 0.111)
+Epoch 2 | Train Loss: 0.105 | Valid Loss: 0.181 | Combined metric: 0.654 | Dice: 0.261 (LB 0.568, SB 0.435, S 0.653) | Hausdorff: 0.085 (LB 0.104, SB 0.119, S 0.031)
+Epoch 3 | Train Loss: 0.091 | Valid Loss: 0.132 | Combined metric: 0.661 | Dice: 0.339 (LB 0.686, SB 0.557, S 0.665) | Hausdorff: 0.124 (LB 0.145, SB 0.086, S 0.142)
+Epoch 4 | Train Loss: 0.081 | Valid Loss: 0.131 | Combined metric: 0.688 | Dice: 0.333 (LB 0.708, SB 0.583, S 0.697) | Hausdorff: 0.076 (LB 0.091, SB 0.088, S 0.048)
+Epoch 5 | Train Loss: 0.074 | Valid Loss: 0.131 | Combined metric: 0.683 | Dice: 0.325 (LB 0.706, SB 0.587, S 0.649) | Hausdorff: 0.079 (LB 0.081, SB 0.069, S 0.087)</t>
   </si>
 </sst>
 </file>
@@ -325,10 +394,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -437,8 +506,93 @@
       <c r="D7" s="1" t="n">
         <v>0.79655</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>0.78819</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0.82225</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.81059</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0.646</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0.80702</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.80199</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0.672</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0.80078</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0.79186</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>0.639</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0.81925</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0.80673</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0.683</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>0.81698</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0.80041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trained on full data and predict on test
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -169,6 +169,20 @@
 Epoch 3 | Train Loss: 0.091 | Valid Loss: 0.132 | Combined metric: 0.661 | Dice: 0.339 (LB 0.686, SB 0.557, S 0.665) | Hausdorff: 0.124 (LB 0.145, SB 0.086, S 0.142)
 Epoch 4 | Train Loss: 0.081 | Valid Loss: 0.131 | Combined metric: 0.688 | Dice: 0.333 (LB 0.708, SB 0.583, S 0.697) | Hausdorff: 0.076 (LB 0.091, SB 0.088, S 0.048)
 Epoch 5 | Train Loss: 0.074 | Valid Loss: 0.131 | Combined metric: 0.683 | Dice: 0.325 (LB 0.706, SB 0.587, S 0.649) | Hausdorff: 0.079 (LB 0.081, SB 0.069, S 0.087)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unet Efficientnet-b1 
+Trained on full data
+(224x224)
+Batch size 64, with AMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Epoch Train Loss
+     1      0.228
+     2      0.104
+     3      0.091
+     4      0.082
+     5      0.078</t>
   </si>
 </sst>
 </file>
@@ -178,7 +192,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -207,6 +221,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -250,7 +269,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -268,6 +287,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,10 +417,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -595,6 +618,20 @@
         <v>0.80041</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0.81126</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0.80336</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
SSR,GridDist augmentations, removed incorrect masks, loss function wt
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -93,6 +93,381 @@
 9     | 0.000072  | 0.050      | 0.126      | 0.818           | 0.656        | 0.074             | 0.712  0.582  0.703  | 0.084  0.090  0.049 
 10    | 0.000050  | 0.048      | 0.126      | 0.824           | 0.662        | 0.068             | 0.716  0.589  0.704  | 0.085  0.074  0.045 </t>
   </si>
+  <si>
+    <t xml:space="preserve">2.5D stride1  H Flip P=0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.307      | 0.167      | 0.759           | 0.561        | 0.109             | 0.620  0.482  0.609  | 0.161  0.097  0.069 
+2     | 0.000500  | 0.106      | 0.140      | 0.801           | 0.633        | 0.088             | 0.691  0.544  0.670  | 0.094  0.096  0.072 
+3     | 0.000500  | 0.091      | 0.157      | 0.800           | 0.603        | 0.068             | 0.637  0.514  0.685  | 0.062  0.077  0.066 
+4     | 0.000478  | 0.084      | 0.135      | 0.798           | 0.629        | 0.089             | 0.685  0.554  0.687  | 0.133  0.084  0.049 
+5     | 0.000415  | 0.077      | 0.133      | 0.808           | 0.646        | 0.084             | 0.695  0.554  0.717  | 0.082  0.099  0.071 
+6     | 0.000325  | 0.069      | 0.130      | 0.823           | 0.659        | 0.068             | 0.711  0.577  0.712  | 0.075  0.069  0.059 
+7     | 0.000225  | 0.065      | 0.124      | 0.813           | 0.650        | 0.078             | 0.710  0.556  0.722  | 0.070  0.118  0.046 
+8     | 0.000135  | 0.061      | 0.128      | 0.821           | 0.654        | 0.068             | 0.712  0.568  0.713  | 0.074  0.072  0.059 
+9     | 0.000072  | 0.059      | 0.125      | 0.827           | 0.666        | 0.065             | 0.714  0.584  0.727  | 0.069  0.071  0.055 
+10    | 0.000050  | 0.057      | 0.124      | 0.827           | 0.668        | 0.068             | 0.716  0.583  0.732  | 0.070  0.076  0.057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5D stride1  H Flip P=0.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.306      | 0.160      | 0.764           | 0.567        | 0.105             | 0.652  0.482  0.597  | 0.092  0.106  0.118 
+2     | 0.000500  | 0.104      | 0.140      | 0.808           | 0.624        | 0.070             | 0.678  0.546  0.666  | 0.066  0.099  0.045 
+3     | 0.000500  | 0.090      | 0.130      | 0.815           | 0.645        | 0.071             | 0.708  0.553  0.702  | 0.084  0.075  0.054 
+4     | 0.000478  | 0.082      | 0.130      | 0.815           | 0.641        | 0.069             | 0.699  0.561  0.689  | 0.071  0.076  0.061 
+5     | 0.000415  | 0.074      | 0.127      | 0.819           | 0.658        | 0.073             | 0.721  0.576  0.697  | 0.074  0.083  0.062 
+6     | 0.000325  | 0.069      | 0.127      | 0.815           | 0.645        | 0.072             | 0.707  0.554  0.719  | 0.082  0.090  0.044 
+7     | 0.000225  | 0.063      | 0.129      | 0.812           | 0.648        | 0.078             | 0.709  0.561  0.708  | 0.078  0.106  0.050 
+8     | 0.000135  | 0.060      | 0.124      | 0.824           | 0.659        | 0.067             | 0.715  0.585  0.708  | 0.074  0.070  0.056 
+9     | 0.000072  | 0.057      | 0.124      | 0.827           | 0.661        | 0.062             | 0.714  0.576  0.723  | 0.071  0.071  0.045 
+10    | 0.000050  | 0.056      | 0.125      | 0.824           | 0.658        | 0.065             | 0.715  0.572  0.714  | 0.071  0.079  0.045 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5D stride1
+GridDistortion(num_steps=5, distort_limit=0.03, 
+                       P=0.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.340      | 0.172      | 0.787           | 0.588        | 0.080             | 0.650  0.514  0.610  | 0.089  0.058  0.092 
+2     | 0.000500  | 0.105      | 0.139      | 0.813           | 0.640        | 0.071             | 0.696  0.553  0.678  | 0.085  0.089  0.039 
+3     | 0.000500  | 0.086      | 0.130      | 0.827           | 0.661        | 0.062             | 0.715  0.579  0.703  | 0.081  0.060  0.047 
+4     | 0.000478  | 0.077      | 0.144      | 0.785           | 0.589        | 0.084             | 0.651  0.520  0.648  | 0.106  0.096  0.050 
+5     | 0.000415  | 0.071      | 0.129      | 0.799           | 0.641        | 0.096             | 0.700  0.585  0.672  | 0.116  0.084  0.086 
+6     | 0.000325  | 0.064      | 0.127      | 0.820           | 0.656        | 0.071             | 0.711  0.595  0.699  | 0.071  0.065  0.078 
+7     | 0.000225  | 0.059      | 0.125      | 0.818           | 0.658        | 0.075             | 0.713  0.583  0.719  | 0.080  0.086  0.058 
+8     | 0.000135  | 0.055      | 0.124      | 0.828           | 0.669        | 0.067             | 0.719  0.596  0.718  | 0.076  0.068  0.055 
+9     | 0.000072  | 0.052      | 0.123      | 0.826           | 0.668        | 0.069             | 0.724  0.597  0.709  | 0.079  0.077  0.050 
+10    | 0.000050  | 0.052      | 0.123      | 0.831           | 0.672        | 0.063             | 0.725  0.597  0.718  | 0.071  0.072  0.045 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5D stride1
+GridDistortion(num_steps=5, distort_limit=0.03, 
+                       P=0.25, cv2.INTER_NEAREST)
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.336      | 0.171      | 0.783           | 0.577        | 0.080             | 0.642  0.490  0.616  | 0.102  0.067  0.070 
+2     | 0.000500  | 0.104      | 0.135      | 0.817           | 0.643        | 0.066             | 0.684  0.569  0.704  | 0.066  0.088  0.044 
+3     | 0.000500  | 0.085      | 0.130      | 0.823           | 0.654        | 0.064             | 0.697  0.581  0.701  | 0.070  0.070  0.052 
+4     | 0.000478  | 0.076      | 0.130      | 0.810           | 0.646        | 0.081             | 0.716  0.562  0.675  | 0.076  0.075  0.092 
+5     | 0.000415  | 0.069      | 0.126      | 0.817           | 0.651        | 0.072             | 0.705  0.572  0.712  | 0.084  0.072  0.061 
+6     | 0.000325  | 0.062      | 0.128      | 0.819           | 0.654        | 0.071             | 0.707  0.589  0.706  | 0.072  0.073  0.068 
+7     | 0.000225  | 0.059      | 0.127      | 0.810           | 0.649        | 0.083             | 0.711  0.571  0.702  | 0.092  0.105  0.052 
+8     | 0.000135  | 0.055      | 0.125      | 0.821           | 0.662        | 0.073             | 0.721  0.588  0.708  | 0.076  0.082  0.062 
+9     | 0.000072  | 0.052      | 0.125      | 0.820           | 0.658        | 0.072             | 0.717  0.582  0.711  | 0.075  0.081  0.060 
+10    | 0.000050  | 0.050      | 0.125      | 0.823           | 0.663        | 0.070             | 0.721  0.585  0.712  | 0.081  0.078  0.051 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5D stride1
+GridDistortion(num_steps=5, distort_limit=0.05, 
+                       P=0.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.303      | 0.168      | 0.788           | 0.588        | 0.078             | 0.644  0.530  0.600  | 0.080  0.075  0.079 
+2     | 0.000500  | 0.100      | 0.133      | 0.824           | 0.655        | 0.064             | 0.711  0.560  0.696  | 0.073  0.063  0.056 
+3     | 0.000500  | 0.084      | 0.138      | 0.815           | 0.639        | 0.067             | 0.689  0.575  0.673  | 0.065  0.061  0.075 
+4     | 0.000478  | 0.076      | 0.138      | 0.787           | 0.614        | 0.097             | 0.673  0.541  0.656  | 0.078  0.123  0.091 
+5     | 0.000415  | 0.070      | 0.128      | 0.811           | 0.652        | 0.082             | 0.702  0.586  0.683  | 0.077  0.099  0.071 
+6     | 0.000325  | 0.063      | 0.131      | 0.811           | 0.642        | 0.076             | 0.695  0.581  0.689  | 0.072  0.086  0.070 
+7     | 0.000225  | 0.059      | 0.123      | 0.816           | 0.660        | 0.080             | 0.718  0.592  0.712  | 0.083  0.086  0.070 
+8     | 0.000135  | 0.055      | 0.122      | 0.828           | 0.672        | 0.068             | 0.723  0.602  0.714  | 0.081  0.067  0.057 
+9     | 0.000072  | 0.053      | 0.122      | 0.821           | 0.661        | 0.073             | 0.714  0.589  0.716  | 0.072  0.078  0.068 
+10    | 0.000050  | 0.051      | 0.121      | 0.828           | 0.671        | 0.067             | 0.723  0.596  0.719  | 0.068  0.071  0.061 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElasticTransform(alpha=1, sigma=50, p=0.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.334      | 0.176      | 0.756           | 0.554        | 0.109             | 0.660  0.507  0.524  | 0.078  0.079  0.170 
+2     | 0.000500  | 0.103      | 0.142      | 0.788           | 0.613        | 0.095             | 0.673  0.550  0.661  | 0.080  0.106  0.101 
+3     | 0.000500  | 0.084      | 0.132      | 0.815           | 0.647        | 0.073             | 0.697  0.569  0.696  | 0.074  0.070  0.075 
+4     | 0.000478  | 0.074      | 0.130      | 0.797           | 0.625        | 0.088             | 0.688  0.560  0.673  | 0.110  0.091  0.063 
+5     | 0.000415  | 0.068      | 0.123      | 0.824           | 0.663        | 0.068             | 0.720  0.582  0.714  | 0.070  0.087  0.048 
+6     | 0.000325  | 0.060      | 0.123      | 0.814           | 0.657        | 0.081             | 0.713  0.592  0.701  | 0.073  0.075  0.095 
+7     | 0.000225  | 0.057      | 0.125      | 0.797           | 0.635        | 0.095             | 0.698  0.568  0.697  | 0.099  0.119  0.066 
+8     | 0.000135  | 0.053      | 0.121      | 0.833           | 0.675        | 0.062             | 0.719  0.602  0.725  | 0.071  0.065  0.050 
+9     | 0.000072  | 0.050      | 0.122      | 0.827           | 0.665        | 0.066             | 0.718  0.586  0.716  | 0.071  0.073  0.052 
+10    | 0.000050  | 0.049      | 0.121      | 0.830           | 0.672        | 0.064             | 0.721  0.593  0.724  | 0.074  0.076  0.042 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElasticTransform(alpha=15, sigma=50, p=0.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.334      | 0.176      | 0.783           | 0.573        | 0.076             | 0.646  0.464  0.611  | 0.106  0.059  0.065 
+2     | 0.000500  | 0.104      | 0.142      | 0.782           | 0.602        | 0.098             | 0.658  0.522  0.689  | 0.096  0.123  0.075 
+3     | 0.000500  | 0.083      | 0.136      | 0.791           | 0.629        | 0.102             | 0.709  0.545  0.648  | 0.086  0.085  0.134 
+4     | 0.000478  | 0.075      | 0.125      | 0.820           | 0.659        | 0.073             | 0.713  0.581  0.711  | 0.098  0.074  0.046 
+5     | 0.000415  | 0.067      | 0.122      | 0.822           | 0.665        | 0.072             | 0.718  0.591  0.714  | 0.089  0.079  0.049 
+6     | 0.000325  | 0.062      | 0.125      | 0.814           | 0.646        | 0.074             | 0.703  0.593  0.684  | 0.073  0.075  0.075 
+7     | 0.000225  | 0.057      | 0.121      | 0.824           | 0.667        | 0.071             | 0.722  0.594  0.712  | 0.077  0.080  0.055 
+8     | 0.000135  | 0.053      | 0.120      | 0.825           | 0.668        | 0.070             | 0.723  0.594  0.719  | 0.079  0.078  0.054 
+9     | 0.000072  | 0.051      | 0.120      | 0.822           | 0.662        | 0.071             | 0.718  0.594  0.714  | 0.077  0.078  0.057 
+10    | 0.000050  | 0.049      | 0.119      | 0.824           | 0.669        | 0.073             | 0.721  0.597  0.720  | 0.087  0.082  0.050 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ElasticTransform(alpha=15, sigma=5, p=0.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.338      | 0.176      | 0.783           | 0.579        | 0.082             | 0.656  0.486  0.622  | 0.105  0.060  0.080 
+2     | 0.000500  | 0.104      | 0.134      | 0.809           | 0.640        | 0.078             | 0.701  0.566  0.681  | 0.075  0.085  0.072 
+3     | 0.000500  | 0.085      | 0.137      | 0.783           | 0.612        | 0.102             | 0.686  0.536  0.660  | 0.126  0.089  0.091 
+4     | 0.000478  | 0.076      | 0.130      | 0.821           | 0.655        | 0.068             | 0.710  0.576  0.693  | 0.079  0.070  0.054 
+5     | 0.000415  | 0.068      | 0.126      | 0.826           | 0.654        | 0.060             | 0.701  0.577  0.715  | 0.068  0.068  0.045 
+6     | 0.000325  | 0.062      | 0.128      | 0.822           | 0.656        | 0.067             | 0.711  0.580  0.702  | 0.084  0.063  0.053 
+7     | 0.000225  | 0.057      | 0.125      | 0.826           | 0.657        | 0.061             | 0.710  0.591  0.704  | 0.067  0.066  0.049 
+8     | 0.000135  | 0.054      | 0.123      | 0.828           | 0.667        | 0.066             | 0.721  0.611  0.703  | 0.074  0.063  0.060 
+9     | 0.000072  | 0.051      | 0.124      | 0.826           | 0.661        | 0.064             | 0.713  0.596  0.705  | 0.083  0.066  0.043 
+10    | 0.000050  | 0.049      | 0.124      | 0.822           | 0.661        | 0.070             | 0.715  0.593  0.707  | 0.086  0.074  0.050 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OneOf([
+   GridDistortion,
+   ElasticTransform
+], P=0.25
+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.333      | 0.158      | 0.803           | 0.608        | 0.067             | 0.671  0.536  0.629  | 0.079  0.067  0.054 
+2     | 0.000500  | 0.104      | 0.134      | 0.796           | 0.630        | 0.093             | 0.698  0.533  0.709  | 0.085  0.124  0.071 
+3     | 0.000500  | 0.084      | 0.136      | 0.828           | 0.651        | 0.053             | 0.693  0.571  0.714  | 0.062  0.056  0.043 
+4     | 0.000478  | 0.075      | 0.126      | 0.820           | 0.658        | 0.071             | 0.717  0.573  0.698  | 0.083  0.071  0.060 
+5     | 0.000415  | 0.067      | 0.124      | 0.827           | 0.663        | 0.064             | 0.716  0.593  0.710  | 0.074  0.065  0.054 
+6     | 0.000325  | 0.062      | 0.127      | 0.795           | 0.635        | 0.098             | 0.717  0.570  0.681  | 0.084  0.120  0.089 
+7     | 0.000225  | 0.058      | 0.124      | 0.823           | 0.657        | 0.067             | 0.713  0.580  0.721  | 0.073  0.081  0.046 
+8     | 0.000135  | 0.053      | 0.124      | 0.829           | 0.666        | 0.062             | 0.719  0.589  0.723  | 0.080  0.066  0.042 
+9     | 0.000072  | 0.051      | 0.122      | 0.830           | 0.668        | 0.062             | 0.720  0.598  0.726  | 0.071  0.072  0.043 
+10    | 0.000050  | 0.049      | 0.124      | 0.825           | 0.660        | 0.066             | 0.714  0.583  0.721  | 0.074  0.080  0.043 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">H Flip P=0.5
+OneOf([
+   GridDistortion,
+   ElasticTransform
+], P=0.25
+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.310      | 0.166      | 0.766           | 0.565        | 0.100             | 0.640  0.490  0.584  | 0.143  0.093  0.065 
+2     | 0.000500  | 0.106      | 0.150      | 0.796           | 0.611        | 0.080             | 0.681  0.502  0.671  | 0.096  0.086  0.057 
+3     | 0.000500  | 0.092      | 0.134      | 0.809           | 0.638        | 0.076             | 0.701  0.549  0.697  | 0.081  0.075  0.073 
+4     | 0.000478  | 0.084      | 0.137      | 0.795           | 0.631        | 0.096             | 0.686  0.551  0.684  | 0.113  0.107  0.069 
+5     | 0.000415  | 0.077      | 0.129      | 0.809           | 0.646        | 0.082             | 0.700  0.560  0.712  | 0.091  0.088  0.068 
+6     | 0.000325  | 0.071      | 0.130      | 0.818           | 0.646        | 0.067             | 0.701  0.567  0.696  | 0.075  0.080  0.047 
+7     | 0.000225  | 0.067      | 0.127      | 0.816           | 0.652        | 0.075             | 0.709  0.574  0.699  | 0.077  0.088  0.060 
+8     | 0.000135  | 0.062      | 0.126      | 0.825           | 0.660        | 0.066             | 0.713  0.585  0.711  | 0.078  0.064  0.055 
+9     | 0.000072  | 0.059      | 0.127      | 0.822           | 0.658        | 0.069             | 0.711  0.580  0.708  | 0.077  0.078  0.052 
+10    | 0.000050  | 0.058      | 0.124      | 0.822           | 0.662        | 0.071             | 0.713  0.580  0.716  | 0.082  0.075  0.055 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.ShiftScaleRotate(shift_limit=0.0625, 
+        Scale_limit=0.05, rotate_limit=5, p=0.5)
+GridDistortion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.298      | 0.159      | 0.766           | 0.575        | 0.107             | 0.645  0.522  0.590  | 0.122  0.087  0.113 
+2     | 0.000500  | 0.101      | 0.136      | 0.814           | 0.640        | 0.069             | 0.689  0.564  0.690  | 0.083  0.087  0.038 
+3     | 0.000500  | 0.088      | 0.136      | 0.794           | 0.622        | 0.092             | 0.692  0.526  0.689  | 0.084  0.142  0.049 
+4     | 0.000478  | 0.082      | 0.130      | 0.817           | 0.658        | 0.077             | 0.713  0.581  0.694  | 0.096  0.066  0.070 
+5     | 0.000415  | 0.074      | 0.126      | 0.819           | 0.655        | 0.071             | 0.698  0.583  0.711  | 0.077  0.068  0.068 
+6     | 0.000325  | 0.069      | 0.129      | 0.770           | 0.602        | 0.118             | 0.682  0.521  0.679  | 0.124  0.131  0.101 
+7     | 0.000225  | 0.065      | 0.125      | 0.823           | 0.663        | 0.070             | 0.714  0.595  0.714  | 0.074  0.081  0.054 
+8     | 0.000135  | 0.061      | 0.122      | 0.829           | 0.672        | 0.066             | 0.727  0.598  0.720  | 0.072  0.072  0.053 
+9     | 0.000072  | 0.058      | 0.125      | 0.823           | 0.660        | 0.068             | 0.714  0.584  0.719  | 0.075  0.080  0.049 
+10    | 0.000050  | 0.056      | 0.123      | 0.827           | 0.667        | 0.067             | 0.719  0.594  0.720  | 0.068  0.075  0.057 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.ShiftScaleRotate(shift_limit=0.0625, 
+        Scale_limit=0.05, rotate_limit=5, p=0.5)
+GridDistortion
+again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.298      | 0.156      | 0.772           | 0.586        | 0.103             | 0.653  0.540  0.596  | 0.132  0.087  0.091 
+2     | 0.000500  | 0.102      | 0.137      | 0.811           | 0.628        | 0.067             | 0.685  0.539  0.692  | 0.079  0.078  0.045 
+3     | 0.000500  | 0.088      | 0.133      | 0.811           | 0.643        | 0.078             | 0.701  0.567  0.692  | 0.101  0.077  0.055 
+4     | 0.000478  | 0.080      | 0.132      | 0.822           | 0.648        | 0.061             | 0.691  0.580  0.691  | 0.065  0.072  0.046 
+5     | 0.000415  | 0.074      | 0.125      | 0.822           | 0.659        | 0.069             | 0.715  0.588  0.698  | 0.081  0.072  0.056 
+6     | 0.000325  | 0.068      | 0.127      | 0.817           | 0.652        | 0.074             | 0.706  0.586  0.700  | 0.077  0.071  0.073 
+7     | 0.000225  | 0.064      | 0.122      | 0.824           | 0.666        | 0.070             | 0.724  0.598  0.711  | 0.082  0.078  0.050 
+8     | 0.000135  | 0.060      | 0.121      | 0.826           | 0.669        | 0.069             | 0.722  0.603  0.715  | 0.077  0.080  0.050 
+9     | 0.000072  | 0.057      | 0.123      | 0.824           | 0.664        | 0.070             | 0.717  0.597  0.712  | 0.072  0.084  0.053 
+10    | 0.000050  | 0.056      | 0.123      | 0.825           | 0.667        | 0.069             | 0.720  0.597  0.717  | 0.069  0.087  0.051 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.ShiftScaleRotate(shift_limit=0.0625, 
+        Scale_limit=0.05, rotate_limit=5, p=0.5)
+GridDistortion
+again with final LR 1e-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.299      | 0.156      | 0.770           | 0.577        | 0.101             | 0.640  0.482  0.648  | 0.092  0.098  0.113 
+2     | 0.000500  | 0.101      | 0.138      | 0.811           | 0.635        | 0.072             | 0.681  0.553  0.703  | 0.091  0.082  0.043 
+3     | 0.000500  | 0.087      | 0.126      | 0.825           | 0.663        | 0.068             | 0.706  0.586  0.718  | 0.063  0.072  0.068 
+4     | 0.000476  | 0.081      | 0.126      | 0.813           | 0.647        | 0.076             | 0.693  0.572  0.721  | 0.080  0.086  0.063 
+5     | 0.000408  | 0.074      | 0.123      | 0.819           | 0.659        | 0.074             | 0.710  0.575  0.732  | 0.084  0.080  0.059 
+6     | 0.000310  | 0.068      | 0.124      | 0.815           | 0.650        | 0.075             | 0.701  0.575  0.720  | 0.084  0.083  0.059 
+7     | 0.000200  | 0.064      | 0.120      | 0.827           | 0.673        | 0.070             | 0.724  0.590  0.739  | 0.076  0.076  0.059 
+8     | 0.000102  | 0.060      | 0.122      | 0.830           | 0.670        | 0.063             | 0.723  0.589  0.723  | 0.068  0.073  0.048 
+9     | 0.000034  | 0.058      | 0.121      | 0.830           | 0.670        | 0.064             | 0.720  0.588  0.737  | 0.070  0.074  0.047 
+10    | 0.000010  | 0.057      | 0.121      | 0.831           | 0.672        | 0.063             | 0.720  0.589  0.739  | 0.067  0.075  0.046 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">grid_distortion with final LR 1e-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.333      | 0.160      | 0.785           | 0.594        | 0.088             | 0.658  0.502  0.636  | 0.107  0.076  0.082 
+2     | 0.000500  | 0.103      | 0.130      | 0.810           | 0.652        | 0.084             | 0.702  0.571  0.705  | 0.089  0.095  0.067 
+3     | 0.000500  | 0.084      | 0.131      | 0.829           | 0.654        | 0.055             | 0.697  0.578  0.711  | 0.068  0.056  0.041 
+4     | 0.000480  | 0.077      | 0.133      | 0.824           | 0.649        | 0.059             | 0.700  0.571  0.694  | 0.076  0.063  0.039 
+5     | 0.000425  | 0.069      | 0.128      | 0.817           | 0.646        | 0.069             | 0.711  0.567  0.699  | 0.064  0.097  0.046 
+6     | 0.000345  | 0.063      | 0.125      | 0.818           | 0.651        | 0.071             | 0.708  0.577  0.706  | 0.073  0.076  0.064 
+7     | 0.000255  | 0.058      | 0.123      | 0.820           | 0.657        | 0.071             | 0.719  0.574  0.719  | 0.064  0.098  0.049 
+8     | 0.000175  | 0.055      | 0.125      | 0.825           | 0.659        | 0.065             | 0.719  0.574  0.722  | 0.069  0.085  0.041 
+9     | 0.000120  | 0.053      | 0.124      | 0.832           | 0.666        | 0.057             | 0.720  0.585  0.727  | 0.061  0.070  0.041 
+10    | 0.000100  | 0.051      | 0.124      | 0.827           | 0.663        | 0.065             | 0.723  0.583  0.718  | 0.067  0.079  0.048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grid_distortion with final LR 1e-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.333      | 0.166      | 0.773           | 0.579        | 0.097             | 0.636  0.488  0.622  | 0.108  0.079  0.105 
+2     | 0.000500  | 0.103      | 0.133      | 0.810           | 0.640        | 0.076             | 0.698  0.559  0.699  | 0.091  0.103  0.035 
+3     | 0.000500  | 0.084      | 0.137      | 0.804           | 0.629        | 0.080             | 0.693  0.530  0.695  | 0.075  0.112  0.054 
+4     | 0.000476  | 0.076      | 0.128      | 0.814           | 0.646        | 0.073             | 0.710  0.564  0.681  | 0.088  0.079  0.052 
+5     | 0.000408  | 0.068      | 0.125      | 0.819           | 0.655        | 0.072             | 0.714  0.573  0.712  | 0.085  0.083  0.048 
+6     | 0.000310  | 0.063      | 0.123      | 0.819           | 0.658        | 0.073             | 0.724  0.591  0.696  | 0.079  0.080  0.061 
+7     | 0.000200  | 0.058      | 0.123      | 0.820           | 0.657        | 0.072             | 0.716  0.573  0.717  | 0.084  0.088  0.045 
+8     | 0.000102  | 0.054      | 0.123      | 0.824           | 0.661        | 0.067             | 0.720  0.582  0.713  | 0.078  0.082  0.040 
+9     | 0.000034  | 0.052      | 0.122      | 0.827           | 0.669        | 0.068             | 0.724  0.588  0.720  | 0.082  0.079  0.042 
+10    | 0.000010  | 0.051      | 0.122      | 0.830           | 0.670        | 0.064             | 0.724  0.589  0.723  | 0.075  0.075  0.041 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.ShiftScaleRotate(shift_limit=0.03, 
+        Scale_limit=0.05, rotate_limit=5, p=0.5)
+GridDistortion
+With final LR 1e-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.307      | 0.155      | 0.774           | 0.575        | 0.092             | 0.657  0.531  0.581  | 0.082  0.069  0.127 
+2     | 0.000500  | 0.101      | 0.133      | 0.809           | 0.645        | 0.081             | 0.694  0.564  0.708  | 0.089  0.111  0.042 
+3     | 0.000500  | 0.087      | 0.149      | 0.815           | 0.619        | 0.054             | 0.653  0.528  0.708  | 0.057  0.059  0.047 
+4     | 0.000476  | 0.080      | 0.124      | 0.805           | 0.649        | 0.091             | 0.709  0.576  0.710  | 0.119  0.088  0.068 
+5     | 0.000408  | 0.073      | 0.122      | 0.825           | 0.666        | 0.069             | 0.715  0.597  0.718  | 0.091  0.061  0.054 
+6     | 0.000310  | 0.067      | 0.126      | 0.802           | 0.639        | 0.089             | 0.708  0.558  0.707  | 0.086  0.114  0.067 
+7     | 0.000200  | 0.063      | 0.120      | 0.820           | 0.664        | 0.077             | 0.722  0.583  0.734  | 0.077  0.101  0.052 
+8     | 0.000102  | 0.059      | 0.120      | 0.825           | 0.669        | 0.071             | 0.722  0.595  0.726  | 0.070  0.083  0.060 
+9     | 0.000034  | 0.057      | 0.119      | 0.834           | 0.677        | 0.062             | 0.727  0.603  0.733  | 0.068  0.070  0.048 
+10    | 0.000010  | 0.057      | 0.119      | 0.833           | 0.676        | 0.062             | 0.726  0.602  0.734  | 0.067  0.070  0.049 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Without 2 problem casedays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.302      | 0.147      | 0.789           | 0.617        | 0.096             | 0.641  0.560  0.715  | 0.143  0.084  0.061 
+2     | 0.000500  | 0.105      | 0.114      | 0.838           | 0.706        | 0.073             | 0.737  0.637  0.765  | 0.085  0.091  0.043 
+3     | 0.000500  | 0.090      | 0.115      | 0.816           | 0.690        | 0.101             | 0.730  0.614  0.756  | 0.074  0.120  0.108 
+4     | 0.000476  | 0.079      | 0.113      | 0.838           | 0.704        | 0.072             | 0.738  0.631  0.764  | 0.069  0.082  0.065 
+5     | 0.000408  | 0.072      | 0.109      | 0.846           | 0.723        | 0.071             | 0.751  0.647  0.788  | 0.089  0.100  0.024 
+6     | 0.000310  | 0.067      | 0.106      | 0.838           | 0.719        | 0.082             | 0.758  0.646  0.749  | 0.087  0.101  0.060 
+7     | 0.000200  | 0.062      | 0.105      | 0.858           | 0.737        | 0.062             | 0.759  0.676  0.793  | 0.069  0.066  0.052 
+8     | 0.000102  | 0.059      | 0.104      | 0.857           | 0.737        | 0.063             | 0.758  0.666  0.802  | 0.071  0.072  0.045 
+9     | 0.000034  | 0.056      | 0.103      | 0.861           | 0.740        | 0.058             | 0.763  0.667  0.807  | 0.070  0.066  0.037 
+10    | 0.000010  | 0.055      | 0.104      | 0.862           | 0.740        | 0.057             | 0.762  0.666  0.808  | 0.069  0.067  0.035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Without 3 problem casedays
+(Took 49min 29s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.292      | 0.144      | 0.802           | 0.626        | 0.081             | 0.679  0.534  0.684  | 0.094  0.070  0.080 
+2     | 0.000500  | 0.100      | 0.137      | 0.816           | 0.641        | 0.068             | 0.668  0.566  0.707  | 0.097  0.075  0.030 
+3     | 0.000500  | 0.086      | 0.127      | 0.825           | 0.669        | 0.071             | 0.706  0.590  0.708  | 0.085  0.068  0.059 
+4     | 0.000476  | 0.078      | 0.132      | 0.820           | 0.657        | 0.072             | 0.699  0.565  0.720  | 0.110  0.067  0.038 
+5     | 0.000408  | 0.071      | 0.123      | 0.822           | 0.673        | 0.078             | 0.703  0.597  0.722  | 0.087  0.081  0.065 
+6     | 0.000310  | 0.065      | 0.120      | 0.837           | 0.692        | 0.066             | 0.718  0.619  0.736  | 0.076  0.077  0.046 
+7     | 0.000200  | 0.061      | 0.120      | 0.831           | 0.685        | 0.071             | 0.712  0.612  0.731  | 0.088  0.080  0.045 
+8     | 0.000102  | 0.057      | 0.119      | 0.844           | 0.694        | 0.057             | 0.718  0.624  0.741  | 0.068  0.070  0.033 
+9     | 0.000034  | 0.056      | 0.119      | 0.842           | 0.693        | 0.059             | 0.717  0.622  0.739  | 0.071  0.070  0.036 
+10    | 0.000010  | 0.054      | 0.118      | 0.843           | 0.695        | 0.059             | 0.720  0.622  0.741  | 0.069  0.072  0.035 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Without 3 problem casedays – 15 epochs
+(Took 1h 12min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.291      | 0.145      | 0.822           | 0.653        | 0.065             | 0.687  0.549  0.712  | 0.084  0.058  0.053 
+2     | 0.000500  | 0.100      | 0.132      | 0.795           | 0.628        | 0.094             | 0.662  0.543  0.724  | 0.106  0.109  0.067 
+3     | 0.000500  | 0.085      | 0.133      | 0.817           | 0.647        | 0.069             | 0.684  0.567  0.701  | 0.080  0.078  0.049 
+4     | 0.000492  | 0.077      | 0.137      | 0.821           | 0.649        | 0.065             | 0.691  0.543  0.711  | 0.083  0.070  0.041 
+5     | 0.000467  | 0.071      | 0.124      | 0.828           | 0.675        | 0.071             | 0.710  0.587  0.722  | 0.073  0.090  0.049 
+6     | 0.000428  | 0.067      | 0.120      | 0.833           | 0.688        | 0.071             | 0.720  0.612  0.742  | 0.096  0.078  0.040 
+7     | 0.000377  | 0.064      | 0.120      | 0.823           | 0.684        | 0.084             | 0.717  0.616  0.724  | 0.092  0.074  0.086 
+8     | 0.000318  | 0.060      | 0.123      | 0.833           | 0.679        | 0.064             | 0.706  0.597  0.737  | 0.080  0.076  0.036 
+9     | 0.000255  | 0.057      | 0.121      | 0.839           | 0.690        | 0.062             | 0.719  0.610  0.752  | 0.077  0.070  0.040 
+10    | 0.000192  | 0.055      | 0.125      | 0.821           | 0.676        | 0.081             | 0.708  0.605  0.727  | 0.109  0.074  0.061 
+11    | 0.000133  | 0.053      | 0.121      | 0.834           | 0.690        | 0.070             | 0.716  0.615  0.741  | 0.085  0.079  0.047 
+12    | 0.000082  | 0.051      | 0.119      | 0.834           | 0.694        | 0.073             | 0.720  0.616  0.748  | 0.085  0.084  0.051 
+13    | 0.000043  | 0.049      | 0.117      | 0.834           | 0.697        | 0.075             | 0.723  0.622  0.752  | 0.092  0.082  0.050 
+14    | 0.000018  | 0.049      | 0.119      | 0.834           | 0.696        | 0.074             | 0.720  0.619  0.750  | 0.090  0.078  0.054 
+15    | 0.000010  | 0.049      | 0.118      | 0.834           | 0.697        | 0.074             | 0.722  0.623  0.749  | 0.092  0.080  0.051 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">loss_weight_0.4
+i.e. dice_loss * 0.4 + BCE_loss * (1-0.4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.258      | 0.129      | 0.806           | 0.613        | 0.065             | 0.650  0.514  0.666  | 0.068  0.073  0.055 
+2     | 0.000500  | 0.083      | 0.108      | 0.808           | 0.636        | 0.078             | 0.683  0.534  0.714  | 0.087  0.104  0.042 
+3     | 0.000500  | 0.070      | 0.110      | 0.813           | 0.645        | 0.075             | 0.685  0.562  0.704  | 0.089  0.086  0.049 
+4     | 0.000476  | 0.062      | 0.111      | 0.826           | 0.659        | 0.063             | 0.703  0.564  0.710  | 0.095  0.057  0.036 
+5     | 0.000408  | 0.057      | 0.098      | 0.841           | 0.695        | 0.061             | 0.720  0.615  0.748  | 0.070  0.071  0.042 
+6     | 0.000310  | 0.052      | 0.099      | 0.831           | 0.684        | 0.072             | 0.715  0.611  0.728  | 0.074  0.082  0.059 
+7     | 0.000200  | 0.049      | 0.099      | 0.836           | 0.685        | 0.063             | 0.716  0.606  0.744  | 0.088  0.071  0.030 
+8     | 0.000102  | 0.046      | 0.097      | 0.837           | 0.691        | 0.066             | 0.722  0.613  0.749  | 0.084  0.079  0.035 
+9     | 0.000034  | 0.044      | 0.097      | 0.838           | 0.691        | 0.064             | 0.724  0.615  0.745  | 0.079  0.077  0.035 
+10    | 0.000010  | 0.044      | 0.097      | 0.837           | 0.691        | 0.066             | 0.723  0.614  0.748  | 0.076  0.078  0.042 </t>
+  </si>
 </sst>
 </file>
 
@@ -101,7 +476,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -134,6 +509,12 @@
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="10"/>
@@ -141,12 +522,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -183,7 +570,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -200,10 +587,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,8 +619,56 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -249,6 +680,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFAFD095"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -363,45 +854,44 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="160.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="13.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.23"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+    <row r="1" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -409,7 +899,7 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="n">
@@ -418,7 +908,7 @@
       <c r="D4" s="3" t="n">
         <v>0.83893</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="3" t="n">
         <v>0.82138</v>
       </c>
     </row>
@@ -427,7 +917,7 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3" t="n">
@@ -436,15 +926,15 @@
       <c r="D6" s="3" t="n">
         <v>0.83844</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="3" t="n">
         <v>0.8158</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3" t="n">
@@ -453,8 +943,261 @@
       <c r="D8" s="3" t="n">
         <v>0.837</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="3" t="n">
         <v>0.81291</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="D10" s="13" t="n">
+        <v>0.84262</v>
+      </c>
+      <c r="E10" s="13" t="n">
+        <v>0.821</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>0.824</v>
+      </c>
+      <c r="D12" s="13" t="n">
+        <v>0.83586</v>
+      </c>
+      <c r="E12" s="13" t="n">
+        <v>0.82377</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="14" t="n">
+        <v>0.831</v>
+      </c>
+      <c r="D14" s="13" t="n">
+        <v>0.83762</v>
+      </c>
+      <c r="E14" s="13" t="n">
+        <v>0.81809</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="14" t="n">
+        <v>0.823</v>
+      </c>
+      <c r="D16" s="13" t="n">
+        <v>0.841</v>
+      </c>
+      <c r="E16" s="13" t="n">
+        <v>0.81975</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="D40" s="13" t="n">
+        <v>0.84358</v>
+      </c>
+      <c r="E40" s="16" t="n">
+        <v>0.82371</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="3" t="n">
+        <v>0.862</v>
+      </c>
+      <c r="D42" s="13" t="n">
+        <v>0.84226</v>
+      </c>
+      <c r="E42" s="13" t="n">
+        <v>0.82784</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="9"/>
+    </row>
+    <row r="44" s="22" customFormat="true" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="19" t="n">
+        <v>0.843</v>
+      </c>
+      <c r="D44" s="20" t="n">
+        <v>0.84494</v>
+      </c>
+      <c r="E44" s="21" t="n">
+        <v>0.83243</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="9"/>
+    </row>
+    <row r="46" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="3" t="n">
+        <v>0.834</v>
+      </c>
+      <c r="D46" s="24" t="n">
+        <v>0.84219</v>
+      </c>
+      <c r="E46" s="24" t="n">
+        <v>0.83364</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="3" t="n">
+        <v>0.837</v>
+      </c>
+      <c r="D48" s="24" t="n">
+        <v>0.84214</v>
+      </c>
+      <c r="E48" s="24" t="n">
+        <v>0.83249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grad accu, pred visualize, sizewise metrics, explored more augment, trained on bigger sizes
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Train logs</t>
   </si>
   <si>
     <t xml:space="preserve">Validation 
@@ -36,6 +33,9 @@
   </si>
   <si>
     <t xml:space="preserve">Private Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train logs</t>
   </si>
   <si>
     <t xml:space="preserve">UNet Efficientnet-b1 
@@ -467,6 +467,606 @@
 8     | 0.000102  | 0.046      | 0.097      | 0.837           | 0.691        | 0.066             | 0.722  0.613  0.749  | 0.084  0.079  0.035 
 9     | 0.000034  | 0.044      | 0.097      | 0.838           | 0.691        | 0.064             | 0.724  0.615  0.745  | 0.079  0.077  0.035 
 10    | 0.000010  | 0.044      | 0.097      | 0.837           | 0.691        | 0.066             | 0.723  0.614  0.748  | 0.076  0.078  0.042 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tversky_loss(alpha=0.4,beta=0.6)*0.5 
++ BCE_loss*0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.286      | 0.147      | 0.809           | 0.632        | 0.073             | 0.668  0.542  0.672  | 0.074  0.083  0.064 
+2     | 0.000500  | 0.097      | 0.127      | 0.787           | 0.631        | 0.108             | 0.671  0.562  0.712  | 0.135  0.125  0.065 
+3     | 0.000500  | 0.085      | 0.125      | 0.790           | 0.638        | 0.108             | 0.698  0.550  0.705  | 0.122  0.139  0.064 
+4     | 0.000476  | 0.077      | 0.131      | 0.822           | 0.659        | 0.069             | 0.699  0.572  0.702  | 0.071  0.075  0.061 
+5     | 0.000408  | 0.070      | 0.124      | 0.823           | 0.660        | 0.069             | 0.689  0.585  0.720  | 0.086  0.076  0.046 
+6     | 0.000310  | 0.064      | 0.117      | 0.832           | 0.688        | 0.071             | 0.715  0.614  0.733  | 0.079  0.088  0.047 
+7     | 0.000200  | 0.059      | 0.120      | 0.832           | 0.685        | 0.069             | 0.720  0.610  0.718  | 0.084  0.080  0.044 
+8     | 0.000102  | 0.056      | 0.114      | 0.842           | 0.698        | 0.062             | 0.729  0.623  0.737  | 0.079  0.071  0.037 
+9     | 0.000034  | 0.054      | 0.116      | 0.838           | 0.693        | 0.065             | 0.727  0.618  0.726  | 0.075  0.078  0.041 
+10    | 0.000010  | 0.053      | 0.116      | 0.836           | 0.692        | 0.068             | 0.724  0.617  0.728  | 0.082  0.078  0.046 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">loss_weight_0.6
+i.e. dice_loss * 0.6 + BCE_loss * (1-0.6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.335      | 0.188      | 0.768           | 0.589        | 0.112             | 0.513  0.067  | 0.301  0.020  | 0.633  0.510  0.650  | 0.118  0.119  0.100 
+2     | 0.000500  | 0.118      | 0.165      | 0.793           | 0.620        | 0.092             | 0.189  0.012  | 0.262  0.020  | 0.655  0.534  0.710  | 0.119  0.108  0.048 
+3     | 0.000500  | 0.102      | 0.148      | 0.809           | 0.662        | 0.093             | 0.162  0.011  | 0.235  0.019  | 0.698  0.595  0.709  | 0.121  0.115  0.042 
+4     | 0.000476  | 0.091      | 0.152      | 0.827           | 0.661        | 0.062             | 0.146  0.010  | 0.240  0.018  | 0.703  0.579  0.690  | 0.075  0.065  0.046 
+5     | 0.000408  | 0.083      | 0.144      | 0.836           | 0.681        | 0.061             | 0.132  0.009  | 0.228  0.020  | 0.705  0.595  0.748  | 0.065  0.082  0.035 
+6     | 0.000310  | 0.077      | 0.141      | 0.829           | 0.677        | 0.071             | 0.122  0.008  | 0.222  0.018  | 0.714  0.603  0.714  | 0.094  0.072  0.046 
+7     | 0.000200  | 0.073      | 0.141      | 0.833           | 0.686        | 0.069             | 0.116  0.008  | 0.223  0.020  | 0.715  0.613  0.733  | 0.086  0.081  0.039 
+8     | 0.000102  | 0.068      | 0.139      | 0.838           | 0.691        | 0.064             | 0.109  0.007  | 0.218  0.019  | 0.723  0.621  0.723  | 0.078  0.068  0.045 
+9     | 0.000034  | 0.066      | 0.138      | 0.838           | 0.692        | 0.065             | 0.105  0.007  | 0.218  0.019  | 0.720  0.623  0.726  | 0.075  0.075  0.046 
+10    | 0.000010  | 0.065      | 0.138      | 0.837           | 0.692        | 0.067             | 0.104  0.007  | 0.217  0.019  | 0.721  0.620  0.726  | 0.078  0.076  0.046 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">loss_weight_0.75
+i.e. dice_loss * 0.75 + BCE_loss * (1-0.75)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.388      | 0.211      | 0.786           | 0.608        | 0.096             | 0.495  0.068  | 0.275  0.018  | 0.651  0.525  0.661  | 0.127  0.087  0.073 
+2     | 0.000500  | 0.144      | 0.185      | 0.766           | 0.619        | 0.136             | 0.188  0.013  | 0.240  0.019  | 0.678  0.557  0.675  | 0.129  0.153  0.127 
+3     | 0.000500  | 0.125      | 0.188      | 0.807           | 0.641        | 0.083             | 0.162  0.012  | 0.244  0.021  | 0.706  0.553  0.695  | 0.079  0.111  0.059 
+4     | 0.000476  | 0.114      | 0.187      | 0.809           | 0.647        | 0.083             | 0.148  0.012  | 0.243  0.021  | 0.690  0.570  0.703  | 0.122  0.080  0.045 
+5     | 0.000408  | 0.103      | 0.183      | 0.783           | 0.634        | 0.118             | 0.133  0.011  | 0.236  0.023  | 0.674  0.572  0.696  | 0.159  0.129  0.066 
+6     | 0.000310  | 0.095      | 0.178      | 0.810           | 0.654        | 0.087             | 0.124  0.010  | 0.231  0.022  | 0.682  0.600  0.713  | 0.136  0.083  0.041 
+7     | 0.000200  | 0.089      | 0.174      | 0.831           | 0.679        | 0.068             | 0.115  0.009  | 0.224  0.022  | 0.719  0.605  0.716  | 0.076  0.078  0.049 
+8     | 0.000102  | 0.084      | 0.170      | 0.838           | 0.694        | 0.067             | 0.109  0.009  | 0.219  0.022  | 0.729  0.620  0.720  | 0.069  0.078  0.053 
+9     | 0.000034  | 0.081      | 0.167      | 0.840           | 0.698        | 0.064             | 0.105  0.008  | 0.215  0.022  | 0.734  0.626  0.723  | 0.069  0.079  0.045 
+10    | 0.000010  | 0.080      | 0.167      | 0.839           | 0.697        | 0.066             | 0.104  0.008  | 0.215  0.022  | 0.733  0.626  0.719  | 0.070  0.079  0.050 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dice_loss * 0.75 + BCE_loss * (1-0.75)
+LR_5e-4_1e-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.384      | 0.203      | 0.796           | 0.628        | 0.093             | 0.489  0.067  | 0.264  0.018  | 0.671  0.553  0.666  | 0.101  0.084  0.094 
+2     | 0.000500  | 0.142      | 0.186      | 0.777           | 0.631        | 0.125             | 0.185  0.013  | 0.242  0.019  | 0.670  0.566  0.710  | 0.203  0.112  0.060 
+3     | 0.000500  | 0.123      | 0.185      | 0.828           | 0.671        | 0.068             | 0.160  0.012  | 0.240  0.021  | 0.709  0.598  0.686  | 0.085  0.059  0.061 
+4     | 0.000480  | 0.113      | 0.203      | 0.823           | 0.651        | 0.062             | 0.147  0.011  | 0.263  0.023  | 0.702  0.545  0.686  | 0.077  0.058  0.051 
+5     | 0.000425  | 0.103      | 0.177      | 0.805           | 0.656        | 0.095             | 0.133  0.011  | 0.228  0.023  | 0.687  0.593  0.714  | 0.127  0.078  0.080 
+6     | 0.000345  | 0.096      | 0.177      | 0.821           | 0.680        | 0.085             | 0.124  0.010  | 0.228  0.021  | 0.717  0.603  0.707  | 0.127  0.074  0.053 
+7     | 0.000255  | 0.090      | 0.183      | 0.821           | 0.672        | 0.080             | 0.117  0.009  | 0.236  0.024  | 0.713  0.591  0.699  | 0.088  0.085  0.067 
+8     | 0.000175  | 0.084      | 0.170      | 0.830           | 0.690        | 0.076             | 0.109  0.009  | 0.220  0.022  | 0.723  0.620  0.731  | 0.094  0.074  0.060 
+9     | 0.000120  | 0.081      | 0.172      | 0.830           | 0.687        | 0.075             | 0.105  0.008  | 0.221  0.023  | 0.719  0.608  0.732  | 0.081  0.091  0.051 
+10    | 0.000100  | 0.079      | 0.170      | 0.828           | 0.685        | 0.077             | 0.103  0.008  | 0.218  0.023  | 0.716  0.614  0.726  | 0.087  0.087  0.059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5 * DiceLoss() + 
+0.5 * LovaszLoss(per_image=True) 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-L  | VLo-D  VLo-L  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.930      | 0.762      | 0.506           | 0.049        | 0.190             | 0.971  0.890  | 0.958  0.566  | 0.145  0.000  0.001  | 0.183  0.145  0.243 
+2     | 0.000500  | 0.720      | 0.683      | 0.568           | 0.153        | 0.156             | 0.911  0.529  | 0.892  0.474  | 0.241  0.221  0.000  | 0.140  0.134  0.193 
+3     | 0.000500  | 0.682      | 0.652      | 0.550           | 0.092        | 0.144             | 0.837  0.528  | 0.829  0.475  | 0.270  0.000  0.001  | 0.141  0.102  0.190 
+4     | 0.000476  | 0.646      | 0.642      | 0.628           | 0.288        | 0.146             | 0.774  0.518  | 0.766  0.517  | 0.348  0.283  0.235  | 0.130  0.124  0.182 
+5     | 0.000408  | 0.629      | 0.622      | 0.640           | 0.310        | 0.140             | 0.745  0.513  | 0.742  0.502  | 0.379  0.304  0.263  | 0.130  0.114  0.177 
+6     | 0.000310  | 0.612      | 0.629      | 0.649           | 0.335        | 0.142             | 0.716  0.508  | 0.716  0.543  | 0.466  0.276  0.275  | 0.125  0.117  0.183 
+7     | 0.000200  | 0.599      | 0.608      | 0.655           | 0.351        | 0.142             | 0.688  0.510  | 0.698  0.519  | 0.468  0.305  0.277  | 0.128  0.115  0.184 
+8     | 0.000102  | 0.588      | 0.607      | 0.653           | 0.350        | 0.144             | 0.670  0.505  | 0.695  0.520  | 0.466  0.309  0.273  | 0.131  0.115  0.188 
+9     | 0.000034  | 0.582      | 0.611      | 0.665           | 0.370        | 0.138             | 0.661  0.502  | 0.682  0.540  | 0.484  0.351  0.277  | 0.125  0.107  0.183 
+10    | 0.000010  | 0.579      | 0.608      | 0.664           | 0.367        | 0.139             | 0.659  0.500  | 0.681  0.535  | 0.486  0.338  0.280  | 0.126  0.107  0.183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5 * DiceLoss() + 
+0.5 * LovaszLoss(per_image=True)
+LR_1e-3_1e-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-L  | VLo-D  VLo-L  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.001000  | 0.852      | 0.814      | 0.473           | 0.073        | 0.260             | 0.958  0.746  | 0.956  0.673  | 0.095  0.080  0.044  | 0.256  0.245  0.280 
+2     | 0.001000  | 0.698      | 0.677      | 0.538           | 0.075        | 0.153             | 0.865  0.532  | 0.853  0.500  | 0.006  0.219  0.000  | 0.134  0.136  0.188 
+3     | 0.001000  | 0.658      | 0.667      | 0.571           | 0.143        | 0.143             | 0.786  0.530  | 0.811  0.522  | 0.002  0.228  0.207  | 0.116  0.130  0.183 
+4     | 0.000955  | 0.638      | 0.695      | 0.610           | 0.224        | 0.133             | 0.743  0.533  | 0.740  0.649  | 0.424  0.010  0.236  | 0.123  0.100  0.176 
+5     | 0.000831  | 0.615      | 0.611      | 0.650           | 0.333        | 0.138             | 0.706  0.524  | 0.720  0.501  | 0.467  0.253  0.270  | 0.129  0.099  0.186 
+6     | 0.000650  | 0.600      | 0.608      | 0.668           | 0.369        | 0.133             | 0.683  0.516  | 0.690  0.526  | 0.479  0.357  0.274  | 0.118  0.101  0.180 
+7     | 0.000450  | 0.585      | 0.599      | 0.673           | 0.374        | 0.129             | 0.660  0.510  | 0.674  0.525  | 0.490  0.338  0.288  | 0.112  0.097  0.176 
+8     | 0.000269  | 0.513      | 0.459      | 0.819           | 0.645        | 0.065             | 0.527  0.499  | 0.376  0.542  | 0.688  0.521  0.679  | 0.074  0.076  0.046 
+9     | 0.000145  | 0.349      | 0.453      | 0.814           | 0.643        | 0.072             | 0.300  0.397  | 0.352  0.553  | 0.691  0.538  0.644  | 0.073  0.078  0.063 
+10    | 0.000100  | 0.321      | 0.435      | 0.822           | 0.658        | 0.068             | 0.272  0.371  | 0.333  0.537  | 0.703  0.546  0.674  | 0.075  0.066  0.063 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5 * DiceLoss() + 
+0.5 * LovaszLoss(per_image=True)
+LR_1e-3_3e-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-L  | VLo-D  VLo-L  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.001000  | 0.871      | 1.000      | 0.162           | 0.000        | 0.730             | 0.963  0.779  | 0.961  1.039  | 0.000  0.000  0.000  | 0.774  0.559  0.857 
+2     | 0.001000  | 0.732      | 0.679      | 0.592           | 0.198        | 0.144             | 0.902  0.562  | 0.851  0.508  | 0.254  0.250  0.107  | 0.134  0.120  0.179 
+3     | 0.001000  | 0.675      | 0.653      | 0.607           | 0.228        | 0.140             | 0.818  0.532  | 0.774  0.532  | 0.283  0.261  0.167  | 0.130  0.116  0.175 
+4     | 0.000965  | 0.678      | 0.645      | 0.573           | 0.138        | 0.138             | 0.796  0.559  | 0.789  0.500  | 0.175  0.123  0.125  | 0.132  0.112  0.170 
+5     | 0.000868  | 0.642      | 0.635      | 0.612           | 0.250        | 0.147             | 0.760  0.524  | 0.778  0.493  | 0.322  0.232  0.202  | 0.135  0.126  0.179 
+6     | 0.000728  | 0.629      | 0.625      | 0.625           | 0.282        | 0.146             | 0.744  0.515  | 0.746  0.504  | 0.359  0.295  0.194  | 0.134  0.122  0.181 
+7     | 0.000572  | 0.619      | 0.619      | 0.612           | 0.234        | 0.137             | 0.731  0.507  | 0.744  0.493  | 0.344  0.102  0.270  | 0.129  0.110  0.171 
+8     | 0.000432  | 0.605      | 0.622      | 0.632           | 0.285        | 0.137             | 0.703  0.506  | 0.713  0.530  | 0.448  0.153  0.267  | 0.125  0.110  0.177 
+9     | 0.000335  | 0.591      | 0.607      | 0.655           | 0.342        | 0.136             | 0.679  0.502  | 0.700  0.514  | 0.471  0.281  0.288  | 0.123  0.107  0.179 
+10    | 0.000300  | 0.589      | 0.607      | 0.684           | 0.402        | 0.127             | 0.669  0.509  | 0.678  0.537  | 0.484  0.425  0.302  | 0.117  0.087  0.176 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dice * 0.45 + lovasz * 0.4 + bce * 0.15
+LR_1e-3_1e-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-L  TLo-B  | VLo-D  VLo-L  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+--------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.001000  | 0.730      | 0.599      | 0.544           | 0.067        | 0.138             | 0.917  0.741  0.138  | 0.829  0.554  0.032  | 0.008  0.001  0.192  | 0.125  0.109  0.179 
+2     | 0.001000  | 0.577      | 0.617      | 0.548           | 0.139        | 0.180             | 0.795  0.537  0.029  | 0.835  0.590  0.035  | 0.220  0.196  0.001  | 0.168  0.174  0.198 
+3     | 0.001000  | 0.558      | 0.543      | 0.639           | 0.299        | 0.135             | 0.746  0.546  0.021  | 0.744  0.512  0.020  | 0.429  0.204  0.252  | 0.124  0.102  0.179 
+4     | 0.000955  | 0.395      | 0.431      | 0.778           | 0.577        | 0.088             | 0.424  0.507  0.009  | 0.426  0.596  0.009  | 0.600  0.543  0.519  | 0.059  0.070  0.135 
+5     | 0.000831  | 0.284      | 0.350      | 0.833           | 0.670        | 0.058             | 0.271  0.402  0.006  | 0.316  0.517  0.007  | 0.700  0.578  0.714  | 0.068  0.063  0.042 
+6     | 0.000650  | 0.244      | 0.354      | 0.831           | 0.670        | 0.062             | 0.229  0.350  0.005  | 0.301  0.543  0.007  | 0.706  0.585  0.703  | 0.077  0.059  0.049 
+7     | 0.000450  | 0.217      | 0.352      | 0.838           | 0.681        | 0.058             | 0.203  0.313  0.004  | 0.288  0.553  0.007  | 0.715  0.603  0.698  | 0.065  0.063  0.047 
+8     | 0.000269  | 0.199      | 0.350      | 0.844           | 0.695        | 0.057             | 0.186  0.288  0.004  | 0.271  0.569  0.007  | 0.728  0.603  0.734  | 0.070  0.063  0.039 
+9     | 0.000145  | 0.186      | 0.356      | 0.839           | 0.687        | 0.060             | 0.173  0.269  0.004  | 0.274  0.578  0.007  | 0.718  0.602  0.731  | 0.071  0.069  0.040 
+10    | 0.000100  | 0.179      | 0.356      | 0.842           | 0.693        | 0.059             | 0.166  0.260  0.003  | 0.266  0.589  0.007  | 0.722  0.609  0.727  | 0.069  0.064  0.043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dice * 0.45 + lovasz * 0.4 + bce * 0.15
+LR_1e-3_1e-4  15epochs
+(1h 18min 4s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-L  TLo-B  | VLo-D  VLo-L  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+--------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.001000  | 0.725      | 0.618      | 0.554           | 0.108        | 0.149             | 0.916  0.729  0.139  | 0.857  0.565  0.041  | 0.156  0.163  0.006  | 0.137  0.124  0.184 
+2     | 0.001000  | 0.583      | 0.561      | 0.614           | 0.247        | 0.141             | 0.800  0.547  0.030  | 0.785  0.509  0.024  | 0.300  0.270  0.173  | 0.133  0.116  0.174 
+3     | 0.001000  | 0.557      | 0.541      | 0.607           | 0.238        | 0.148             | 0.756  0.535  0.023  | 0.764  0.486  0.022  | 0.330  0.246  0.141  | 0.137  0.123  0.183 
+4     | 0.000985  | 0.543      | 0.536      | 0.653           | 0.330        | 0.131             | 0.721  0.538  0.019  | 0.711  0.534  0.017  | 0.465  0.323  0.219  | 0.117  0.102  0.174 
+5     | 0.000940  | 0.400      | 0.361      | 0.825           | 0.656        | 0.063             | 0.431  0.511  0.010  | 0.350  0.507  0.007  | 0.684  0.552  0.730  | 0.082  0.070  0.037 
+6     | 0.000868  | 0.291      | 0.366      | 0.826           | 0.658        | 0.062             | 0.278  0.411  0.006  | 0.328  0.542  0.008  | 0.692  0.554  0.723  | 0.081  0.075  0.029 
+7     | 0.000775  | 0.259      | 0.352      | 0.822           | 0.657        | 0.068             | 0.244  0.370  0.005  | 0.313  0.526  0.007  | 0.693  0.556  0.721  | 0.100  0.061  0.043 
+8     | 0.000666  | 0.232      | 0.363      | 0.830           | 0.673        | 0.065             | 0.217  0.335  0.005  | 0.295  0.573  0.008  | 0.704  0.590  0.715  | 0.080  0.080  0.037 
+9     | 0.000550  | 0.215      | 0.364      | 0.836           | 0.680        | 0.061             | 0.199  0.312  0.004  | 0.286  0.586  0.008  | 0.712  0.590  0.726  | 0.072  0.071  0.040 
+10    | 0.000434  | 0.197      | 0.334      | 0.845           | 0.697        | 0.057             | 0.182  0.286  0.004  | 0.270  0.529  0.007  | 0.729  0.605  0.735  | 0.068  0.068  0.034 
+11    | 0.000325  | 0.186      | 0.337      | 0.846           | 0.698        | 0.056             | 0.171  0.270  0.004  | 0.270  0.535  0.007  | 0.734  0.608  0.743  | 0.067  0.071  0.031 
+12    | 0.000232  | 0.178      | 0.355      | 0.845           | 0.699        | 0.058             | 0.165  0.257  0.003  | 0.265  0.587  0.008  | 0.731  0.605  0.738  | 0.073  0.067  0.033 
+13    | 0.000160  | 0.170      | 0.343      | 0.848           | 0.708        | 0.058             | 0.158  0.247  0.003  | 0.258  0.566  0.007  | 0.737  0.620  0.749  | 0.068  0.071  0.036 
+14    | 0.000115  | 0.166      | 0.355      | 0.845           | 0.701        | 0.059             | 0.154  0.241  0.003  | 0.258  0.595  0.008  | 0.734  0.610  0.739  | 0.069  0.069  0.040 
+15    | 0.000100  | 0.161      | 0.350      | 0.847           | 0.705        | 0.058             | 0.149  0.233  0.003  | 0.255  0.586  0.008  | 0.732  0.617  0.745  | 0.067  0.071  0.035 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also include 
+A.CoarseDropout(
+    num_holes_range = (3,6), 
+    hole_height_range = (0.025,0.05),
+    hole_width_range = (0.025,0.05), 
+    fill_mask = 0, p = 0.25
+)
+loss_wt = 0.5
+i.e. dice_loss * 0.5 + BCE_loss * 0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.294      | 0.145      | 0.814           | 0.638        | 0.068             | 0.522  0.066  | 0.274  0.016  | 0.681  0.541  0.686  | 0.075  0.069  0.060 
+2     | 0.000500  | 0.100      | 0.133      | 0.828           | 0.661        | 0.060             | 0.189  0.011  | 0.250  0.016  | 0.685  0.575  0.724  | 0.075  0.072  0.034 
+3     | 0.000500  | 0.085      | 0.126      | 0.820           | 0.667        | 0.079             | 0.160  0.010  | 0.235  0.017  | 0.697  0.592  0.728  | 0.089  0.084  0.063 
+4     | 0.000476  | 0.078      | 0.137      | 0.831           | 0.664        | 0.058             | 0.147  0.009  | 0.255  0.018  | 0.702  0.559  0.720  | 0.073  0.051  0.049 
+5     | 0.000408  | 0.071      | 0.122      | 0.830           | 0.683        | 0.072             | 0.134  0.008  | 0.226  0.018  | 0.707  0.609  0.743  | 0.083  0.094  0.039 
+6     | 0.000310  | 0.066      | 0.124      | 0.819           | 0.669        | 0.081             | 0.124  0.008  | 0.230  0.018  | 0.703  0.591  0.728  | 0.123  0.075  0.045 
+7     | 0.000200  | 0.061      | 0.121      | 0.835           | 0.684        | 0.063             | 0.115  0.007  | 0.224  0.018  | 0.714  0.608  0.734  | 0.069  0.070  0.052 
+8     | 0.000102  | 0.058      | 0.119      | 0.835           | 0.693        | 0.070             | 0.109  0.007  | 0.221  0.017  | 0.720  0.618  0.744  | 0.080  0.089  0.042 
+9     | 0.000034  | 0.056      | 0.119      | 0.836           | 0.692        | 0.068             | 0.105  0.006  | 0.220  0.018  | 0.720  0.621  0.738  | 0.077  0.083  0.042 
+10    | 0.000010  | 0.055      | 0.119      | 0.834           | 0.692        | 0.071             | 0.103  0.006  | 0.220  0.018  | 0.720  0.619  0.740  | 0.080  0.083  0.051 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.CoarseDropout(
+    num_holes_range = (1,4), 
+    hole_height_range = (0.01,0.05),
+    hole_width_range = (0.01,0.05), 
+    fill_mask = 0, p = 0.25
+)
+loss_wt = 0.5
+i.e. dice_loss * 0.5 + BCE_loss * 0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.291      | 0.142      | 0.810           | 0.636        | 0.074             | 0.515  0.066  | 0.269  0.015  | 0.681  0.551  0.681  | 0.077  0.075  0.072 
+2     | 0.000500  | 0.098      | 0.131      | 0.816           | 0.659        | 0.079             | 0.186  0.011  | 0.245  0.016  | 0.693  0.574  0.723  | 0.074  0.104  0.059 
+3     | 0.000500  | 0.086      | 0.131      | 0.807           | 0.645        | 0.086             | 0.162  0.010  | 0.244  0.018  | 0.693  0.558  0.708  | 0.098  0.088  0.071 
+4     | 0.000476  | 0.077      | 0.129      | 0.827           | 0.668        | 0.067             | 0.145  0.009  | 0.240  0.017  | 0.712  0.587  0.707  | 0.079  0.070  0.051 
+5     | 0.000408  | 0.070      | 0.121      | 0.823           | 0.670        | 0.075             | 0.133  0.008  | 0.224  0.017  | 0.702  0.591  0.744  | 0.075  0.104  0.044 
+6     | 0.000310  | 0.064      | 0.120      | 0.842           | 0.693        | 0.059             | 0.121  0.008  | 0.224  0.017  | 0.717  0.620  0.741  | 0.066  0.069  0.042 
+7     | 0.000200  | 0.060      | 0.121      | 0.833           | 0.688        | 0.071             | 0.113  0.007  | 0.224  0.018  | 0.720  0.610  0.734  | 0.077  0.070  0.064 
+8     | 0.000102  | 0.057      | 0.121      | 0.834           | 0.687        | 0.068             | 0.107  0.007  | 0.225  0.018  | 0.711  0.609  0.750  | 0.080  0.080  0.043 
+9     | 0.000034  | 0.055      | 0.121      | 0.836           | 0.691        | 0.067             | 0.104  0.006  | 0.225  0.017  | 0.714  0.614  0.751  | 0.084  0.075  0.042 
+10    | 0.000010  | 0.054      | 0.120      | 0.836           | 0.694        | 0.069             | 0.103  0.006  | 0.223  0.018  | 0.717  0.614  0.751  | 0.088  0.078  0.042 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.RandomBrightnessContrast(
+   brightness_limit = 0.1, 
+   contrast_limit = 0.1, 
+   p = 0.25
+)
+loss_wt = 0.5
+i.e. dice_loss * 0.5 + BCE_loss * 0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.291      | 0.175      | 0.795           | 0.587        | 0.066             | 0.517  0.066  | 0.332  0.018  | 0.615  0.488  0.626  | 0.060  0.061  0.077 
+2     | 0.000500  | 0.103      | 0.132      | 0.763           | 0.602        | 0.130             | 0.194  0.011  | 0.249  0.016  | 0.647  0.544  0.696  | 0.164  0.152  0.073 
+3     | 0.000500  | 0.088      | 0.131      | 0.792           | 0.637        | 0.104             | 0.165  0.010  | 0.244  0.018  | 0.686  0.548  0.728  | 0.104  0.147  0.061 
+4     | 0.000476  | 0.078      | 0.129      | 0.819           | 0.654        | 0.072             | 0.147  0.009  | 0.241  0.018  | 0.696  0.566  0.714  | 0.097  0.065  0.053 
+5     | 0.000408  | 0.071      | 0.125      | 0.830           | 0.678        | 0.069             | 0.133  0.008  | 0.232  0.018  | 0.704  0.607  0.726  | 0.079  0.065  0.062 
+6     | 0.000310  | 0.065      | 0.120      | 0.827           | 0.688        | 0.080             | 0.123  0.008  | 0.223  0.017  | 0.726  0.612  0.726  | 0.096  0.083  0.060 
+7     | 0.000200  | 0.061      | 0.125      | 0.820           | 0.673        | 0.082             | 0.115  0.007  | 0.230  0.019  | 0.704  0.606  0.715  | 0.104  0.078  0.064 
+8     | 0.000102  | 0.058      | 0.121      | 0.827           | 0.680        | 0.075             | 0.110  0.007  | 0.224  0.018  | 0.714  0.608  0.720  | 0.087  0.083  0.056 
+9     | 0.000034  | 0.056      | 0.121      | 0.828           | 0.681        | 0.074             | 0.105  0.006  | 0.224  0.018  | 0.715  0.610  0.719  | 0.087  0.079  0.057 
+10    | 0.000010  | 0.056      | 0.121      | 0.827           | 0.682        | 0.076             | 0.105  0.006  | 0.224  0.018  | 0.717  0.610  0.721  | 0.094  0.079  0.056 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.RandomBrightnessContrast(
+   brightness_limit = 0.075, 
+   contrast_limit = 0.075, 
+   p = 0.25
+)
+loss_wt = 0.5
+i.e. dice_loss * 0.5 + BCE_loss * 0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.291      | 0.147      | 0.814           | 0.635        | 0.067             | 0.515  0.066  | 0.278  0.016  | 0.665  0.536  0.692  | 0.064  0.075  0.062 
+2     | 0.000500  | 0.099      | 0.131      | 0.770           | 0.600        | 0.117             | 0.186  0.011  | 0.245  0.017  | 0.674  0.514  0.714  | 0.124  0.181  0.046 
+3     | 0.000500  | 0.086      | 0.130      | 0.803           | 0.647        | 0.093             | 0.163  0.010  | 0.241  0.018  | 0.673  0.578  0.717  | 0.129  0.094  0.055 
+4     | 0.000476  | 0.076      | 0.129      | 0.824           | 0.665        | 0.070             | 0.142  0.009  | 0.240  0.017  | 0.692  0.578  0.730  | 0.104  0.065  0.041 
+5     | 0.000408  | 0.069      | 0.121      | 0.832           | 0.683        | 0.069             | 0.130  0.008  | 0.224  0.018  | 0.704  0.605  0.745  | 0.089  0.077  0.041 
+6     | 0.000310  | 0.064      | 0.122      | 0.824           | 0.679        | 0.080             | 0.121  0.008  | 0.226  0.018  | 0.704  0.614  0.731  | 0.119  0.072  0.050 
+7     | 0.000200  | 0.060      | 0.119      | 0.842           | 0.697        | 0.061             | 0.112  0.007  | 0.221  0.017  | 0.724  0.620  0.750  | 0.077  0.064  0.043 
+8     | 0.000102  | 0.057      | 0.116      | 0.840           | 0.703        | 0.068             | 0.107  0.007  | 0.215  0.017  | 0.729  0.627  0.754  | 0.087  0.074  0.042 
+9     | 0.000034  | 0.055      | 0.116      | 0.841           | 0.701        | 0.065             | 0.104  0.006  | 0.215  0.017  | 0.724  0.628  0.754  | 0.074  0.077  0.045 
+10    | 0.000010  | 0.054      | 0.115      | 0.841           | 0.703        | 0.067             | 0.101  0.006  | 0.213  0.017  | 0.728  0.629  0.753  | 0.075  0.082  0.045 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.GaussNoise(
+   std_range = (0.01, 0.05), 
+   mean_range = (0.0, 0.0), 
+   P = 0.125
+)
+loss_wt = 0.5
+i.e. dice_loss * 0.5 + BCE_loss * 0.5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.289      | 0.149      | 0.814           | 0.635        | 0.066             | 0.512  0.066  | 0.283  0.015  | 0.665  0.545  0.683  | 0.078  0.064  0.057 
+2     | 0.000500  | 0.101      | 0.136      | 0.809           | 0.643        | 0.080             | 0.191  0.011  | 0.255  0.017  | 0.679  0.551  0.721  | 0.111  0.082  0.048 
+3     | 0.000500  | 0.088      | 0.132      | 0.817           | 0.652        | 0.073             | 0.165  0.010  | 0.246  0.018  | 0.688  0.573  0.729  | 0.103  0.081  0.036 
+4     | 0.000476  | 0.077      | 0.139      | 0.821           | 0.655        | 0.069             | 0.145  0.009  | 0.259  0.019  | 0.681  0.568  0.726  | 0.083  0.080  0.043 
+5     | 0.000408  | 0.072      | 0.123      | 0.818           | 0.672        | 0.085             | 0.135  0.009  | 0.228  0.018  | 0.712  0.589  0.733  | 0.103  0.108  0.045 
+6     | 0.000310  | 0.066      | 0.121      | 0.831           | 0.683        | 0.071             | 0.123  0.008  | 0.226  0.017  | 0.716  0.611  0.726  | 0.088  0.072  0.052 
+7     | 0.000200  | 0.061      | 0.123      | 0.833           | 0.691        | 0.072             | 0.115  0.007  | 0.227  0.018  | 0.725  0.623  0.725  | 0.086  0.086  0.044 
+8     | 0.000102  | 0.058      | 0.121      | 0.831           | 0.684        | 0.070             | 0.110  0.007  | 0.224  0.018  | 0.712  0.610  0.733  | 0.085  0.087  0.037 
+9     | 0.000034  | 0.056      | 0.121      | 0.839           | 0.691        | 0.063             | 0.106  0.006  | 0.223  0.018  | 0.722  0.614  0.733  | 0.078  0.072  0.038 
+10    | 0.000010  | 0.054      | 0.120      | 0.838           | 0.692        | 0.065             | 0.102  0.006  | 0.222  0.018  | 0.722  0.616  0.736  | 0.084  0.073  0.037 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.GaussNoise(
+   std_range = (0.01, 0.03), 
+   mean_range = (0.0, 0.0), 
+   P = 0.125
+)
+loss_wt = 0.5
+i.e. dice_loss * 0.5 + BCE_loss * 0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.296      | 0.152      | 0.778           | 0.597        | 0.101             | 0.525  0.066  | 0.290  0.015  | 0.640  0.521  0.641  | 0.161  0.086  0.058 
+2     | 0.000500  | 0.102      | 0.137      | 0.781           | 0.609        | 0.104             | 0.193  0.011  | 0.257  0.018  | 0.644  0.541  0.689  | 0.143  0.107  0.063 
+3     | 0.000500  | 0.087      | 0.130      | 0.791           | 0.632        | 0.102             | 0.163  0.010  | 0.242  0.019  | 0.678  0.554  0.722  | 0.136  0.128  0.043 
+4     | 0.000476  | 0.079      | 0.131      | 0.825           | 0.664        | 0.068             | 0.148  0.009  | 0.245  0.018  | 0.702  0.565  0.719  | 0.092  0.059  0.052 
+5     | 0.000408  | 0.072      | 0.126      | 0.805           | 0.645        | 0.089             | 0.135  0.008  | 0.234  0.018  | 0.674  0.584  0.723  | 0.136  0.074  0.057 
+6     | 0.000310  | 0.066      | 0.125      | 0.802           | 0.655        | 0.099             | 0.125  0.008  | 0.231  0.018  | 0.689  0.591  0.708  | 0.149  0.085  0.063 
+7     | 0.000200  | 0.061      | 0.121      | 0.831           | 0.675        | 0.065             | 0.116  0.007  | 0.224  0.018  | 0.710  0.607  0.713  | 0.078  0.075  0.041 
+8     | 0.000102  | 0.058      | 0.119      | 0.831           | 0.683        | 0.071             | 0.109  0.007  | 0.220  0.017  | 0.715  0.615  0.720  | 0.091  0.076  0.045 
+9     | 0.000034  | 0.056      | 0.119      | 0.830           | 0.681        | 0.070             | 0.105  0.006  | 0.220  0.017  | 0.714  0.615  0.716  | 0.089  0.075  0.047 
+10    | 0.000010  | 0.055      | 0.118      | 0.829           | 0.681        | 0.072             | 0.104  0.006  | 0.218  0.018  | 0.715  0.617  0.716  | 0.088  0.078  0.050 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.120      | 0.830           | 0.684        | 0.073             | 0.221  0.018  | 0.714  0.618  0.722  | 0.092  0.077  0.051 
+360     | 310     | 0.135      | 0.816           | 0.647        | 0.071             | 0.258  0.011  | 0.692  0.588  0.721  | 0.069  0.103  0.041 
+276     | 276     | 0.105      | 0.842           | 0.691        | 0.058             | 0.188  0.022  | 0.763  0.633  0.610  | 0.058  0.060  0.055 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Trained on 256x256 images with settings from
+'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Without 3 problem casedays</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">’ run
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(used LOAD_RESIZED = True)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(1h 7min 12s)
+(Max GPU mem usage : 15060.875 MB)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.288      | 0.141      | 0.785           | 0.614        | 0.100             | 0.511  0.065  | 0.268  0.015  | 0.699  0.536  0.644  | 0.109  0.096  0.096 
+2     | 0.000500  | 0.096      | 0.130      | 0.787           | 0.622        | 0.103             | 0.181  0.010  | 0.243  0.017  | 0.702  0.529  0.726  | 0.095  0.184  0.030 
+3     | 0.000500  | 0.083      | 0.120      | 0.795           | 0.653        | 0.111             | 0.157  0.010  | 0.223  0.016  | 0.710  0.574  0.723  | 0.127  0.147  0.058 
+4     | 0.000476  | 0.074      | 0.125      | 0.833           | 0.679        | 0.065             | 0.139  0.009  | 0.232  0.017  | 0.708  0.599  0.728  | 0.072  0.061  0.062 
+5     | 0.000408  | 0.068      | 0.122      | 0.833           | 0.679        | 0.065             | 0.128  0.008  | 0.226  0.018  | 0.715  0.604  0.733  | 0.074  0.068  0.053 
+6     | 0.000310  | 0.062      | 0.115      | 0.834           | 0.691        | 0.071             | 0.117  0.007  | 0.214  0.016  | 0.725  0.627  0.727  | 0.082  0.081  0.051 
+7     | 0.000200  | 0.059      | 0.118      | 0.833           | 0.688        | 0.071             | 0.111  0.007  | 0.219  0.017  | 0.724  0.608  0.746  | 0.074  0.094  0.045 
+8     | 0.000102  | 0.055      | 0.113      | 0.850           | 0.709        | 0.055             | 0.104  0.006  | 0.209  0.017  | 0.733  0.631  0.760  | 0.063  0.067  0.035 
+9     | 0.000034  | 0.053      | 0.113      | 0.846           | 0.707        | 0.060             | 0.100  0.006  | 0.210  0.017  | 0.734  0.630  0.754  | 0.069  0.072  0.040 
+10    | 0.000010  | 0.052      | 0.113      | 0.842           | 0.703        | 0.066             | 0.098  0.006  | 0.209  0.017  | 0.731  0.627  0.754  | 0.073  0.081  0.042 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.113      | 0.842           | 0.704        | 0.066             | 0.207  0.018  | 0.728  0.626  0.759  | 0.072  0.083  0.044 
+360     | 310     | 0.129      | 0.833           | 0.682        | 0.066             | 0.247  0.011  | 0.735  0.630  0.734  | 0.095  0.073  0.029 
+276     | 276     | 0.095      | 0.859           | 0.725        | 0.052             | 0.170  0.020  | 0.792  0.654  0.708  | 0.051  0.073  0.031 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trained on 288x288 images with settings from
+'Without 3 problem casedays’ run
+(used LOAD_RESIZED = False)
+(1h 20min 55s)
+(Max GPU mem usage : 12884.875 MB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.288      | 0.145      | 0.818           | 0.639        | 0.063             | 0.510  0.065  | 0.274  0.015  | 0.673  0.550  0.687  | 0.060  0.062  0.066 
+2     | 0.000500  | 0.094      | 0.132      | 0.817           | 0.643        | 0.067             | 0.178  0.010  | 0.247  0.016  | 0.673  0.562  0.704  | 0.086  0.081  0.034 
+3     | 0.000500  | 0.083      | 0.120      | 0.836           | 0.687        | 0.064             | 0.156  0.010  | 0.223  0.017  | 0.727  0.606  0.730  | 0.063  0.073  0.055 
+4     | 0.000476  | 0.074      | 0.117      | 0.841           | 0.699        | 0.064             | 0.139  0.009  | 0.219  0.016  | 0.737  0.623  0.730  | 0.071  0.062  0.060 
+5     | 0.000408  | 0.068      | 0.118      | 0.833           | 0.685        | 0.069             | 0.127  0.008  | 0.219  0.017  | 0.715  0.619  0.727  | 0.089  0.089  0.029 
+6     | 0.000310  | 0.062      | 0.123      | 0.822           | 0.669        | 0.076             | 0.117  0.007  | 0.228  0.017  | 0.702  0.599  0.734  | 0.074  0.101  0.052 
+7     | 0.000200  | 0.058      | 0.113      | 0.844           | 0.705        | 0.064             | 0.109  0.007  | 0.208  0.017  | 0.735  0.630  0.749  | 0.063  0.072  0.058 
+8     | 0.000102  | 0.055      | 0.111      | 0.844           | 0.705        | 0.064             | 0.103  0.006  | 0.205  0.017  | 0.732  0.638  0.749  | 0.071  0.069  0.053 
+9     | 0.000034  | 0.053      | 0.111      | 0.848           | 0.710        | 0.060             | 0.099  0.006  | 0.205  0.017  | 0.736  0.640  0.753  | 0.066  0.072  0.042 
+10    | 0.000010  | 0.052      | 0.111      | 0.846           | 0.710        | 0.062             | 0.097  0.006  | 0.205  0.017  | 0.737  0.639  0.754  | 0.067  0.072  0.048 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.112      | 0.846           | 0.709        | 0.064             | 0.206  0.018  | 0.731  0.638  0.760  | 0.069  0.072  0.050 
+360     | 310     | 0.116      | 0.847           | 0.693        | 0.051             | 0.223  0.010  | 0.747  0.627  0.761  | 0.057  0.067  0.029 
+276     | 276     | 0.089      | 0.862           | 0.745        | 0.060             | 0.159  0.019  | 0.824  0.679  0.650  | 0.060  0.068  0.051 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">On 224x224 images with final LR 5e-5
+BS = 64
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(used LOAD_RESIZED = False)
+(52min 54s)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Max GPU mem usage : 9768.875 MB)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.291      | 0.150      | 0.817           | 0.629        | 0.057             | 0.516  0.066  | 0.285  0.016  | 0.652  0.549  0.684  | 0.071  0.071  0.030 
+2     | 0.000500  | 0.099      | 0.128      | 0.823           | 0.662        | 0.070             | 0.187  0.011  | 0.241  0.016  | 0.699  0.579  0.721  | 0.097  0.073  0.040 
+3     | 0.000500  | 0.085      | 0.126      | 0.774           | 0.627        | 0.128             | 0.161  0.010  | 0.236  0.017  | 0.667  0.581  0.702  | 0.198  0.099  0.087 
+4     | 0.000478  | 0.076      | 0.130      | 0.831           | 0.666        | 0.060             | 0.143  0.009  | 0.243  0.018  | 0.708  0.573  0.722  | 0.074  0.073  0.033 
+5     | 0.000415  | 0.070      | 0.121      | 0.838           | 0.688        | 0.062             | 0.133  0.008  | 0.226  0.017  | 0.718  0.612  0.733  | 0.072  0.062  0.053 
+6     | 0.000325  | 0.065      | 0.124      | 0.826           | 0.672        | 0.071             | 0.122  0.008  | 0.231  0.017  | 0.709  0.596  0.712  | 0.087  0.086  0.040 
+7     | 0.000225  | 0.061      | 0.123      | 0.832           | 0.684        | 0.069             | 0.114  0.007  | 0.227  0.018  | 0.713  0.610  0.734  | 0.082  0.080  0.045 
+8     | 0.000135  | 0.057      | 0.119      | 0.836           | 0.690        | 0.066             | 0.107  0.007  | 0.221  0.017  | 0.720  0.615  0.734  | 0.077  0.076  0.044 
+9     | 0.000072  | 0.054      | 0.121      | 0.837           | 0.691        | 0.065             | 0.102  0.006  | 0.224  0.018  | 0.722  0.614  0.734  | 0.070  0.081  0.044 
+10    | 0.000050  | 0.053      | 0.119      | 0.841           | 0.694        | 0.060             | 0.100  0.006  | 0.220  0.018  | 0.725  0.619  0.733  | 0.067  0.068  0.046 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.121      | 0.842           | 0.697        | 0.061             | 0.223  0.019  | 0.722  0.622  0.745  | 0.069  0.070  0.045 
+360     | 310     | 0.136      | 0.833           | 0.654        | 0.047             | 0.261  0.011  | 0.732  0.559  0.693  | 0.056  0.059  0.027 
+276     | 276     | 0.106      | 0.839           | 0.696        | 0.065             | 0.190  0.023  | 0.765  0.651  0.611  | 0.053  0.062  0.081 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On 224x224 images 
+with grad_accu = 2, BS = 32 
+with final LR 5e-5
+(used LOAD_RESIZED = False)
+(58m 5s)
+(Max GPU mem usage : 5730.875 MB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.296      | 0.122      | 0.779           | 0.616        | 0.113             | 0.525  0.066  | 0.228  0.016  | 0.660  0.541  0.675  | 0.168  0.091  0.080 
+2     | 0.000500  | 0.101      | 0.110      | 0.795           | 0.627        | 0.093             | 0.192  0.011  | 0.204  0.016  | 0.675  0.555  0.698  | 0.126  0.079  0.074 
+3     | 0.000500  | 0.089      | 0.106      | 0.827           | 0.668        | 0.067             | 0.168  0.010  | 0.196  0.017  | 0.709  0.596  0.701  | 0.076  0.080  0.046 
+4     | 0.000478  | 0.081      | 0.110      | 0.820           | 0.662        | 0.075             | 0.152  0.009  | 0.203  0.018  | 0.685  0.587  0.734  | 0.118  0.076  0.031 
+5     | 0.000415  | 0.075      | 0.103      | 0.805           | 0.659        | 0.098             | 0.141  0.009  | 0.189  0.017  | 0.705  0.584  0.731  | 0.116  0.119  0.060 
+6     | 0.000325  | 0.068      | 0.105      | 0.819           | 0.672        | 0.084             | 0.128  0.008  | 0.193  0.017  | 0.710  0.618  0.709  | 0.113  0.103  0.036 
+7     | 0.000225  | 0.064      | 0.101      | 0.834           | 0.688        | 0.069             | 0.121  0.007  | 0.185  0.018  | 0.719  0.621  0.742  | 0.081  0.087  0.038 
+8     | 0.000135  | 0.060      | 0.102      | 0.826           | 0.689        | 0.082             | 0.113  0.007  | 0.187  0.018  | 0.726  0.614  0.752  | 0.109  0.088  0.049 
+9     | 0.000072  | 0.059      | 0.101      | 0.836           | 0.692        | 0.068             | 0.110  0.007  | 0.185  0.017  | 0.727  0.621  0.741  | 0.081  0.077  0.047 
+10    | 0.000050  | 0.057      | 0.100      | 0.835           | 0.692        | 0.069             | 0.107  0.006  | 0.182  0.018  | 0.723  0.623  0.743  | 0.083  0.078  0.048 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.096      | 0.835           | 0.693        | 0.070             | 0.175  0.018  | 0.720  0.623  0.750  | 0.080  0.080  0.049 
+360     | 310     | 0.087      | 0.827           | 0.675        | 0.072             | 0.164  0.009  | 0.729  0.599  0.722  | 0.135  0.055  0.026 
+276     | 276     | 0.101      | 0.846           | 0.711        | 0.064             | 0.182  0.020  | 0.773  0.657  0.671  | 0.056  0.083  0.054 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On 256x256 images with final LR 5e-5
+(used LOAD_RESIZED = False)
+(1h 9min 48s)
+(Max GPU mem usage : 15060.875 MB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.289      | 0.146      | 0.801           | 0.625        | 0.081             | 0.512  0.065  | 0.276  0.015  | 0.660  0.544  0.696  | 0.076  0.079  0.089 
+2     | 0.000500  | 0.097      | 0.130      | 0.759           | 0.581        | 0.122             | 0.184  0.011  | 0.244  0.017  | 0.639  0.508  0.716  | 0.158  0.161  0.046 
+3     | 0.000500  | 0.083      | 0.130      | 0.722           | 0.562        | 0.170             | 0.156  0.010  | 0.243  0.018  | 0.674  0.483  0.700  | 0.151  0.204  0.157 
+4     | 0.000478  | 0.076      | 0.126      | 0.830           | 0.677        | 0.067             | 0.143  0.009  | 0.235  0.017  | 0.713  0.597  0.719  | 0.085  0.087  0.031 
+5     | 0.000415  | 0.069      | 0.117      | 0.833           | 0.692        | 0.073             | 0.130  0.008  | 0.217  0.017  | 0.721  0.618  0.743  | 0.092  0.056  0.070 
+6     | 0.000325  | 0.064      | 0.115      | 0.831           | 0.689        | 0.075             | 0.120  0.008  | 0.213  0.016  | 0.722  0.615  0.741  | 0.072  0.105  0.048 
+7     | 0.000225  | 0.059      | 0.116      | 0.842           | 0.700        | 0.064             | 0.112  0.007  | 0.214  0.017  | 0.726  0.628  0.747  | 0.079  0.079  0.034 
+8     | 0.000135  | 0.056      | 0.113      | 0.848           | 0.708        | 0.059             | 0.106  0.007  | 0.210  0.017  | 0.735  0.635  0.753  | 0.071  0.065  0.040 
+9     | 0.000072  | 0.054      | 0.112      | 0.850           | 0.709        | 0.056             | 0.101  0.006  | 0.208  0.017  | 0.738  0.637  0.754  | 0.065  0.068  0.034 
+10    | 0.000050  | 0.052      | 0.112      | 0.848           | 0.710        | 0.060             | 0.098  0.006  | 0.207  0.017  | 0.736  0.640  0.748  | 0.070  0.067  0.043 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.112      | 0.848           | 0.714        | 0.062             | 0.207  0.018  | 0.736  0.642  0.756  | 0.073  0.070  0.044 
+360     | 310     | 0.125      | 0.843           | 0.670        | 0.042             | 0.239  0.011  | 0.715  0.615  0.736  | 0.051  0.052  0.024 
+276     | 276     | 0.106      | 0.847           | 0.695        | 0.051             | 0.189  0.022  | 0.765  0.638  0.649  | 0.057  0.051  0.046 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On 288x288 images with final LR 5e-5
+(used LOAD_RESIZED = False)
+(1h 20min 47s)
+(Max GPU mem usage : 12884.875 MB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.286      | 0.137      | 0.823           | 0.653        | 0.063             | 0.507  0.065  | 0.260  0.014  | 0.684  0.568  0.708  | 0.079  0.066  0.045 
+2     | 0.000500  | 0.094      | 0.128      | 0.804           | 0.637        | 0.085             | 0.178  0.011  | 0.239  0.016  | 0.685  0.565  0.715  | 0.092  0.117  0.045 
+3     | 0.000500  | 0.084      | 0.123      | 0.837           | 0.681        | 0.059             | 0.157  0.010  | 0.229  0.017  | 0.718  0.597  0.719  | 0.063  0.074  0.039 
+4     | 0.000478  | 0.076      | 0.120      | 0.843           | 0.693        | 0.056             | 0.142  0.009  | 0.224  0.016  | 0.735  0.606  0.732  | 0.073  0.065  0.032 
+5     | 0.000415  | 0.068      | 0.120      | 0.814           | 0.674        | 0.092             | 0.128  0.008  | 0.223  0.017  | 0.700  0.603  0.751  | 0.132  0.090  0.056 
+6     | 0.000325  | 0.063      | 0.115      | 0.830           | 0.692        | 0.079             | 0.119  0.008  | 0.213  0.016  | 0.726  0.625  0.735  | 0.091  0.102  0.043 
+7     | 0.000225  | 0.059      | 0.119      | 0.835           | 0.686        | 0.066             | 0.111  0.007  | 0.220  0.017  | 0.724  0.611  0.730  | 0.078  0.080  0.041 
+8     | 0.000135  | 0.056      | 0.116      | 0.842           | 0.696        | 0.061             | 0.105  0.007  | 0.216  0.017  | 0.726  0.619  0.751  | 0.083  0.069  0.033 
+9     | 0.000072  | 0.053      | 0.114      | 0.846           | 0.706        | 0.061             | 0.100  0.006  | 0.211  0.017  | 0.736  0.629  0.750  | 0.068  0.071  0.045 
+10    | 0.000050  | 0.052      | 0.116      | 0.842           | 0.703        | 0.065             | 0.098  0.006  | 0.214  0.017  | 0.736  0.623  0.751  | 0.077  0.075  0.042 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.117      | 0.842           | 0.704        | 0.067             | 0.216  0.018  | 0.735  0.624  0.754  | 0.080  0.077  0.044 
+360     | 310     | 0.133      | 0.831           | 0.660        | 0.056             | 0.254  0.012  | 0.704  0.563  0.753  | 0.056  0.085  0.028 
+276     | 276     | 0.089      | 0.868           | 0.740        | 0.046             | 0.160  0.018  | 0.793  0.686  0.704  | 0.060  0.038  0.041 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On 320x320 images with final LR 5e-5
+(used LOAD_RESIZED = False)
+(1h 35min 48s)
+(Max GPU mem usage : 14754.875 MB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.284      | 0.128      | 0.821           | 0.659        | 0.070             | 0.503  0.065  | 0.242  0.013  | 0.700  0.567  0.748  | 0.085  0.082  0.043 
+2     | 0.000500  | 0.094      | 0.120      | 0.834           | 0.681        | 0.065             | 0.177  0.011  | 0.224  0.015  | 0.710  0.598  0.759  | 0.085  0.078  0.031 
+3     | 0.000500  | 0.081      | 0.115      | 0.833           | 0.686        | 0.069             | 0.151  0.010  | 0.215  0.016  | 0.716  0.612  0.752  | 0.084  0.061  0.060 
+4     | 0.000478  | 0.073      | 0.124      | 0.839           | 0.682        | 0.057             | 0.138  0.009  | 0.231  0.018  | 0.721  0.586  0.737  | 0.064  0.052  0.055 
+5     | 0.000415  | 0.067      | 0.119      | 0.818           | 0.667        | 0.082             | 0.125  0.008  | 0.221  0.017  | 0.700  0.597  0.747  | 0.082  0.103  0.059 
+6     | 0.000325  | 0.062      | 0.111      | 0.849           | 0.706        | 0.056             | 0.117  0.007  | 0.206  0.016  | 0.734  0.629  0.761  | 0.062  0.075  0.030 
+7     | 0.000225  | 0.057      | 0.110      | 0.850           | 0.710        | 0.058             | 0.108  0.007  | 0.204  0.016  | 0.738  0.631  0.772  | 0.071  0.070  0.031 
+8     | 0.000135  | 0.055      | 0.110      | 0.849           | 0.710        | 0.058             | 0.103  0.006  | 0.204  0.017  | 0.733  0.635  0.771  | 0.073  0.069  0.032 
+9     | 0.000072  | 0.051      | 0.110      | 0.851           | 0.710        | 0.055             | 0.097  0.006  | 0.203  0.017  | 0.733  0.632  0.770  | 0.066  0.066  0.034 
+10    | 0.000050  | 0.050      | 0.110      | 0.849           | 0.710        | 0.059             | 0.095  0.006  | 0.204  0.017  | 0.733  0.631  0.769  | 0.065  0.076  0.035 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.110      | 0.847           | 0.709        | 0.061             | 0.203  0.018  | 0.728  0.629  0.773  | 0.066  0.080  0.036 
+360     | 310     | 0.116      | 0.855           | 0.712        | 0.049             | 0.222  0.010  | 0.753  0.636  0.779  | 0.063  0.060  0.025 
+276     | 276     | 0.096      | 0.864           | 0.728        | 0.045             | 0.171  0.020  | 0.795  0.661  0.684  | 0.045  0.051  0.039 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On 384x384 images with final LR 5e-5
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32 
+(2h 17min 36s)
+(Max GPU mem usage : 13222.875 MB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.279      | 0.108      | 0.828           | 0.670        | 0.066             | 0.494  0.064  | 0.201  0.015  | 0.707  0.576  0.739  | 0.101  0.067  0.030 
+2     | 0.000500  | 0.094      | 0.102      | 0.806           | 0.630        | 0.076             | 0.177  0.011  | 0.187  0.016  | 0.654  0.588  0.758  | 0.108  0.077  0.042 
+3     | 0.000500  | 0.083      | 0.100      | 0.843           | 0.699        | 0.062             | 0.156  0.010  | 0.184  0.016  | 0.726  0.639  0.737  | 0.084  0.079  0.022 
+4     | 0.000478  | 0.076      | 0.100      | 0.850           | 0.706        | 0.054             | 0.143  0.009  | 0.185  0.016  | 0.739  0.628  0.753  | 0.071  0.057  0.034 
+5     | 0.000415  | 0.069      | 0.099      | 0.841           | 0.697        | 0.064             | 0.130  0.009  | 0.181  0.016  | 0.722  0.631  0.760  | 0.097  0.060  0.035 
+6     | 0.000325  | 0.063      | 0.097      | 0.840           | 0.686        | 0.057             | 0.118  0.008  | 0.177  0.016  | 0.710  0.621  0.754  | 0.076  0.060  0.036 
+7     | 0.000225  | 0.059      | 0.099      | 0.846           | 0.702        | 0.058             | 0.111  0.007  | 0.181  0.017  | 0.735  0.627  0.752  | 0.064  0.074  0.035 
+8     | 0.000135  | 0.056      | 0.093      | 0.854           | 0.720        | 0.056             | 0.105  0.007  | 0.170  0.016  | 0.747  0.652  0.770  | 0.073  0.062  0.035 
+9     | 0.000072  | 0.053      | 0.094      | 0.853           | 0.718        | 0.057             | 0.101  0.006  | 0.171  0.016  | 0.745  0.654  0.767  | 0.073  0.062  0.034 
+10    | 0.000050  | 0.052      | 0.093      | 0.856           | 0.724        | 0.057             | 0.098  0.006  | 0.170  0.016  | 0.749  0.657  0.768  | 0.073  0.060  0.036 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.089      | 0.854           | 0.723        | 0.059             | 0.162  0.017  | 0.745  0.655  0.769  | 0.076  0.062  0.038 
+360     | 310     | 0.076      | 0.863           | 0.720        | 0.041             | 0.144  0.008  | 0.745  0.649  0.804  | 0.052  0.058  0.012 
+276     | 276     | 0.090      | 0.875           | 0.753        | 0.044             | 0.162  0.019  | 0.821  0.690  0.680  | 0.056  0.036  0.039 </t>
   </si>
 </sst>
 </file>
@@ -513,13 +1113,13 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -570,7 +1170,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -580,11 +1180,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -640,34 +1240,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -854,41 +1442,49 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D94" activeCellId="0" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="160.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="13.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.23"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="192.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="13.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="12.23"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
@@ -899,17 +1495,17 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="2" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0.83893</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0.82138</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>0.827</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>0.83893</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>0.82138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -917,109 +1513,109 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="2" t="n">
+        <v>0.812</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0.83844</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0.8158</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>0.812</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>0.83844</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <v>0.8158</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="2" t="n">
+        <v>0.824</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0.837</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0.81291</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>0.824</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>0.837</v>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>0.81291</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="2" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="C10" s="13" t="n">
+        <v>0.84262</v>
+      </c>
+      <c r="D10" s="13" t="n">
+        <v>0.821</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>13</v>
-      </c>
-      <c r="C10" s="3" t="n">
-        <v>0.827</v>
-      </c>
-      <c r="D10" s="13" t="n">
-        <v>0.84262</v>
-      </c>
-      <c r="E10" s="13" t="n">
-        <v>0.821</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="2" t="n">
+        <v>0.824</v>
+      </c>
+      <c r="C12" s="13" t="n">
+        <v>0.83586</v>
+      </c>
+      <c r="D12" s="13" t="n">
+        <v>0.82377</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="C12" s="3" t="n">
-        <v>0.824</v>
-      </c>
-      <c r="D12" s="13" t="n">
-        <v>0.83586</v>
-      </c>
-      <c r="E12" s="13" t="n">
-        <v>0.82377</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="14" t="n">
+        <v>0.831</v>
+      </c>
+      <c r="C14" s="13" t="n">
+        <v>0.83762</v>
+      </c>
+      <c r="D14" s="13" t="n">
+        <v>0.81809</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="C14" s="14" t="n">
-        <v>0.831</v>
-      </c>
-      <c r="D14" s="13" t="n">
-        <v>0.83762</v>
-      </c>
-      <c r="E14" s="13" t="n">
-        <v>0.81809</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="14" t="n">
+        <v>0.823</v>
+      </c>
+      <c r="C16" s="13" t="n">
+        <v>0.841</v>
+      </c>
+      <c r="D16" s="13" t="n">
+        <v>0.81975</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="C16" s="14" t="n">
-        <v>0.823</v>
-      </c>
-      <c r="D16" s="13" t="n">
-        <v>0.841</v>
-      </c>
-      <c r="E16" s="13" t="n">
-        <v>0.81975</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1027,18 +1623,18 @@
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="2" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="C20" s="3" t="n">
-        <v>0.83</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1046,7 +1642,7 @@
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1054,7 +1650,7 @@
       <c r="A26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1062,7 +1658,7 @@
       <c r="A28" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="E28" s="11" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1070,18 +1666,18 @@
       <c r="A30" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="E30" s="11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2"/>
+      <c r="A31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="E32" s="11" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1089,7 +1685,7 @@
       <c r="A34" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="E34" s="11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1097,7 +1693,7 @@
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="E36" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1105,7 +1701,7 @@
       <c r="A38" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="E38" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1113,91 +1709,437 @@
       <c r="A40" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="2" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="C40" s="13" t="n">
+        <v>0.84358</v>
+      </c>
+      <c r="D40" s="16" t="n">
+        <v>0.82371</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="C40" s="3" t="n">
-        <v>0.833</v>
-      </c>
-      <c r="D40" s="13" t="n">
-        <v>0.84358</v>
-      </c>
-      <c r="E40" s="16" t="n">
-        <v>0.82371</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="2" t="n">
+        <v>0.862</v>
+      </c>
+      <c r="C42" s="13" t="n">
+        <v>0.84226</v>
+      </c>
+      <c r="D42" s="13" t="n">
+        <v>0.82784</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="3" t="n">
-        <v>0.862</v>
-      </c>
-      <c r="D42" s="13" t="n">
-        <v>0.84226</v>
-      </c>
-      <c r="E42" s="13" t="n">
-        <v>0.82784</v>
-      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="9"/>
-    </row>
-    <row r="44" s="22" customFormat="true" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="17" t="s">
+      <c r="E43" s="9"/>
+    </row>
+    <row r="44" s="3" customFormat="true" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="2" t="n">
+        <v>0.843</v>
+      </c>
+      <c r="C44" s="17" t="n">
+        <v>0.84494</v>
+      </c>
+      <c r="D44" s="13" t="n">
+        <v>0.83243</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="19" t="n">
-        <v>0.843</v>
-      </c>
-      <c r="D44" s="20" t="n">
-        <v>0.84494</v>
-      </c>
-      <c r="E44" s="21" t="n">
-        <v>0.83243</v>
-      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="9"/>
+      <c r="E45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="23" t="s">
+      <c r="B46" s="2" t="n">
+        <v>0.834</v>
+      </c>
+      <c r="C46" s="13" t="n">
+        <v>0.84219</v>
+      </c>
+      <c r="D46" s="13" t="n">
+        <v>0.83364</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="C46" s="3" t="n">
-        <v>0.834</v>
-      </c>
-      <c r="D46" s="24" t="n">
-        <v>0.84219</v>
-      </c>
-      <c r="E46" s="24" t="n">
-        <v>0.83364</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="23" t="s">
+      <c r="B48" s="2" t="n">
+        <v>0.837</v>
+      </c>
+      <c r="C48" s="13" t="n">
+        <v>0.84214</v>
+      </c>
+      <c r="D48" s="13" t="n">
+        <v>0.83249</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="3" t="n">
+    </row>
+    <row r="50" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>0.836</v>
+      </c>
+      <c r="C50" s="13" t="n">
+        <v>0.84298</v>
+      </c>
+      <c r="D50" s="13" t="n">
+        <v>0.83234</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="2" t="n">
         <v>0.837</v>
       </c>
-      <c r="D48" s="24" t="n">
-        <v>0.84214</v>
-      </c>
-      <c r="E48" s="24" t="n">
-        <v>0.83249</v>
+      <c r="C52" s="13" t="n">
+        <v>0.84494</v>
+      </c>
+      <c r="D52" s="13" t="n">
+        <v>0.83193</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>0.839</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>0.828</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="2" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="2" t="n">
+        <v>0.822</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="2" t="n">
+        <v>0.684</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="2" t="n">
+        <v>0.842</v>
+      </c>
+      <c r="C64" s="13" t="n">
+        <v>0.83724</v>
+      </c>
+      <c r="D64" s="13" t="n">
+        <v>0.82728</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="382.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="2" t="n">
+        <v>0.847</v>
+      </c>
+      <c r="C66" s="13" t="n">
+        <v>0.83782</v>
+      </c>
+      <c r="D66" s="13" t="n">
+        <v>0.8276</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="2" t="n">
+        <v>0.834</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="2" t="n">
+        <v>0.836</v>
+      </c>
+      <c r="C70" s="13" t="n">
+        <v>0.84333</v>
+      </c>
+      <c r="D70" s="13" t="n">
+        <v>0.83245</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="14" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" s="14" t="n">
+        <v>0.841</v>
+      </c>
+      <c r="C74" s="13" t="n">
+        <v>0.84477</v>
+      </c>
+      <c r="D74" s="13" t="n">
+        <v>0.83245</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" s="2" t="n">
+        <v>0.838</v>
+      </c>
+      <c r="C76" s="13" t="n">
+        <v>0.84349</v>
+      </c>
+      <c r="D76" s="13" t="n">
+        <v>0.8311</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" s="2" t="n">
+        <v>0.829</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" s="2" t="n">
+        <v>0.842</v>
+      </c>
+      <c r="C80" s="2" t="n">
+        <v>0.84717</v>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>0.83537</v>
+      </c>
+      <c r="E80" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" s="2" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="C82" s="2" t="n">
+        <v>0.8494</v>
+      </c>
+      <c r="D82" s="2" t="n">
+        <v>0.8408</v>
+      </c>
+      <c r="E82" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B84" s="2" t="n">
+        <v>0.841</v>
+      </c>
+      <c r="C84" s="20" t="n">
+        <v>0.84386</v>
+      </c>
+      <c r="D84" s="20" t="n">
+        <v>0.82848</v>
+      </c>
+      <c r="E84" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86" s="2" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="C86" s="2" t="n">
+        <v>0.84361</v>
+      </c>
+      <c r="D86" s="2" t="n">
+        <v>0.83301</v>
+      </c>
+      <c r="E86" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" s="2" t="n">
+        <v>0.848</v>
+      </c>
+      <c r="C88" s="2" t="n">
+        <v>0.84611</v>
+      </c>
+      <c r="D88" s="2" t="n">
+        <v>0.83529</v>
+      </c>
+      <c r="E88" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B90" s="2" t="n">
+        <v>0.842</v>
+      </c>
+      <c r="C90" s="21" t="n">
+        <v>0.84998</v>
+      </c>
+      <c r="D90" s="2" t="n">
+        <v>0.84112</v>
+      </c>
+      <c r="E90" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B92" s="2" t="n">
+        <v>0.849</v>
+      </c>
+      <c r="C92" s="2" t="n">
+        <v>0.84915</v>
+      </c>
+      <c r="D92" s="2" t="n">
+        <v>0.84107</v>
+      </c>
+      <c r="E92" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B94" s="2" t="n">
+        <v>0.856</v>
+      </c>
+      <c r="C94" s="2" t="n">
+        <v>0.85739</v>
+      </c>
+      <c r="D94" s="2" t="n">
+        <v>0.84292</v>
+      </c>
+      <c r="E94" s="18" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried UNeteffnetv2, UNetconvnext, segformer-mitb1
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -787,53 +787,11 @@
 276     | 276     | 0.105      | 0.842           | 0.691        | 0.058             | 0.188  0.022  | 0.763  0.633  0.610  | 0.058  0.060  0.055 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Trained on 256x256 images with settings from
-'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Without 3 problem casedays</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">’ run
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(used LOAD_RESIZED = True)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(1h 7min 12s)
+    <t xml:space="preserve">Trained on 256x256 images with settings from
+'Without 3 problem casedays’ run
+(used LOAD_RESIZED = True)
+(1h 7min 12s)
 (Max GPU mem usage : 15060.875 MB)</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
@@ -881,45 +839,11 @@
 276     | 276     | 0.089      | 0.862           | 0.745        | 0.060             | 0.159  0.019  | 0.824  0.679  0.650  | 0.060  0.068  0.051 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">On 224x224 images with final LR 5e-5
+    <t xml:space="preserve">On 224x224 images with final LR 5e-5
 BS = 64
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(used LOAD_RESIZED = False)
+(used LOAD_RESIZED = False)
 (52min 54s)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Max GPU mem usage : 9768.875 MB)</t>
-    </r>
+(Max GPU mem usage : 9768.875 MB)</t>
   </si>
   <si>
     <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
@@ -1068,6 +992,128 @@
 360     | 310     | 0.076      | 0.863           | 0.720        | 0.041             | 0.144  0.008  | 0.745  0.649  0.804  | 0.052  0.058  0.012 
 276     | 276     | 0.090      | 0.875           | 0.753        | 0.044             | 0.162  0.019  | 0.821  0.690  0.680  | 0.056  0.036  0.039 </t>
   </si>
+  <si>
+    <t xml:space="preserve">Encoder : tu-convnextv2_tiny
+On 384x384 images with final LR 5e-5
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32 
+(6h 43min 52s)
+(Max GPU mem usage : 15284.875 MB)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.345      | 0.140      | 0.792           | 0.573        | 0.062             | 0.604  0.087  | 0.263  0.017  | 0.599  0.488  0.646  | 0.058  0.078  0.051 
+2     | 0.000500  | 0.115      | 0.110      | 0.814           | 0.632        | 0.065             | 0.216  0.013  | 0.204  0.015  | 0.670  0.556  0.700  | 0.082  0.062  0.050 
+3     | 0.000500  | 0.092      | 0.115      | 0.827           | 0.652        | 0.056             | 0.173  0.011  | 0.214  0.016  | 0.688  0.563  0.698  | 0.052  0.054  0.064 
+4     | 0.000478  | 0.083      | 0.109      | 0.832           | 0.659        | 0.052             | 0.156  0.010  | 0.202  0.016  | 0.687  0.578  0.728  | 0.055  0.066  0.037 
+5     | 0.000415  | 0.073      | 0.098      | 0.843           | 0.686        | 0.052             | 0.137  0.009  | 0.182  0.014  | 0.716  0.614  0.732  | 0.056  0.056  0.042 
+6     | 0.000325  | 0.066      | 0.100      | 0.805           | 0.640        | 0.085             | 0.124  0.008  | 0.184  0.015  | 0.688  0.585  0.675  | 0.113  0.068  0.074 
+7     | 0.000225  | 0.060      | 0.098      | 0.849           | 0.698        | 0.050             | 0.114  0.007  | 0.182  0.015  | 0.723  0.619  0.770  | 0.058  0.057  0.036 
+8     | 0.000135  | 0.056      | 0.098      | 0.840           | 0.694        | 0.063             | 0.105  0.006  | 0.182  0.015  | 0.726  0.623  0.742  | 0.068  0.061  0.060 
+9     | 0.000072  | 0.053      | 0.094      | 0.848           | 0.702        | 0.054             | 0.100  0.006  | 0.174  0.015  | 0.729  0.626  0.771  | 0.063  0.065  0.033 
+10    | 0.000050  | 0.051      | 0.096      | 0.824           | 0.674        | 0.077             | 0.096  0.006  | 0.176  0.016  | 0.704  0.602  0.772  | 0.103  0.088  0.039 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.094      | 0.820           | 0.672        | 0.080             | 0.172  0.016  | 0.699  0.602  0.777  | 0.109  0.091  0.042 
+360     | 310     | 0.085      | 0.829           | 0.663        | 0.061             | 0.161  0.009  | 0.686  0.556  0.792  | 0.076  0.088  0.019 
+276     | 276     | 0.095      | 0.871           | 0.736        | 0.039             | 0.172  0.017  | 0.811  0.674  0.659  | 0.052  0.036  0.031 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder : tu-tf_efficientnetv2_s
+On 384x384 images with final LR 5e-5
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32 
+(2h 37m 54s)
+(Max GPU mem usage : 14240.875 MB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.262      | 0.113      | 0.827           | 0.655        | 0.059             | 0.474  0.051  | 0.211  0.014  | 0.690  0.559  0.729  | 0.069  0.068  0.041 
+2     | 0.000500  | 0.097      | 0.106      | 0.836           | 0.677        | 0.058             | 0.183  0.011  | 0.196  0.015  | 0.717  0.604  0.733  | 0.060  0.066  0.048 
+3     | 0.000500  | 0.086      | 0.103      | 0.821           | 0.674        | 0.082             | 0.162  0.010  | 0.191  0.015  | 0.721  0.590  0.741  | 0.096  0.100  0.050 
+4     | 0.000478  | 0.079      | 0.098      | 0.847           | 0.697        | 0.053             | 0.148  0.010  | 0.182  0.015  | 0.721  0.608  0.781  | 0.055  0.074  0.030 
+5     | 0.000415  | 0.071      | 0.101      | 0.840           | 0.689        | 0.059             | 0.134  0.009  | 0.185  0.016  | 0.717  0.594  0.778  | 0.071  0.076  0.031 
+6     | 0.000325  | 0.065      | 0.098      | 0.850           | 0.710        | 0.056             | 0.123  0.008  | 0.180  0.015  | 0.741  0.622  0.785  | 0.057  0.074  0.037 
+7     | 0.000225  | 0.059      | 0.096      | 0.856           | 0.722        | 0.054             | 0.111  0.007  | 0.177  0.015  | 0.748  0.642  0.794  | 0.062  0.073  0.028 
+8     | 0.000135  | 0.055      | 0.095      | 0.861           | 0.728        | 0.051             | 0.104  0.006  | 0.175  0.015  | 0.753  0.648  0.789  | 0.056  0.061  0.035 
+9     | 0.000072  | 0.053      | 0.093      | 0.860           | 0.724        | 0.049             | 0.100  0.006  | 0.172  0.015  | 0.748  0.645  0.790  | 0.053  0.064  0.031 
+10    | 0.000050  | 0.051      | 0.098      | 0.859           | 0.723        | 0.051             | 0.097  0.006  | 0.181  0.015  | 0.748  0.639  0.792  | 0.052  0.061  0.041 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.092      | 0.859           | 0.726        | 0.053             | 0.169  0.016  | 0.747  0.642  0.798  | 0.053  0.064  0.042 
+360     | 310     | 0.083      | 0.848           | 0.684        | 0.042             | 0.157  0.009  | 0.720  0.584  0.791  | 0.041  0.049  0.037 
+276     | 276     | 0.096      | 0.868           | 0.732        | 0.042             | 0.173  0.019  | 0.806  0.660  0.684  | 0.040  0.045  0.040 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder : tu-tf_efficientnetv2_s
+On 384x384 images with final LR 1e-5
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32 
+(2h 38m 22s)
+(Max GPU mem usage : 14240.875 MB)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.268      | 0.112      | 0.823           | 0.651        | 0.062             | 0.485  0.051  | 0.210  0.015  | 0.697  0.566  0.702  | 0.071  0.085  0.030 
+2     | 0.000500  | 0.095      | 0.105      | 0.843           | 0.682        | 0.049             | 0.179  0.011  | 0.195  0.015  | 0.693  0.611  0.764  | 0.048  0.071  0.028 
+3     | 0.000500  | 0.084      | 0.104      | 0.834           | 0.680        | 0.063             | 0.158  0.010  | 0.192  0.016  | 0.716  0.593  0.753  | 0.060  0.080  0.049 
+4     | 0.000480  | 0.077      | 0.102      | 0.843           | 0.699        | 0.061             | 0.144  0.009  | 0.188  0.015  | 0.725  0.617  0.771  | 0.063  0.082  0.037 
+5     | 0.000425  | 0.071      | 0.097      | 0.848           | 0.705        | 0.057             | 0.134  0.009  | 0.179  0.015  | 0.737  0.624  0.770  | 0.061  0.079  0.031 
+6     | 0.000345  | 0.066      | 0.095      | 0.848           | 0.706        | 0.057             | 0.124  0.008  | 0.176  0.015  | 0.731  0.628  0.786  | 0.073  0.071  0.025 
+7     | 0.000255  | 0.061      | 0.095      | 0.849           | 0.714        | 0.060             | 0.115  0.007  | 0.176  0.014  | 0.732  0.641  0.790  | 0.064  0.080  0.037 
+8     | 0.000175  | 0.057      | 0.093      | 0.852           | 0.717        | 0.057             | 0.107  0.007  | 0.170  0.015  | 0.741  0.639  0.791  | 0.063  0.071  0.038 
+9     | 0.000120  | 0.054      | 0.093      | 0.859           | 0.731        | 0.055             | 0.102  0.006  | 0.170  0.015  | 0.752  0.656  0.796  | 0.059  0.069  0.038 
+10    | 0.000100  | 0.052      | 0.092      | 0.856           | 0.726        | 0.057             | 0.097  0.006  | 0.169  0.015  | 0.746  0.650  0.800  | 0.065  0.071  0.033 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.087      | 0.856           | 0.727        | 0.057             | 0.158  0.015  | 0.745  0.651  0.805  | 0.067  0.072  0.033 
+360     | 310     | 0.079      | 0.847           | 0.699        | 0.055             | 0.149  0.008  | 0.713  0.616  0.816  | 0.074  0.062  0.029 
+276     | 276     | 0.091      | 0.869           | 0.747        | 0.049             | 0.165  0.017  | 0.818  0.682  0.685  | 0.034  0.080  0.033 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     Epoch 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     Epoch 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with final LR 1e-5
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32  
+(2h 28m 52s)
+(Max GPU mem usage : 14122.875 MB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.315      | 0.131      | 0.797           | 0.603        | 0.073             | 0.567  0.063  | 0.246  0.017  | 0.643  0.536  0.669  | 0.090  0.061  0.070 
+2     | 0.000500  | 0.111      | 0.134      | 0.688           | 0.453        | 0.155             | 0.212  0.011  | 0.245  0.024  | 0.485  0.413  0.602  | 0.193  0.172  0.099 
+3     | 0.000500  | 0.097      | 0.105      | 0.836           | 0.680        | 0.059             | 0.184  0.010  | 0.194  0.016  | 0.712  0.619  0.714  | 0.077  0.058  0.043 
+4     | 0.000480  | 0.088      | 0.105      | 0.816           | 0.653        | 0.076             | 0.167  0.010  | 0.192  0.018  | 0.682  0.600  0.722  | 0.119  0.064  0.046 
+5     | 0.000425  | 0.080      | 0.105      | 0.835           | 0.667        | 0.053             | 0.151  0.009  | 0.195  0.015  | 0.710  0.582  0.731  | 0.054  0.067  0.038 
+6     | 0.000345  | 0.075      | 0.100      | 0.837           | 0.683        | 0.060             | 0.141  0.008  | 0.183  0.016  | 0.707  0.612  0.760  | 0.075  0.072  0.033 
+7     | 0.000255  | 0.069      | 0.095      | 0.855           | 0.714        | 0.050             | 0.130  0.008  | 0.176  0.015  | 0.741  0.639  0.757  | 0.056  0.061  0.034 
+8     | 0.000175  | 0.063      | 0.097      | 0.853           | 0.710        | 0.051             | 0.119  0.007  | 0.180  0.015  | 0.736  0.630  0.766  | 0.062  0.054  0.038 
+9     | 0.000120  | 0.061      | 0.095      | 0.851           | 0.711        | 0.056             | 0.115  0.007  | 0.175  0.015  | 0.733  0.641  0.774  | 0.061  0.070  0.038 
+10    | 0.000100  | 0.059      | 0.096      | 0.853           | 0.710        | 0.051             | 0.111  0.006  | 0.176  0.016  | 0.733  0.638  0.768  | 0.063  0.058  0.033 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.090      | 0.851           | 0.707        | 0.053             | 0.164  0.016  | 0.724  0.637  0.768  | 0.066  0.059  0.034 
+360     | 310     | 0.079      | 0.863           | 0.721        | 0.043             | 0.149  0.008  | 0.769  0.617  0.811  | 0.049  0.059  0.020 
+276     | 276     | 0.091      | 0.879           | 0.757        | 0.040             | 0.165  0.017  | 0.828  0.681  0.693  | 0.036  0.047  0.036 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     Epoch 7</t>
+  </si>
 </sst>
 </file>
 
@@ -1076,12 +1122,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1100,18 +1145,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1170,7 +1203,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1237,22 +1270,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1442,10 +1459,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K94"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D94" activeCellId="0" sqref="D94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A90" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1749,7 +1766,7 @@
       <c r="B44" s="2" t="n">
         <v>0.843</v>
       </c>
-      <c r="C44" s="17" t="n">
+      <c r="C44" s="13" t="n">
         <v>0.84494</v>
       </c>
       <c r="D44" s="13" t="n">
@@ -2019,12 +2036,12 @@
       <c r="D80" s="2" t="n">
         <v>0.83537</v>
       </c>
-      <c r="E80" s="18" t="s">
+      <c r="E80" s="11" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="19" t="s">
+      <c r="A82" s="8" t="s">
         <v>84</v>
       </c>
       <c r="B82" s="2" t="n">
@@ -2036,7 +2053,7 @@
       <c r="D82" s="2" t="n">
         <v>0.8408</v>
       </c>
-      <c r="E82" s="18" t="s">
+      <c r="E82" s="11" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2047,18 +2064,18 @@
       <c r="B84" s="2" t="n">
         <v>0.841</v>
       </c>
-      <c r="C84" s="20" t="n">
+      <c r="C84" s="13" t="n">
         <v>0.84386</v>
       </c>
-      <c r="D84" s="20" t="n">
+      <c r="D84" s="13" t="n">
         <v>0.82848</v>
       </c>
-      <c r="E84" s="18" t="s">
+      <c r="E84" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="19" t="s">
+      <c r="A86" s="8" t="s">
         <v>88</v>
       </c>
       <c r="B86" s="2" t="n">
@@ -2070,12 +2087,12 @@
       <c r="D86" s="2" t="n">
         <v>0.83301</v>
       </c>
-      <c r="E86" s="18" t="s">
+      <c r="E86" s="11" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="19" t="s">
+      <c r="A88" s="8" t="s">
         <v>90</v>
       </c>
       <c r="B88" s="2" t="n">
@@ -2087,29 +2104,29 @@
       <c r="D88" s="2" t="n">
         <v>0.83529</v>
       </c>
-      <c r="E88" s="18" t="s">
+      <c r="E88" s="11" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="19" t="s">
+      <c r="A90" s="8" t="s">
         <v>92</v>
       </c>
       <c r="B90" s="2" t="n">
         <v>0.842</v>
       </c>
-      <c r="C90" s="21" t="n">
+      <c r="C90" s="2" t="n">
         <v>0.84998</v>
       </c>
       <c r="D90" s="2" t="n">
         <v>0.84112</v>
       </c>
-      <c r="E90" s="18" t="s">
+      <c r="E90" s="11" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="19" t="s">
+      <c r="A92" s="8" t="s">
         <v>94</v>
       </c>
       <c r="B92" s="2" t="n">
@@ -2121,25 +2138,129 @@
       <c r="D92" s="2" t="n">
         <v>0.84107</v>
       </c>
-      <c r="E92" s="18" t="s">
+      <c r="E92" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="19" t="s">
+      <c r="A94" s="8" t="s">
         <v>96</v>
       </c>
       <c r="B94" s="2" t="n">
         <v>0.856</v>
       </c>
-      <c r="C94" s="2" t="n">
+      <c r="C94" s="17" t="n">
         <v>0.85739</v>
       </c>
       <c r="D94" s="2" t="n">
         <v>0.84292</v>
       </c>
-      <c r="E94" s="18" t="s">
+      <c r="E94" s="11" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B96" s="2" t="n">
+        <v>0.824</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" s="2" t="n">
+        <v>0.859</v>
+      </c>
+      <c r="C98" s="2" t="n">
+        <v>0.85267</v>
+      </c>
+      <c r="D98" s="2" t="n">
+        <v>0.83613</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" s="2" t="n">
+        <v>0.856</v>
+      </c>
+      <c r="C100" s="13" t="n">
+        <v>0.85477</v>
+      </c>
+      <c r="D100" s="13" t="n">
+        <v>0.84072</v>
+      </c>
+      <c r="E100" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101" s="2" t="n">
+        <v>0.859</v>
+      </c>
+      <c r="C101" s="13" t="n">
+        <v>0.85394</v>
+      </c>
+      <c r="D101" s="13" t="n">
+        <v>0.84257</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B102" s="2" t="n">
+        <v>0.852</v>
+      </c>
+      <c r="C102" s="13" t="n">
+        <v>0.85532</v>
+      </c>
+      <c r="D102" s="13" t="n">
+        <v>0.84371</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" s="2" t="n">
+        <v>0.853</v>
+      </c>
+      <c r="C104" s="14" t="n">
+        <v>0.85341</v>
+      </c>
+      <c r="D104" s="14" t="n">
+        <v>0.8418</v>
+      </c>
+      <c r="E104" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B105" s="2" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="C105" s="14" t="n">
+        <v>0.8469</v>
+      </c>
+      <c r="D105" s="14" t="n">
+        <v>0.83303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
segformer mit-b1 with better LR and evaluation
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -1049,7 +1049,7 @@
   </si>
   <si>
     <t xml:space="preserve">Encoder : tu-tf_efficientnetv2_s
-On 384x384 images with final LR 1e-5
+On 384x384 images with final LR 1e-4
 (used LOAD_RESIZED = False)
 with grad_accu = 2, BS = 32 
 (2h 38m 22s)
@@ -1085,7 +1085,7 @@
     <t xml:space="preserve">Segformer with mit_b1 encoder
 With AdamW optim 
 0.01 weight_decay for params except bias&amp;norm
-On 384x384 images with final LR 1e-5
+On 384x384 images with final LR 1e-4
 (used LOAD_RESIZED = False)
 with grad_accu = 2, BS = 32  
 (2h 28m 52s)
@@ -1114,6 +1114,39 @@
   <si>
     <t xml:space="preserve">                                     Epoch 7</t>
   </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with LR 3e-4 to 3e-5
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32  
+(2h 32m 54s)
+(Max GPU mem usage : 14122.875 MB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.306      | 0.116      | 0.821           | 0.641        | 0.058             | 0.543  0.068  | 0.220  0.012  | 0.679  0.554  0.723  | 0.076  0.061  0.038 
+2     | 0.000300  | 0.108      | 0.106      | 0.810           | 0.637        | 0.074             | 0.205  0.010  | 0.198  0.014  | 0.669  0.573  0.740  | 0.091  0.076  0.056 
+3     | 0.000300  | 0.093      | 0.106      | 0.841           | 0.687        | 0.056             | 0.177  0.009  | 0.195  0.017  | 0.724  0.591  0.744  | 0.068  0.050  0.052 
+4     | 0.000287  | 0.084      | 0.100      | 0.841           | 0.696        | 0.062             | 0.159  0.009  | 0.184  0.015  | 0.725  0.616  0.756  | 0.078  0.064  0.044 
+5     | 0.000249  | 0.077      | 0.100      | 0.846           | 0.700        | 0.057             | 0.147  0.008  | 0.185  0.015  | 0.727  0.621  0.765  | 0.061  0.071  0.039 
+6     | 0.000195  | 0.071      | 0.096      | 0.857           | 0.711        | 0.046             | 0.135  0.007  | 0.178  0.014  | 0.738  0.633  0.768  | 0.057  0.055  0.027 
+7     | 0.000135  | 0.066      | 0.099      | 0.854           | 0.711        | 0.050             | 0.125  0.007  | 0.183  0.015  | 0.734  0.632  0.774  | 0.054  0.058  0.038 
+8     | 0.000081  | 0.062      | 0.096      | 0.846           | 0.700        | 0.057             | 0.118  0.006  | 0.176  0.015  | 0.725  0.629  0.773  | 0.068  0.064  0.040 
+9     | 0.000043  | 0.059      | 0.094      | 0.851           | 0.713        | 0.056             | 0.113  0.006  | 0.172  0.016  | 0.735  0.646  0.778  | 0.066  0.062  0.041 
+10    | 0.000030  | 0.057      | 0.094      | 0.861           | 0.723        | 0.047             | 0.109  0.006  | 0.172  0.015  | 0.742  0.652  0.785  | 0.054  0.058  0.030 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+266     | 266     | 0.093      | 0.860           | 0.721        | 0.048             | 0.170  0.016  | 0.735  0.654  0.789  | 0.055  0.058  0.031 
+360     | 310     | 0.079      | 0.855           | 0.708        | 0.047             | 0.149  0.008  | 0.763  0.596  0.789  | 0.055  0.057  0.028 
+276     | 276     | 0.087      | 0.880           | 0.767        | 0.046             | 0.158  0.015  | 0.840  0.690  0.711  | 0.042  0.065  0.031 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                     Epoch 6</t>
+  </si>
 </sst>
 </file>
 
@@ -1127,6 +1160,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1148,11 +1182,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1459,10 +1495,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K105"/>
+  <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A90" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A102" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D107" activeCellId="0" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2263,6 +2299,37 @@
         <v>0.83303</v>
       </c>
     </row>
+    <row r="107" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107" s="2" t="n">
+        <v>0.861</v>
+      </c>
+      <c r="C107" s="14" t="n">
+        <v>0.85232</v>
+      </c>
+      <c r="D107" s="14" t="n">
+        <v>0.84214</v>
+      </c>
+      <c r="E107" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B108" s="2" t="n">
+        <v>0.857</v>
+      </c>
+      <c r="C108" s="14" t="n">
+        <v>0.84383</v>
+      </c>
+      <c r="D108" s="14" t="n">
+        <v>0.83613</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
pad before resize, improved DLB loss
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="124">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -1147,6 +1147,199 @@
   <si>
     <t xml:space="preserve">                                     Epoch 6</t>
   </si>
+  <si>
+    <t xml:space="preserve">Unet with effnet-b1
+On padded images with final LR 5e-5
+With Adam
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32 
+(2h 20m 21s)
+(Max GPU mem usage : 13222.875 MB)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.277      | 0.111      | 0.798           | 0.626        | 0.088             | 0.490  0.064  | 0.207  0.016  | 0.670  0.566  0.716  | 0.142  0.079  0.044 
+2     | 0.000500  | 0.093      | 0.105      | 0.811           | 0.641        | 0.077             | 0.176  0.011  | 0.193  0.016  | 0.672  0.592  0.743  | 0.115  0.085  0.029 
+3     | 0.000500  | 0.083      | 0.101      | 0.831           | 0.677        | 0.066             | 0.155  0.010  | 0.187  0.015  | 0.712  0.605  0.752  | 0.088  0.075  0.036 
+4     | 0.000478  | 0.075      | 0.101      | 0.849           | 0.703        | 0.053             | 0.142  0.009  | 0.187  0.016  | 0.721  0.627  0.769  | 0.060  0.051  0.050 
+5     | 0.000415  | 0.068      | 0.098      | 0.829           | 0.692        | 0.079             | 0.128  0.008  | 0.180  0.016  | 0.715  0.637  0.769  | 0.140  0.071  0.027 
+6     | 0.000325  | 0.064      | 0.096      | 0.844           | 0.706        | 0.063             | 0.120  0.008  | 0.176  0.016  | 0.739  0.639  0.748  | 0.094  0.071  0.025 
+7     | 0.000225  | 0.059      | 0.100      | 0.846           | 0.707        | 0.061             | 0.111  0.007  | 0.183  0.017  | 0.745  0.624  0.760  | 0.063  0.088  0.033 
+8     | 0.000135  | 0.055      | 0.100      | 0.852           | 0.707        | 0.051             | 0.104  0.006  | 0.183  0.017  | 0.746  0.631  0.753  | 0.063  0.056  0.033 
+9     | 0.000072  | 0.054      | 0.097      | 0.857           | 0.718        | 0.050             | 0.101  0.006  | 0.178  0.016  | 0.748  0.644  0.765  | 0.057  0.060  0.034 
+10    | 0.000050  | 0.052      | 0.096      | 0.856           | 0.721        | 0.053             | 0.098  0.006  | 0.176  0.017  | 0.751  0.648  0.769  | 0.065  0.063  0.031 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.096      | 0.856           | 0.721        | 0.053             | 0.176  0.017  | 0.751  0.648  0.769  | 0.065  0.063  0.031 
+266     | 266     | 0.091      | 0.856           | 0.721        | 0.054             | 0.165  0.017  | 0.747  0.648  0.774  | 0.065  0.065  0.031 
+360     | 310     | 0.074      | 0.851           | 0.704        | 0.051             | 0.141  0.007  | 0.745  0.622  0.791  | 0.082  0.053  0.019 
+276     | 276     | 0.092      | 0.868           | 0.740        | 0.047             | 0.165  0.019  | 0.821  0.678  0.653  | 0.042  0.049  0.049 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder
+On padded images
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with LR 3e-4 to 3e-5
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32   
+(2h 33m 26s)
+(Max GPU mem usage : 14122.875 MB)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.302      | 0.122      | 0.816           | 0.628        | 0.058             | 0.538  0.065  | 0.232  0.012  | 0.664  0.555  0.680  | 0.062  0.060  0.053 
+2     | 0.000300  | 0.108      | 0.112      | 0.795           | 0.607        | 0.080             | 0.206  0.010  | 0.206  0.017  | 0.635  0.545  0.732  | 0.105  0.091  0.043 
+3     | 0.000300  | 0.094      | 0.106      | 0.834           | 0.674        | 0.059             | 0.179  0.009  | 0.197  0.015  | 0.721  0.590  0.711  | 0.075  0.050  0.052 
+4     | 0.000287  | 0.085      | 0.099      | 0.846           | 0.702        | 0.059             | 0.161  0.009  | 0.183  0.014  | 0.734  0.616  0.762  | 0.061  0.079  0.036 
+5     | 0.000249  | 0.079      | 0.104      | 0.840           | 0.678        | 0.052             | 0.151  0.008  | 0.192  0.016  | 0.705  0.590  0.769  | 0.056  0.067  0.034 
+6     | 0.000195  | 0.072      | 0.097      | 0.849           | 0.700        | 0.051             | 0.138  0.007  | 0.179  0.015  | 0.725  0.620  0.774  | 0.062  0.056  0.036 
+7     | 0.000135  | 0.067      | 0.096      | 0.847           | 0.706        | 0.059             | 0.127  0.007  | 0.176  0.015  | 0.735  0.626  0.764  | 0.068  0.065  0.043 
+8     | 0.000081  | 0.063      | 0.094      | 0.858           | 0.718        | 0.049             | 0.120  0.006  | 0.173  0.015  | 0.745  0.638  0.778  | 0.056  0.058  0.032 
+9     | 0.000043  | 0.060      | 0.095      | 0.856           | 0.715        | 0.051             | 0.115  0.006  | 0.174  0.015  | 0.743  0.632  0.782  | 0.057  0.056  0.039 
+10    | 0.000030  | 0.059      | 0.094      | 0.862           | 0.726        | 0.047             | 0.112  0.006  | 0.173  0.015  | 0.750  0.646  0.784  | 0.055  0.054  0.032 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.094      | 0.862           | 0.726        | 0.047             | 0.173  0.015  | 0.750  0.646  0.784  | 0.055  0.054  0.032 
+266     | 266     | 0.095      | 0.861           | 0.725        | 0.048             | 0.173  0.016  | 0.744  0.647  0.789  | 0.056  0.055  0.033 
+360     | 310     | 0.078      | 0.860           | 0.713        | 0.043             | 0.150  0.007  | 0.767  0.605  0.783  | 0.043  0.060  0.024 
+276     | 276     | 0.090      | 0.881           | 0.759        | 0.037             | 0.163  0.016  | 0.826  0.682  0.710  | 0.048  0.038  0.026 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder
+Loss : 0.75*dice+0.25*BCE
+On padded images
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with LR 3e-4 to 3e-5
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+(2h 32m 20s)  
+(Max GPU mem usage : 14122.875 MB) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.362      | 0.165      | 0.815           | 0.640        | 0.068             | 0.463  0.062  | 0.215  0.015  | 0.675  0.571  0.711  | 0.098  0.066  0.038 
+2     | 0.000300  | 0.155      | 0.154      | 0.801           | 0.631        | 0.086             | 0.203  0.011  | 0.200  0.017  | 0.663  0.553  0.742  | 0.093  0.101  0.063 
+3     | 0.000300  | 0.133      | 0.144      | 0.837           | 0.688        | 0.063             | 0.174  0.011  | 0.187  0.017  | 0.719  0.608  0.749  | 0.081  0.065  0.045 
+4     | 0.000287  | 0.122      | 0.138      | 0.851           | 0.705        | 0.051             | 0.159  0.010  | 0.179  0.018  | 0.736  0.625  0.764  | 0.070  0.058  0.025 
+5     | 0.000249  | 0.112      | 0.138      | 0.840           | 0.698        | 0.064             | 0.146  0.010  | 0.178  0.018  | 0.725  0.628  0.766  | 0.081  0.071  0.041 
+6     | 0.000195  | 0.103      | 0.140      | 0.853           | 0.709        | 0.051             | 0.134  0.009  | 0.180  0.019  | 0.734  0.629  0.771  | 0.059  0.065  0.030 
+7     | 0.000135  | 0.096      | 0.137      | 0.854           | 0.711        | 0.052             | 0.125  0.008  | 0.176  0.019  | 0.737  0.632  0.776  | 0.058  0.061  0.036 
+8     | 0.000081  | 0.090      | 0.138      | 0.853           | 0.711        | 0.053             | 0.117  0.008  | 0.178  0.019  | 0.735  0.632  0.780  | 0.062  0.060  0.036 
+9     | 0.000043  | 0.087      | 0.137      | 0.852           | 0.708        | 0.052             | 0.114  0.008  | 0.176  0.020  | 0.732  0.631  0.783  | 0.061  0.060  0.036 
+10    | 0.000030  | 0.084      | 0.137      | 0.856           | 0.715        | 0.050             | 0.110  0.007  | 0.176  0.020  | 0.738  0.638  0.785  | 0.059  0.061  0.030 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.137      | 0.856           | 0.715        | 0.050             | 0.176  0.020  | 0.738  0.638  0.785  | 0.059  0.061  0.030 
+266     | 266     | 0.131      | 0.856           | 0.716        | 0.051             | 0.168  0.021  | 0.732  0.641  0.793  | 0.061  0.061  0.030 
+360     | 310     | 0.124      | 0.846           | 0.682        | 0.045             | 0.162  0.009  | 0.744  0.558  0.774  | 0.057  0.051  0.027 
+276     | 276     | 0.129      | 0.871           | 0.751        | 0.049             | 0.166  0.019  | 0.833  0.691  0.669  | 0.039  0.063  0.045 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder
+Loss : 0.25*dice+0.75*BCE
+On padded images
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with LR 3e-4 to 3e-5
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+(2h 34m 52s)  
+(Max GPU mem usage : 14122.875 MB) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.214      | 0.074      | 0.792           | 0.587        | 0.071             | 0.647  0.070  | 0.263  0.010  | 0.628  0.517  0.655  | 0.077  0.089  0.045 
+2     | 0.000300  | 0.063      | 0.061      | 0.793           | 0.620        | 0.091             | 0.228  0.008  | 0.208  0.012  | 0.647  0.558  0.726  | 0.112  0.098  0.062 
+3     | 0.000300  | 0.051      | 0.057      | 0.820           | 0.657        | 0.072             | 0.182  0.007  | 0.192  0.012  | 0.685  0.602  0.748  | 0.092  0.080  0.045 
+4     | 0.000287  | 0.046      | 0.058      | 0.838           | 0.683        | 0.058             | 0.164  0.007  | 0.197  0.012  | 0.711  0.608  0.738  | 0.065  0.072  0.037 
+5     | 0.000249  | 0.042      | 0.055      | 0.845           | 0.702        | 0.059             | 0.149  0.006  | 0.185  0.011  | 0.730  0.617  0.773  | 0.065  0.074  0.037 
+6     | 0.000195  | 0.039      | 0.055      | 0.845           | 0.695        | 0.055             | 0.139  0.006  | 0.185  0.011  | 0.721  0.619  0.759  | 0.063  0.065  0.038 
+7     | 0.000135  | 0.036      | 0.053      | 0.853           | 0.715        | 0.055             | 0.127  0.005  | 0.179  0.011  | 0.743  0.639  0.762  | 0.062  0.059  0.045 
+8     | 0.000081  | 0.034      | 0.052      | 0.858           | 0.719        | 0.050             | 0.120  0.005  | 0.174  0.012  | 0.745  0.646  0.779  | 0.064  0.056  0.030 
+9     | 0.000043  | 0.032      | 0.053      | 0.856           | 0.719        | 0.053             | 0.114  0.005  | 0.176  0.012  | 0.748  0.643  0.774  | 0.063  0.060  0.036 
+10    | 0.000030  | 0.031      | 0.053      | 0.859           | 0.721        | 0.050             | 0.111  0.004  | 0.177  0.012  | 0.745  0.644  0.781  | 0.062  0.057  0.031 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.053      | 0.859           | 0.721        | 0.050             | 0.177  0.012  | 0.745  0.644  0.781  | 0.062  0.057  0.031 
+266     | 266     | 0.051      | 0.859           | 0.723        | 0.051             | 0.166  0.012  | 0.741  0.649  0.788  | 0.063  0.058  0.031 
+360     | 310     | 0.047      | 0.845           | 0.682        | 0.046             | 0.170  0.006  | 0.735  0.544  0.762  | 0.055  0.057  0.028 
+276     | 276     | 0.052      | 0.876           | 0.754        | 0.043             | 0.168  0.013  | 0.821  0.681  0.706  | 0.046  0.050  0.032 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder
+Loss : 0.25*dice+0.75*BCE
+On padded images
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with LR 3e-4 to 1e-4
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+(2h 34m 26s)  
+(Max GPU mem usage : 14122.875 MB) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-B  | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.218      | 0.071      | 0.818           | 0.633        | 0.058             | 0.659  0.071  | 0.254  0.010  | 0.663  0.558  0.695  | 0.074  0.068  0.032 
+2     | 0.000300  | 0.064      | 0.061      | 0.805           | 0.637        | 0.083             | 0.231  0.008  | 0.209  0.012  | 0.677  0.563  0.728  | 0.094  0.104  0.050 
+3     | 0.000300  | 0.051      | 0.060      | 0.818           | 0.653        | 0.072             | 0.182  0.007  | 0.198  0.013  | 0.681  0.573  0.753  | 0.091  0.087  0.038 
+4     | 0.000290  | 0.046      | 0.056      | 0.828           | 0.677        | 0.071             | 0.164  0.007  | 0.190  0.011  | 0.708  0.610  0.744  | 0.081  0.084  0.049 
+5     | 0.000262  | 0.043      | 0.058      | 0.827           | 0.669        | 0.068             | 0.151  0.006  | 0.192  0.013  | 0.704  0.588  0.743  | 0.076  0.088  0.041 
+6     | 0.000222  | 0.039      | 0.056      | 0.848           | 0.690        | 0.047             | 0.140  0.006  | 0.190  0.011  | 0.712  0.612  0.771  | 0.046  0.068  0.027 
+7     | 0.000178  | 0.037      | 0.053      | 0.855           | 0.715        | 0.052             | 0.131  0.005  | 0.177  0.011  | 0.739  0.638  0.777  | 0.058  0.060  0.038 
+8     | 0.000138  | 0.035      | 0.053      | 0.860           | 0.717        | 0.045             | 0.124  0.005  | 0.176  0.012  | 0.742  0.641  0.773  | 0.059  0.053  0.024 
+9     | 0.000110  | 0.033      | 0.052      | 0.860           | 0.721        | 0.047             | 0.119  0.005  | 0.174  0.012  | 0.747  0.652  0.777  | 0.058  0.056  0.028 
+10    | 0.000100  | 0.032      | 0.053      | 0.865           | 0.729        | 0.044             | 0.114  0.005  | 0.177  0.012  | 0.752  0.652  0.787  | 0.045  0.058  0.028 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.053      | 0.865           | 0.729        | 0.044             | 0.177  0.012  | 0.752  0.652  0.787  | 0.045  0.058  0.028 
+266     | 266     | 0.054      | 0.866           | 0.730        | 0.044             | 0.178  0.012  | 0.748  0.655  0.794  | 0.046  0.059  0.026 
+360     | 310     | 0.043      | 0.848           | 0.693        | 0.048             | 0.157  0.006  | 0.761  0.575  0.778  | 0.042  0.061  0.043 
+276     | 276     | 0.049      | 0.881           | 0.755        | 0.035             | 0.159  0.012  | 0.814  0.696  0.698  | 0.031  0.044  0.029 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder
+Loss : dice * 0.2 + lovasz * 0.2 + bce * 0.6
+On padded images
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with LR 3e-4 to 1e-4
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+(2h 36m 41s)  
+(Max GPU mem usage : 14124.875 MB) 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-D  TLo-L  TLo-B  | VLo-D  VLo-L  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+--------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.409      | 0.203      | 0.807           | 0.612        | 0.064             | 0.888  0.768  0.130  | 0.511  0.450  0.018  | 0.673  0.509  0.614  | 0.062  0.057  0.072 
+2     | 0.000300  | 0.185      | 0.162      | 0.834           | 0.677        | 0.061             | 0.464  0.430  0.009  | 0.281  0.508  0.007  | 0.709  0.590  0.736  | 0.081  0.063  0.037 
+3     | 0.000300  | 0.132      | 0.145      | 0.852           | 0.707        | 0.050             | 0.280  0.364  0.005  | 0.237  0.466  0.007  | 0.740  0.616  0.748  | 0.058  0.057  0.036 
+4     | 0.000290  | 0.114      | 0.138      | 0.855           | 0.714        | 0.051             | 0.232  0.324  0.004  | 0.229  0.444  0.006  | 0.743  0.628  0.768  | 0.060  0.063  0.030 
+5     | 0.000262  | 0.102      | 0.141      | 0.858           | 0.716        | 0.047             | 0.205  0.295  0.004  | 0.222  0.467  0.006  | 0.741  0.636  0.760  | 0.056  0.057  0.028 
+6     | 0.000222  | 0.094      | 0.138      | 0.858           | 0.713        | 0.044             | 0.187  0.273  0.004  | 0.221  0.453  0.006  | 0.735  0.629  0.772  | 0.055  0.056  0.022 
+7     | 0.000178  | 0.088      | 0.145      | 0.860           | 0.726        | 0.051             | 0.174  0.256  0.003  | 0.208  0.495  0.006  | 0.750  0.648  0.777  | 0.059  0.053  0.041 
+8     | 0.000138  | 0.083      | 0.147      | 0.863           | 0.721        | 0.042             | 0.163  0.241  0.003  | 0.210  0.505  0.007  | 0.740  0.645  0.775  | 0.049  0.052  0.025 
+9     | 0.000110  | 0.078      | 0.147      | 0.865           | 0.732        | 0.045             | 0.153  0.229  0.003  | 0.200  0.514  0.006  | 0.753  0.654  0.781  | 0.054  0.055  0.028 
+10    | 0.000100  | 0.076      | 0.152      | 0.862           | 0.729        | 0.050             | 0.148  0.221  0.003  | 0.200  0.541  0.007  | 0.752  0.649  0.781  | 0.054  0.062  0.033 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-D  VLo-L  VLo-B  | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+--------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.152      | 0.862           | 0.729        | 0.050             | 0.200  0.541  0.007  | 0.752  0.649  0.781  | 0.054  0.062  0.033 
+266     | 266     | 0.148      | 0.862           | 0.732        | 0.051             | 0.190  0.529  0.007  | 0.748  0.656  0.788  | 0.055  0.065  0.033 
+360     | 310     | 0.157      | 0.847           | 0.682        | 0.043             | 0.205  0.569  0.003  | 0.737  0.545  0.770  | 0.053  0.049  0.026 
+276     | 276     | 0.189      | 0.879           | 0.753        | 0.038             | 0.204  0.720  0.007  | 0.828  0.667  0.694  | 0.046  0.035  0.033 </t>
+  </si>
 </sst>
 </file>
 
@@ -1155,7 +1348,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1189,6 +1382,16 @@
       <name val="Courier New"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1239,7 +1442,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1310,6 +1513,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1495,10 +1706,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K108"/>
+  <dimension ref="A1:K126"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A102" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D107" activeCellId="0" sqref="D107"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B124" activeCellId="0" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1507,7 +1718,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="192.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="207.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="13.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="12.23"/>
   </cols>
@@ -1939,7 +2150,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="138.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="8" t="s">
         <v>66</v>
       </c>
@@ -1957,7 +2168,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="382.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="199.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="8" t="s">
         <v>68</v>
       </c>
@@ -2328,6 +2539,192 @@
       </c>
       <c r="D108" s="14" t="n">
         <v>0.83613</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" s="2" t="n">
+        <v>0.856</v>
+      </c>
+      <c r="C110" s="14" t="n">
+        <v>0.85422</v>
+      </c>
+      <c r="D110" s="14" t="n">
+        <v>0.84085</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B111" s="2" t="n">
+        <v>0.857</v>
+      </c>
+      <c r="C111" s="14" t="n">
+        <v>0.8555</v>
+      </c>
+      <c r="D111" s="14" t="n">
+        <v>0.841</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B113" s="2" t="n">
+        <v>0.862</v>
+      </c>
+      <c r="C113" s="14" t="n">
+        <v>0.85393</v>
+      </c>
+      <c r="D113" s="14" t="n">
+        <v>0.84427</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B114" s="2" t="n">
+        <v>0.858</v>
+      </c>
+      <c r="C114" s="14" t="n">
+        <v>0.85244</v>
+      </c>
+      <c r="D114" s="14" t="n">
+        <v>0.84507</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116" s="2" t="n">
+        <v>0.856</v>
+      </c>
+      <c r="C116" s="14" t="n">
+        <v>0.85488</v>
+      </c>
+      <c r="D116" s="14" t="n">
+        <v>0.84438</v>
+      </c>
+      <c r="E116" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118" s="2" t="n">
+        <v>0.859</v>
+      </c>
+      <c r="C118" s="14" t="n">
+        <v>0.85533</v>
+      </c>
+      <c r="D118" s="14" t="n">
+        <v>0.844</v>
+      </c>
+      <c r="E118" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B119" s="2" t="n">
+        <v>0.858</v>
+      </c>
+      <c r="C119" s="14" t="n">
+        <v>0.8522</v>
+      </c>
+      <c r="D119" s="14" t="n">
+        <v>0.8404</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B121" s="2" t="n">
+        <v>0.865</v>
+      </c>
+      <c r="C121" s="14" t="n">
+        <v>0.84192</v>
+      </c>
+      <c r="D121" s="14" t="n">
+        <v>0.83443</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B122" s="2" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="C122" s="14" t="n">
+        <v>0.84455</v>
+      </c>
+      <c r="D122" s="14" t="n">
+        <v>0.83667</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B124" s="2" t="n">
+        <v>0.862</v>
+      </c>
+      <c r="C124" s="18" t="n">
+        <v>0.85614</v>
+      </c>
+      <c r="D124" s="18" t="n">
+        <v>0.84691</v>
+      </c>
+      <c r="E124" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B125" s="2" t="n">
+        <v>0.865</v>
+      </c>
+      <c r="C125" s="18" t="n">
+        <v>0.8544</v>
+      </c>
+      <c r="D125" s="18" t="n">
+        <v>0.84696</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B126" s="2" t="n">
+        <v>0.863</v>
+      </c>
+      <c r="C126" s="18" t="n">
+        <v>0.84032</v>
+      </c>
+      <c r="D126" s="18" t="n">
+        <v>0.83256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected seg loss presence gate, included presence loss pos_weight
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="145">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -1339,6 +1339,428 @@
 266     | 266     | 0.148      | 0.862           | 0.732        | 0.051             | 0.190  0.529  0.007  | 0.748  0.656  0.788  | 0.055  0.065  0.033 
 360     | 310     | 0.157      | 0.847           | 0.682        | 0.043             | 0.205  0.569  0.003  | 0.737  0.545  0.770  | 0.053  0.049  0.026 
 276     | 276     | 0.189      | 0.879           | 0.753        | 0.038             | 0.204  0.720  0.007  | 0.828  0.667  0.694  | 0.046  0.035  0.033 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder 
+with presence head
+per class seg loss : 
+dice * 0.2 + lovasz * 0.2 + bce * 0.6
+total_loss = 1.0 * presence_loss + 1.0 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+On padded images
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with LR 3e-4 to 1e-4
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+(2h 36m 44s – failed before visualizing/evaluation)  
+(Max GPU mem usage : ? MB) 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-L TLo-LB-B TLo-SB-D TLo-SB-L TLo-SB-B TLo-S-D  TLo-S-L  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.502      | 0.292      | 0.807           | 0.609        | 0.062             | 0.184    0.318    0.701    0.529    0.057    0.875    0.561    0.111    0.889    0.450    0.103   | 0.113    0.179    0.367    0.440    0.009    0.537    0.418    0.020    0.413    0.251    0.009   | 0.677  0.510  0.614  | 0.074  0.064  0.047 
+2     | 0.000300  | 0.240      | 0.282      | 0.830           | 0.659        | 0.056             | 0.079    0.161    0.323    0.374    0.007    0.554    0.418    0.013    0.403    0.258    0.005   | 0.127    0.155    0.269    0.471    0.008    0.383    0.487    0.012    0.209    0.257    0.003   | 0.703  0.590  0.690  | 0.067  0.063  0.039 
+3     | 0.000300  | 0.185      | 0.261      | 0.839           | 0.687        | 0.059             | 0.058    0.127    0.253    0.322    0.006    0.416    0.380    0.009    0.234    0.211    0.003   | 0.117    0.144    0.255    0.453    0.008    0.344    0.493    0.011    0.163    0.233    0.003   | 0.706  0.613  0.749  | 0.064  0.062  0.052 
+4     | 0.000290  | 0.162      | 0.256      | 0.843           | 0.695        | 0.058             | 0.048    0.114    0.224    0.295    0.005    0.364    0.354    0.008    0.193    0.190    0.002   | 0.118    0.138    0.238    0.426    0.007    0.338    0.465    0.010    0.154    0.240    0.002   | 0.734  0.612  0.732  | 0.066  0.068  0.041 
+5     | 0.000262  | 0.140      | 0.245      | 0.845           | 0.694        | 0.055             | 0.037    0.103    0.201    0.269    0.005    0.327    0.327    0.007    0.168    0.169    0.002   | 0.105    0.140    0.240    0.443    0.008    0.333    0.479    0.010    0.144    0.250    0.003   | 0.727  0.602  0.749  | 0.058  0.064  0.044 
+6     | 0.000222  | 0.125      | 0.257      | 0.848           | 0.699        | 0.053             | 0.030    0.095    0.184    0.248    0.004    0.299    0.301    0.006    0.151    0.156    0.002   | 0.117    0.140    0.237    0.464    0.008    0.319    0.465    0.010    0.143    0.243    0.003   | 0.718  0.625  0.760  | 0.054  0.057  0.049 
+7     | 0.000178  | 0.110      | 0.333      | 0.849           | 0.714        | 0.060             | 0.023    0.087    0.168    0.228    0.004    0.276    0.282    0.006    0.139    0.142    0.002   | 0.186    0.147    0.216    0.526    0.008    0.297    0.559    0.011    0.128    0.236    0.002   | 0.740  0.633  0.773  | 0.067  0.067  0.047 
+8     | 0.000138  | 0.100      | 0.277      | 0.853           | 0.712        | 0.053             | 0.019    0.082    0.157    0.214    0.004    0.259    0.267    0.006    0.131    0.134    0.002   | 0.136    0.141    0.222    0.472    0.007    0.299    0.517    0.010    0.135    0.248    0.002   | 0.741  0.632  0.757  | 0.056  0.060  0.043 
+9     | 0.000110  | 0.092      | 0.271      | 0.856           | 0.718        | 0.052             | 0.014    0.078    0.149    0.205    0.004    0.246    0.255    0.005    0.124    0.125    0.002   | 0.131    0.140    0.213    0.469    0.008    0.292    0.508    0.010    0.131    0.257    0.002   | 0.744  0.642  0.762  | 0.056  0.055  0.046 
+10   | 0.000100  | 0.087      | 0.295      | 0.854           | 0.711        | 0.051             | 0.012    0.075    0.143    0.195    0.003    0.235    0.244    0.005    0.120    0.121    0.002   | 0.151    0.145    0.211    0.498    0.008    0.289    0.539    0.010    0.131    0.264    0.002   | 0.741  0.632  0.761  | 0.058  0.061  0.034 
+Cutoffs(LB,SB,S) | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+(0.00,0.00,0.00) | 0.295      | 0.852           | 0.707        | 0.052             | 0.151    0.145    0.211    0.498    0.008    0.289    0.539    0.010    0.131    0.264    0.002   | 0.739  0.628  0.756  | 0.058  0.061  0.036 
+(0.25,0.25,0.25) | 0.295      | 0.852           | 0.708        | 0.051             | 0.151    0.145    0.211    0.498    0.008    0.289    0.539    0.010    0.131    0.264    0.002   | 0.738  0.628  0.760  | 0.058  0.061  0.034 
+(0.50,0.50,0.50) | 0.295      | 0.854           | 0.711        | 0.051             | 0.151    0.145    0.211    0.498    0.008    0.289    0.539    0.010    0.131    0.264    0.002   | 0.741  0.632  0.761  | 0.058  0.061  0.034 
+(0.75,0.75,0.75) | 0.295      | 0.854           | 0.711        | 0.051             | 0.151    0.145    0.211    0.498    0.008    0.289    0.539    0.010    0.131    0.264    0.002   | 0.739  0.632  0.761  | 0.058  0.061  0.033 
+(0.60,0.70,0.70) | 0.295      | 0.854           | 0.712        | 0.051             | 0.151    0.145    0.211    0.498    0.008    0.289    0.539    0.010    0.131    0.264    0.002   | 0.742  0.632  0.762  | 0.058  0.061  0.033 
+(0.60,0.70,0.80) | 0.295      | 0.854           | 0.712        | 0.051             | 0.151    0.145    0.211    0.498    0.008    0.289    0.539    0.010    0.131    0.264    0.002   | 0.742  0.632  0.761  | 0.058  0.061  0.033 
+(0.50,0.75,0.75) | 0.295      | 0.853           | 0.710        | 0.051             | 0.151    0.145    0.211    0.498    0.008    0.289    0.539    0.010    0.131    0.264    0.002   | 0.741  0.632  0.761  | 0.058  0.061  0.033 
+best cutoff : (0.6, 0.7, 0.7) best combined metric : (0.8543)
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.295      | 0.854           | 0.712        | 0.051             | 0.151    0.145    0.211    0.498    0.008    0.289    0.539    0.010    0.131    0.264    0.002   | 0.742  0.632  0.762  | 0.058  0.061  0.033 
+266     | 266     | 0.283      | 0.854           | 0.714        | 0.053             | 0.143    0.141    0.210    0.501    0.008    0.290    0.531    0.011    0.112    0.242    0.002   | 0.739  0.634  0.773  | 0.061  0.064  0.033 
+360     | 310     | 0.302      | 0.839           | 0.660        | 0.041             | 0.169    0.133    0.181    0.400    0.003    0.321    0.488    0.006    0.167    0.370    0.002   | 0.714  0.558  0.697  | 0.040  0.047  0.037 
+276     | 276     | 0.472      | 0.880           | 0.755        | 0.037             | 0.293    0.179    0.183    0.565    0.006    0.299    0.785    0.012    0.141    0.518    0.003   | 0.819  0.693  0.702  | 0.036  0.042  0.032 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder 
+with presence head
+per class seg loss : 
+dice * 0.2 + lovasz * 0.2 + bce * 0.6
+total_loss = 1.0 * presence_loss + 1.0 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+On padded images
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with LR 5e-4 to 2.5e-4
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+(3h 14m 20s)  
+(Max GPU mem usage : 15512.875 MB) 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-L TLo-LB-B TLo-SB-D TLo-SB-L TLo-SB-B TLo-S-D  TLo-S-L  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.738      | 0.353      | 0.766           | 0.515        | 0.067             | 0.378    0.360    0.810    0.718    0.076    0.891    0.637    0.106    0.921    0.552    0.097   | 0.153    0.200    0.420    0.522    0.013    0.531    0.484    0.022    0.427    0.318    0.009   | 0.590  0.437  0.466  | 0.079  0.073  0.050 
+2     | 0.000500  | 0.289      | 0.326      | 0.812           | 0.618        | 0.059             | 0.114    0.175    0.361    0.426    0.008    0.565    0.455    0.013    0.394    0.308    0.005   | 0.159    0.166    0.292    0.526    0.009    0.396    0.514    0.011    0.206    0.303    0.003   | 0.675  0.536  0.656  | 0.076  0.053  0.047 
+3     | 0.000500  | 0.215      | 0.289      | 0.834           | 0.668        | 0.055             | 0.078    0.137    0.274    0.354    0.006    0.436    0.413    0.010    0.238    0.232    0.003   | 0.137    0.153    0.256    0.472    0.008    0.356    0.513    0.011    0.177    0.283    0.003   | 0.712  0.586  0.702  | 0.069  0.060  0.037 
+4     | 0.000488  | 0.186      | 0.240      | 0.837           | 0.678        | 0.058             | 0.063    0.123    0.246    0.322    0.006    0.390    0.385    0.009    0.200    0.204    0.003   | 0.102    0.138    0.258    0.407    0.007    0.351    0.427    0.010    0.165    0.264    0.003   | 0.719  0.604  0.708  | 0.060  0.078  0.035 
+5     | 0.000453  | 0.162      | 0.269      | 0.844           | 0.687        | 0.051             | 0.050    0.112    0.220    0.292    0.005    0.352    0.353    0.008    0.179    0.186    0.002   | 0.125    0.144    0.244    0.452    0.008    0.346    0.458    0.010    0.156    0.292    0.003   | 0.727  0.606  0.713  | 0.059  0.062  0.030 
+6     | 0.000403  | 0.149      | 0.269      | 0.847           | 0.695        | 0.052             | 0.044    0.105    0.206    0.278    0.005    0.329    0.335    0.007    0.165    0.174    0.002   | 0.125    0.144    0.233    0.501    0.008    0.316    0.484    0.010    0.145    0.254    0.003   | 0.719  0.625  0.746  | 0.056  0.058  0.043 
+7     | 0.000347  | 0.129      | 0.296      | 0.838           | 0.692        | 0.064             | 0.033    0.096    0.185    0.253    0.004    0.298    0.307    0.007    0.149    0.157    0.002   | 0.153    0.143    0.242    0.492    0.008    0.324    0.492    0.010    0.143    0.253    0.002   | 0.715  0.620  0.751  | 0.083  0.070  0.038 
+8     | 0.000297  | 0.119      | 0.298      | 0.845           | 0.683        | 0.048             | 0.029    0.091    0.176    0.240    0.004    0.284    0.295    0.006    0.141    0.148    0.002   | 0.146    0.152    0.245    0.498    0.009    0.318    0.552    0.011    0.150    0.270    0.003   | 0.715  0.591  0.738  | 0.054  0.054  0.035 
+9     | 0.000262  | 0.110      | 0.275      | 0.850           | 0.703        | 0.052             | 0.024    0.086    0.164    0.228    0.004    0.267    0.282    0.006    0.132    0.139    0.002   | 0.128    0.147    0.229    0.495    0.008    0.303    0.532    0.011    0.137    0.277    0.003   | 0.729  0.629  0.749  | 0.060  0.068  0.028 
+10    | 0.000250  | 0.104      | 0.287      | 0.844           | 0.689        | 0.053             | 0.022    0.083    0.159    0.220    0.004    0.257    0.271    0.006    0.130    0.136    0.002   | 0.135    0.151    0.239    0.507    0.008    0.312    0.529    0.011    0.150    0.291    0.003   | 0.714  0.614  0.738  | 0.062  0.058  0.040 
+Confusion Matrix raw counts
+    LB		SB		S
+TP	2402	1870	1429
+FP	173		172		88
+FN	175		199		97
+TN	4546	5055	5682
+Confusion Matrix normalized per class
+	LB		SB		S
+TP	0.329	0.256	0.196
+FP	0.024	0.024	0.012
+FN	0.024	0.027	0.013
+TN	0.623	0.693	0.779
+Cutoffs(LB,SB,S) | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+(0.00,0.00,0.00) | 0.287      | 0.842522        | 0.688        | 0.055             | 0.135    0.151    0.239    0.507    0.008    0.312    0.529    0.011    0.150    0.291    0.003   | 0.719  0.613  0.729  | 0.062  0.058  0.044 
+(0.25,0.25,0.25) | 0.287      | 0.843225        | 0.688        | 0.053             | 0.135    0.151    0.239    0.507    0.008    0.312    0.529    0.011    0.150    0.291    0.003   | 0.715  0.613  0.738  | 0.062  0.058  0.040 
+(0.50,0.50,0.50) | 0.287      | 0.843513        | 0.689        | 0.053             | 0.135    0.151    0.239    0.507    0.008    0.312    0.529    0.011    0.150    0.291    0.003   | 0.714  0.614  0.738  | 0.062  0.058  0.040 
+(0.75,0.75,0.75) | 0.287      | 0.841375        | 0.683        | 0.053             | 0.135    0.151    0.239    0.507    0.008    0.312    0.529    0.011    0.150    0.291    0.003   | 0.709  0.609  0.728  | 0.062  0.057  0.040 
+(0.60,0.70,0.70) | 0.287      | 0.841884        | 0.684        | 0.053             | 0.135    0.151    0.239    0.507    0.008    0.312    0.529    0.011    0.150    0.291    0.003   | 0.712  0.610  0.731  | 0.062  0.057  0.040 
+(0.60,0.70,0.80) | 0.287      | 0.841926        | 0.684        | 0.052             | 0.135    0.151    0.239    0.507    0.008    0.312    0.529    0.011    0.150    0.291    0.003   | 0.712  0.610  0.726  | 0.062  0.057  0.038 
+(0.50,0.75,0.75) | 0.287      | 0.841382        | 0.683        | 0.053             | 0.135    0.151    0.239    0.507    0.008    0.312    0.529    0.011    0.150    0.291    0.003   | 0.714  0.609  0.728  | 0.062  0.057  0.040
+best cutoff : (0.5, 0.5, 0.5) best combined metric : (0.8435)
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.287      | 0.844           | 0.689        | 0.053             | 0.135    0.151    0.239    0.507    0.008    0.312    0.529    0.011    0.150    0.291    0.003   | 0.714  0.614  0.738  | 0.062  0.058  0.040 
+266     | 266     | 0.275      | 0.846           | 0.696        | 0.054             | 0.129    0.146    0.232    0.515    0.009    0.305    0.520    0.011    0.124    0.250    0.003   | 0.713  0.621  0.762  | 0.064  0.059  0.041 
+360     | 310     | 0.320      | 0.798           | 0.571        | 0.051             | 0.158    0.162    0.221    0.353    0.003    0.372    0.501    0.005    0.241    0.620    0.005   | 0.663  0.471  0.566  | 0.064  0.057  0.032 
+276     | 276     | 0.405      | 0.865           | 0.725        | 0.041             | 0.225    0.180    0.207    0.565    0.007    0.324    0.753    0.013    0.149    0.535    0.003   | 0.784  0.665  0.674  | 0.041  0.045  0.038 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder 
+with presence head
+per class seg loss : 
+dice * 0.1 + lovasz * 0.6 + bce * 0.3
+total_loss = 1.0 * presence_loss + 1.0 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+On padded images
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with LR 3e-4 to 1e-4
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+(2h 48m 31s)  
+(Max GPU mem usage : 14358.875 MB) 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-L TLo-LB-B TLo-SB-D TLo-SB-L TLo-SB-B TLo-S-D  TLo-S-L  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.621      | 0.448      | 0.782           | 0.586        | 0.088             | 0.184    0.437    0.899    0.498    0.115    0.949    0.528    0.180    0.963    0.436    0.160   | 0.141    0.307    0.622    0.388    0.033    0.676    0.372    0.077    0.604    0.253    0.054   | 0.664  0.470  0.602  | 0.077  0.101  0.085 
+2     | 0.000300  | 0.351      | 0.413      | 0.822           | 0.647        | 0.061             | 0.081    0.270    0.591    0.323    0.017    0.850    0.354    0.045    0.809    0.227    0.025   | 0.144    0.269    0.400    0.383    0.011    0.570    0.378    0.027    0.408    0.209    0.009   | 0.696  0.554  0.664  | 0.069  0.069  0.044 
+3     | 0.000300  | 0.280      | 0.380      | 0.833           | 0.682        | 0.066             | 0.061    0.219    0.389    0.280    0.008    0.683    0.323    0.019    0.488    0.184    0.006   | 0.134    0.246    0.337    0.358    0.008    0.476    0.368    0.015    0.267    0.201    0.004   | 0.716  0.601  0.723  | 0.066  0.073  0.059 
+4     | 0.000290  | 0.242      | 0.377      | 0.842           | 0.693        | 0.059             | 0.049    0.193    0.322    0.255    0.006    0.555    0.301    0.012    0.318    0.162    0.003   | 0.136    0.241    0.321    0.362    0.008    0.443    0.371    0.013    0.216    0.184    0.003   | 0.718  0.613  0.754  | 0.067  0.072  0.039 
+5     | 0.000262  | 0.210      | 0.363      | 0.848           | 0.694        | 0.049             | 0.039    0.172    0.279    0.230    0.005    0.475    0.276    0.009    0.251    0.144    0.002   | 0.120    0.242    0.300    0.359    0.008    0.415    0.367    0.011    0.189    0.209    0.003   | 0.726  0.615  0.716  | 0.058  0.058  0.030 
+6     | 0.000222  | 0.189      | 0.409      | 0.852           | 0.712        | 0.055             | 0.030    0.159    0.252    0.213    0.005    0.424    0.258    0.008    0.219    0.134    0.002   | 0.166    0.243    0.270    0.379    0.007    0.379    0.382    0.010    0.177    0.185    0.002   | 0.738  0.633  0.765  | 0.064  0.056  0.044 
+7     | 0.000178  | 0.173      | 0.391      | 0.850           | 0.712        | 0.058             | 0.025    0.148    0.229    0.200    0.004    0.385    0.243    0.007    0.196    0.124    0.002   | 0.148    0.243    0.269    0.380    0.007    0.367    0.385    0.010    0.180    0.194    0.002   | 0.739  0.634  0.761  | 0.059  0.066  0.051 
+8     | 0.000138  | 0.156      | 0.408      | 0.852           | 0.709        | 0.053             | 0.019    0.137    0.212    0.185    0.004    0.358    0.228    0.007    0.181    0.116    0.002   | 0.159    0.248    0.258    0.384    0.007    0.349    0.405    0.009    0.166    0.197    0.002   | 0.735  0.626  0.765  | 0.056  0.060  0.041 
+9     | 0.000110  | 0.143      | 0.399      | 0.854           | 0.716        | 0.054             | 0.013    0.129    0.196    0.175    0.004    0.331    0.216    0.006    0.168    0.108    0.002   | 0.145    0.253    0.248    0.398    0.007    0.342    0.413    0.010    0.156    0.197    0.002   | 0.742  0.634  0.767  | 0.060  0.060  0.041 
+10    | 0.000100  | 0.139      | 0.390      | 0.855           | 0.717        | 0.053             | 0.013    0.126    0.188    0.171    0.004    0.318    0.210    0.006    0.161    0.106    0.002   | 0.141    0.249    0.247    0.382    0.007    0.340    0.404    0.009    0.152    0.204    0.002   | 0.746  0.634  0.762  | 0.058  0.057  0.044 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.390      | 0.855           | 0.717        | 0.053             | 0.141    0.249    0.247    0.382    0.007    0.340    0.404    0.009    0.152    0.204    0.002   | 0.746  0.634  0.762  | 0.058  0.057  0.044 
+266     | 266     | 0.377      | 0.854           | 0.717        | 0.055             | 0.135    0.242    0.241    0.381    0.007    0.335    0.396    0.009    0.137    0.191    0.002   | 0.741  0.636  0.768  | 0.060  0.058  0.047 
+360     | 310     | 0.365      | 0.854           | 0.692        | 0.038             | 0.141    0.225    0.211    0.336    0.003    0.362    0.350    0.005    0.174    0.258    0.002   | 0.745  0.597  0.741  | 0.043  0.046  0.026 
+276     | 276     | 0.634      | 0.877           | 0.751        | 0.039             | 0.281    0.352    0.243    0.466    0.007    0.388    0.684    0.013    0.171    0.385    0.003   | 0.816  0.659  0.718  | 0.037  0.058  0.023 
+Cutoffs(LB,SB,S) | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+(0.00,0.00,0.00) | 0.390      | 0.854827        | 0.717        | 0.053             | 0.141    0.249    0.247    0.382    0.007    0.340    0.404    0.009    0.152    0.204    0.002   | 0.747  0.636  0.758  | 0.058  0.057  0.045 
+(0.25,0.25,0.25) | 0.390      | 0.854580        | 0.716        | 0.053             | 0.141    0.249    0.247    0.382    0.007    0.340    0.404    0.009    0.152    0.204    0.002   | 0.745  0.636  0.759  | 0.058  0.057  0.044 
+(0.50,0.50,0.50) | 0.390      | 0.855196        | 0.717        | 0.053             | 0.141    0.249    0.247    0.382    0.007    0.340    0.404    0.009    0.152    0.204    0.002   | 0.746  0.634  0.762  | 0.058  0.057  0.044 
+(0.75,0.75,0.75) | 0.390      | 0.854655        | 0.716        | 0.053             | 0.141    0.249    0.247    0.382    0.007    0.340    0.404    0.009    0.152    0.204    0.002   | 0.741  0.635  0.763  | 0.058  0.057  0.043 
+(0.60,0.70,0.70) | 0.390      | 0.854759        | 0.716        | 0.053             | 0.141    0.249    0.247    0.382    0.007    0.340    0.404    0.009    0.152    0.204    0.002   | 0.744  0.634  0.763  | 0.058  0.057  0.043 
+(0.60,0.70,0.80) | 0.390      | 0.855022        | 0.717        | 0.053             | 0.141    0.249    0.247    0.382    0.007    0.340    0.404    0.009    0.152    0.204    0.002   | 0.744  0.634  0.764  | 0.058  0.057  0.043 
+(0.50,0.75,0.75) | 0.390      | 0.855121        | 0.717        | 0.053             | 0.141    0.249    0.247    0.382    0.007    0.340    0.404    0.009    0.152    0.204    0.002   | 0.746  0.635  0.763  | 0.058  0.057  0.043 
+best cutoff : (0.50,0.50,0.50)  best combined metric : (0.855196)
+Confusion Matrix raw counts
+	LB		SB		S
+TP	2474	1907	1454
+FP	170		166		80
+FN	103		162		72
+TN	4549	5061	5690
+Confusion Matrix normalized per class
+	LB		SB		S
+TP	0.339	0.261	0.199
+FP	0.023	0.023	0.011
+FN	0.014	0.022	0.010
+TN	0.623	0.694	0.780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA (0.5,0.5,0.5) cutoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cutoffs(LB,SB,S) | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+(0.00,0.00,0.00) | 0.395      | 0.857176        | 0.725        | 0.055             | 0.155    0.240    0.250    0.380    0.007    0.349    0.387    0.010    0.159    0.181    0.002   | 0.752  0.651  0.774  | 0.059  0.062  0.044 
+(0.25,0.25,0.25) | 0.395      | 0.857421        | 0.726        | 0.055             | 0.155    0.240    0.250    0.380    0.007    0.349    0.387    0.010    0.159    0.181    0.002   | 0.751  0.650  0.777  | 0.059  0.062  0.044 
+(0.50,0.50,0.50) | 0.395      | 0.857811        | 0.727        | 0.055             | 0.155    0.240    0.250    0.380    0.007    0.349    0.387    0.010    0.159    0.181    0.002   | 0.751  0.650  0.778  | 0.059  0.062  0.044 
+(0.75,0.75,0.75) | 0.395      | 0.857864        | 0.727        | 0.055             | 0.155    0.240    0.250    0.380    0.007    0.349    0.387    0.010    0.159    0.181    0.002   | 0.750  0.649  0.779  | 0.059  0.062  0.043 
+(0.60,0.70,0.70) | 0.395      | 0.858289        | 0.728        | 0.055             | 0.155    0.240    0.250    0.380    0.007    0.349    0.387    0.010    0.159    0.181    0.002   | 0.751  0.649  0.780  | 0.059  0.062  0.043 
+(0.60,0.70,0.80) | 0.395      | 0.858175        | 0.727        | 0.054             | 0.155    0.240    0.250    0.380    0.007    0.349    0.387    0.010    0.159    0.181    0.002   | 0.751  0.649  0.778  | 0.059  0.062  0.042 
+(0.50,0.75,0.75) | 0.395      | 0.857740        | 0.726        | 0.055             | 0.155    0.240    0.250    0.380    0.007    0.349    0.387    0.010    0.159    0.181    0.002   | 0.751  0.649  0.779  | 0.059  0.062  0.043 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA with (0.6,0.7,0.7) cutoffs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.395      | 0.858           | 0.728        | 0.055             | 0.155    0.240    0.250    0.380    0.007    0.349    0.387    0.010    0.159    0.181    0.002   | 0.751  0.649  0.780  | 0.059  0.062  0.043 
+266     | 266     | 0.375      | 0.858           | 0.731        | 0.057             | 0.143    0.232    0.241    0.374    0.007    0.341    0.374    0.010    0.142    0.167    0.002   | 0.750  0.653  0.789  | 0.061  0.063  0.046 
+360     | 310     | 0.431      | 0.851           | 0.686        | 0.040             | 0.197    0.234    0.227    0.367    0.003    0.387    0.373    0.006    0.179    0.248    0.002   | 0.724  0.600  0.746  | 0.045  0.047  0.028 
+276     | 276     | 0.720      | 0.868           | 0.734        | 0.042             | 0.348    0.372    0.254    0.512    0.008    0.413    0.709    0.015    0.189    0.366    0.003   | 0.800  0.651  0.703  | 0.040  0.060  0.026 
+Confusion Matrix raw counts
+	LB		SB		S
+TP	2511	1943	1453
+FP	215		207		61
+FN	66		126		73
+TN	4504	5020	5709
+Confusion Matrix normalized per class
+	LB		SB		S
+TP	0.344	0.266	0.199
+FP	0.029	0.028	0.008
+FN	0.009	0.017	0.010
+TN	0.617	0.688	0.782
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder 
+with presence head
+per class seg loss : 
+dice * 0.1 + lovasz * 0.6 + bce * 0.3
+total_loss = 0.75 * presence_loss + 0.25 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+On padded images
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with LR 3e-4 to 1e-4
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+BS = 32 (train/valid/test)
+(2h 48m 47s)  
+(Max GPU mem usage : 10900.875 MB)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-L TLo-LB-B TLo-SB-D TLo-SB-L TLo-SB-B TLo-S-D  TLo-S-L  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.285      | 0.223      | 0.752           | 0.536        | 0.103             | 0.236    0.432    0.923    0.551    0.137    0.955    0.556    0.199    0.970    0.480    0.177   | 0.125    0.515    0.475    0.406    0.044    0.465    0.374    0.076    0.398    0.272    0.056   | 0.620  0.440  0.496  | 0.112  0.110  0.088 
+2     | 0.000300  | 0.132      | 0.215      | 0.802           | 0.611        | 0.072             | 0.085    0.276    0.696    0.367    0.025    0.880    0.372    0.055    0.873    0.261    0.034   | 0.134    0.459    0.330    0.402    0.013    0.421    0.377    0.036    0.314    0.234    0.015   | 0.675  0.505  0.628  | 0.068  0.084  0.064 
+3     | 0.000300  | 0.105      | 0.203      | 0.811           | 0.640        | 0.075             | 0.062    0.236    0.487    0.326    0.011    0.776    0.354    0.028    0.659    0.222    0.011   | 0.126    0.435    0.292    0.383    0.011    0.384    0.389    0.023    0.238    0.221    0.006   | 0.688  0.533  0.676  | 0.080  0.088  0.058 
+4     | 0.000290  | 0.090      | 0.193      | 0.819           | 0.657        | 0.074             | 0.051    0.209    0.398    0.298    0.008    0.669    0.334    0.017    0.455    0.196    0.005   | 0.120    0.413    0.268    0.360    0.009    0.354    0.373    0.018    0.192    0.230    0.004   | 0.707  0.576  0.667  | 0.078  0.085  0.057 
+5     | 0.000262  | 0.078      | 0.226      | 0.817           | 0.644        | 0.068             | 0.041    0.189    0.351    0.269    0.007    0.594    0.314    0.013    0.359    0.178    0.004   | 0.150    0.457    0.263    0.380    0.009    0.340    0.396    0.015    0.175    0.270    0.004   | 0.702  0.555  0.622  | 0.073  0.078  0.054 
+6     | 0.000222  | 0.068      | 0.193      | 0.841           | 0.685        | 0.055             | 0.032    0.174    0.315    0.251    0.006    0.535    0.295    0.011    0.297    0.161    0.003   | 0.124    0.402    0.231    0.370    0.008    0.310    0.366    0.012    0.150    0.217    0.003   | 0.719  0.610  0.724  | 0.058  0.061  0.046 
+7     | 0.000178  | 0.061      | 0.233      | 0.839           | 0.689        | 0.061             | 0.026    0.164    0.288    0.236    0.006    0.491    0.280    0.010    0.265    0.150    0.003   | 0.177    0.401    0.223    0.399    0.008    0.299    0.391    0.012    0.144    0.209    0.003   | 0.725  0.612  0.727  | 0.068  0.070  0.047 
+8     | 0.000138  | 0.053      | 0.212      | 0.841           | 0.697        | 0.063             | 0.020    0.152    0.266    0.220    0.005    0.457    0.266    0.009    0.242    0.139    0.002   | 0.149    0.400    0.208    0.379    0.007    0.282    0.384    0.011    0.140    0.219    0.003   | 0.731  0.618  0.734  | 0.065  0.064  0.061 
+9     | 0.000110  | 0.047      | 0.211      | 0.843           | 0.700        | 0.062             | 0.015    0.144    0.247    0.207    0.005    0.428    0.254    0.008    0.220    0.130    0.002   | 0.146    0.407    0.202    0.387    0.007    0.275    0.389    0.011    0.132    0.220    0.003   | 0.732  0.627  0.737  | 0.064  0.070  0.052 
+10    | 0.000100  | 0.045      | 0.230      | 0.844           | 0.703        | 0.062             | 0.014    0.141    0.239    0.204    0.005    0.411    0.248    0.008    0.211    0.126    0.002   | 0.175    0.396    0.199    0.406    0.007    0.266    0.396    0.010    0.127    0.205    0.002   | 0.735  0.637  0.739  | 0.065  0.068  0.053 
+Confusion Matrix raw counts
+	LB		SB		S
+TP	2528	1984	1434
+FP	255		234		101
+FN	49		85		92
+TN	4464	4993	5669
+Confusion Matrix normalized per class
+	LB		SB		S
+TP	0.346	0.272	0.197
+FP	0.035	0.032	0.014
+FN	0.007	0.012	0.013
+TN	0.612	0.684	0.777
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.230      | 0.844           | 0.703        | 0.062             | 0.175    0.396    0.199    0.406    0.007    0.266    0.396    0.010    0.127    0.205    0.002   | 0.735  0.637  0.739  | 0.065  0.068  0.053 
+266     | 266     | 0.223      | 0.845           | 0.707        | 0.063             | 0.165    0.394    0.190    0.406    0.007    0.263    0.389    0.011    0.110    0.190    0.002   | 0.732  0.640  0.752  | 0.067  0.069  0.054 
+360     | 310     | 0.259      | 0.827           | 0.645        | 0.052             | 0.209    0.406    0.194    0.356    0.003    0.311    0.371    0.007    0.158    0.297    0.002   | 0.725  0.589  0.657  | 0.057  0.057  0.042 
+276     | 276     | 0.411      | 0.854           | 0.721        | 0.057             | 0.354    0.584    0.302    0.564    0.008    0.326    0.671    0.015    0.206    0.366    0.003   | 0.794  0.650  0.677  | 0.042  0.067  0.061 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder 
+with presence head
+per class seg loss : 
+dice * 0.25 + bce * 0.75
+total_loss = 0.75 * presence_loss + 0.25 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+On padded images
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with LR 3e-4 to 1e-4
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32  
+BS = 32 (train/valid/test)  
+(2h 34m 50s)  
+(Max GPU mem usage : 10716.875 MB)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-B TLo-SB-D TLo-SB-B TLo-S-D  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.173      | 0.124      | 0.765           | 0.558        | 0.098             | 0.159    0.213    0.599    0.049    0.796    0.099    0.824    0.092   | 0.127    0.115    0.239    0.014    0.310    0.022    0.225    0.008   | 0.633  0.463  0.528  | 0.084  0.114  0.094 
+2     | 0.000300  | 0.078      | 0.125      | 0.811           | 0.617        | 0.061             | 0.076    0.086    0.280    0.011    0.458    0.015    0.345    0.006   | 0.138    0.089    0.186    0.014    0.253    0.020    0.142    0.005   | 0.676  0.530  0.601  | 0.072  0.072  0.039 
+3     | 0.000300  | 0.062      | 0.134      | 0.818           | 0.640        | 0.063             | 0.059    0.071    0.237    0.010    0.383    0.014    0.246    0.005   | 0.152    0.080    0.180    0.014    0.233    0.017    0.118    0.005   | 0.675  0.548  0.680  | 0.065  0.068  0.057 
+4     | 0.000290  | 0.053      | 0.109      | 0.822           | 0.651        | 0.064             | 0.049    0.064    0.216    0.010    0.348    0.013    0.202    0.005   | 0.119    0.079    0.169    0.013    0.233    0.020    0.109    0.005   | 0.695  0.549  0.685  | 0.062  0.080  0.049 
+5     | 0.000262  | 0.044      | 0.115      | 0.825           | 0.658        | 0.063             | 0.040    0.058    0.199    0.009    0.322    0.012    0.180    0.004   | 0.127    0.078    0.179    0.014    0.230    0.018    0.099    0.005   | 0.686  0.559  0.727  | 0.067  0.068  0.055 
+6     | 0.000222  | 0.037      | 0.129      | 0.832           | 0.672        | 0.061             | 0.031    0.054    0.183    0.008    0.298    0.012    0.161    0.004   | 0.148    0.073    0.164    0.013    0.215    0.017    0.095    0.004   | 0.701  0.581  0.730  | 0.066  0.066  0.051 
+7     | 0.000178  | 0.032      | 0.129      | 0.836           | 0.685        | 0.063             | 0.026    0.051    0.172    0.008    0.280    0.011    0.150    0.004   | 0.148    0.071    0.159    0.013    0.211    0.018    0.093    0.004   | 0.713  0.593  0.739  | 0.065  0.072  0.052 
+8     | 0.000138  | 0.025      | 0.145      | 0.834           | 0.675        | 0.060             | 0.018    0.047    0.160    0.007    0.263    0.010    0.140    0.003   | 0.169    0.073    0.161    0.015    0.212    0.020    0.095    0.004   | 0.705  0.588  0.721  | 0.059  0.075  0.047 
+9     | 0.000110  | 0.021      | 0.142      | 0.840           | 0.689        | 0.060             | 0.013    0.045    0.153    0.007    0.252    0.010    0.131    0.003   | 0.165    0.072    0.164    0.015    0.208    0.018    0.093    0.004   | 0.714  0.602  0.744  | 0.060  0.070  0.048 
+10    | 0.000100  | 0.021      | 0.130      | 0.840           | 0.694        | 0.062             | 0.014    0.044    0.150    0.007    0.247    0.010    0.128    0.003   | 0.150    0.069    0.154    0.013    0.207    0.017    0.093    0.004   | 0.727  0.605  0.739  | 0.067  0.065  0.056 
+Confusion Matrix raw counts
+	LB		SB		S
+TP	2464	1902	1439
+FP	179		175		85
+FN	113		167		87
+TN	4540	5052	5685
+Confusion Matrix normalized per class
+	LB		SB		S
+TP	0.338	0.261	0.197
+FP	0.025	0.024	0.012
+FN	0.015	0.023	0.012
+TN	0.622	0.692	0.779
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.130      | 0.840           | 0.694        | 0.062             | 0.150    0.069    0.154    0.013    0.207    0.017    0.093    0.004   | 0.727  0.605  0.739  | 0.067  0.065  0.056 
+266     | 266     | 0.125      | 0.841           | 0.697        | 0.063             | 0.144    0.069    0.152    0.014    0.206    0.018    0.077    0.004   | 0.723  0.607  0.756  | 0.067  0.066  0.056 
+360     | 310     | 0.117      | 0.833           | 0.661        | 0.052             | 0.134    0.066    0.121    0.005    0.219    0.008    0.122    0.005   | 0.733  0.568  0.656  | 0.066  0.055  0.035 
+276     | 276     | 0.287      | 0.838           | 0.696        | 0.067             | 0.352    0.093    0.203    0.014    0.242    0.028    0.167    0.006   | 0.781  0.628  0.621  | 0.062  0.064  0.076 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder 
+with presence head with dropout 0.4
+per class seg loss : 
+dice * 0.1 + lovasz * 0.6 + bce * 0.3
+total_loss = 0.5 * presence_loss + 0.5 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+Presence loss pos_weight = [65/35, 72/28, 79/21]
+On padded images
+With AdamW optim 
+0.01 weight_decay for params except bias&amp;norm
+On 384x384 images with LR 3e-4 to 1e-4
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+BS = 32 (train/valid/test)
+(2h 44m 22s)  
+(Max GPU mem usage : 10900.875 MB)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-L TLo-LB-B TLo-SB-D TLo-SB-L TLo-SB-B TLo-S-D  TLo-S-L  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.336      | 0.349      | 0.752           | 0.542        | 0.108             | 0.271    0.402    0.894    0.495    0.109    0.948    0.535    0.180    0.964    0.440    0.165   | 0.190    0.507    0.448    0.405    0.035    0.463    0.368    0.071    0.390    0.303    0.059   | 0.629  0.472  0.477  | 0.103  0.084  0.139 
+2     | 0.000300  | 0.190      | 0.383      | 0.795           | 0.607        | 0.080             | 0.124    0.256    0.609    0.335    0.018    0.854    0.360    0.046    0.839    0.237    0.029   | 0.299    0.467    0.318    0.391    0.012    0.410    0.430    0.036    0.294    0.244    0.012   | 0.689  0.483  0.597  | 0.088  0.095  0.056 
+3     | 0.000300  | 0.157      | 0.286      | 0.832           | 0.672        | 0.061             | 0.098    0.216    0.423    0.301    0.009    0.719    0.337    0.022    0.570    0.198    0.008   | 0.171    0.402    0.270    0.342    0.009    0.356    0.366    0.017    0.203    0.221    0.005   | 0.719  0.579  0.699  | 0.067  0.066  0.049 
+4     | 0.000290  | 0.135      | 0.285      | 0.833           | 0.678        | 0.064             | 0.080    0.189    0.347    0.270    0.007    0.597    0.314    0.014    0.371    0.175    0.004   | 0.178    0.392    0.247    0.369    0.008    0.325    0.381    0.015    0.160    0.197    0.003   | 0.716  0.596  0.725  | 0.070  0.079  0.043 
+5     | 0.000262  | 0.117      | 0.291      | 0.834           | 0.678        | 0.062             | 0.063    0.172    0.309    0.248    0.006    0.521    0.293    0.011    0.293    0.158    0.003   | 0.176    0.405    0.232    0.356    0.008    0.307    0.370    0.012    0.151    0.211    0.003   | 0.722  0.594  0.708  | 0.073  0.071  0.042 
+6     | 0.000222  | 0.106      | 0.317      | 0.841           | 0.687        | 0.057             | 0.052    0.159    0.278    0.230    0.005    0.471    0.276    0.009    0.251    0.146    0.002   | 0.229    0.406    0.220    0.380    0.007    0.288    0.372    0.011    0.143    0.218    0.003   | 0.716  0.614  0.724  | 0.060  0.058  0.053 
+7     | 0.000178  | 0.094      | 0.284      | 0.846           | 0.706        | 0.060             | 0.040    0.148    0.253    0.214    0.005    0.430    0.260    0.008    0.225    0.134    0.002   | 0.180    0.388    0.212    0.367    0.007    0.278    0.370    0.010    0.129    0.195    0.002   | 0.735  0.623  0.757  | 0.071  0.065  0.044 
+8     | 0.000138  | 0.082      | 0.301      | 0.848           | 0.706        | 0.057             | 0.029    0.136    0.229    0.197    0.004    0.396    0.243    0.007    0.203    0.124    0.002   | 0.205    0.397    0.196    0.380    0.007    0.259    0.389    0.010    0.125    0.202    0.002   | 0.741  0.626  0.751  | 0.059  0.062  0.050 
+9     | 0.000110  | 0.078      | 0.298      | 0.856           | 0.718        | 0.052             | 0.024    0.132    0.218    0.191    0.004    0.375    0.236    0.007    0.190    0.119    0.002   | 0.205    0.392    0.192    0.385    0.007    0.254    0.384    0.010    0.118    0.195    0.002   | 0.739  0.644  0.769  | 0.060  0.061  0.034 
+10    | 0.000100  | 0.074      | 0.298      | 0.851           | 0.713        | 0.057             | 0.021    0.126    0.206    0.184    0.004    0.355    0.227    0.007    0.181    0.115    0.002   | 0.209    0.387    0.199    0.369    0.007    0.255    0.381    0.009    0.119    0.200    0.002   | 0.740  0.641  0.760  | 0.061  0.061  0.048 
+Confusion Matrix raw counts
+    LB      SB      S
+TP  2482    1919    1471
+FP  190     192     97
+FN  95      150     55
+TN  4529    5035    5673
+Confusion Matrix normalized per class
+    LB      SB      S
+TP  0.340   0.263   0.202
+FP  0.026   0.026   0.013
+FN  0.013   0.021   0.008
+TN  0.621   0.690   0.778
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.298      | 0.851           | 0.713        | 0.057             | 0.209    0.387    0.199    0.369    0.007    0.255    0.381    0.009    0.119    0.200    0.002   | 0.740  0.641  0.760  | 0.061  0.061  0.048 
+266     | 266     | 0.292      | 0.852           | 0.716        | 0.057             | 0.198    0.386    0.191    0.371    0.007    0.251    0.377    0.010    0.101    0.181    0.002   | 0.737  0.643  0.773  | 0.063  0.062  0.047 
+360     | 310     | 0.290      | 0.840           | 0.673        | 0.048             | 0.203    0.377    0.194    0.299    0.003    0.306    0.330    0.006    0.149    0.284    0.002   | 0.724  0.588  0.719  | 0.052  0.053  0.040 
+276     | 276     | 0.531      | 0.856           | 0.726        | 0.058             | 0.490    0.573    0.291    0.497    0.007    0.293    0.592    0.012    0.200    0.472    0.003   | 0.797  0.672  0.641  | 0.037  0.067  0.070 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA Epoch 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder 
+with presence head with dropout 0.4
+per class seg loss : 
+dice * 0.1 + lovasz * 0.6 + bce * 0.3
+total_loss = 0.5 * presence_loss + 0.5 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+Presence loss pos_weight = [65/35, 72/28, 79/21]
+On padded images
+With AdamW optim 
+1e-3 weight decay for presence head
+0.01 weight_decay for other params except 
+                               bias &amp; norm
+On 384x384 images with LR 3e-4 to 1e-4
+LR*0.1 for presence head
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+BS = 32 (train/valid/test)
+(2h 44m 22s)  
+(Max GPU mem usage : 10900.875 MB)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder 
+with presence head with dropout 0.4
+per class seg loss : 
+dice * 0.1 + lovasz * 0.6 + bce * 0.3
+total_loss = 0.5 * presence_loss + 0.5 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+Presence loss pos_weight = [65/35, 72/28, 79/21]
+On padded images
+With AdamW optim 
+1e-6 weight decay for presence head
+1e-4 weight_decay for other params except 
+                               bias &amp; norm
+On 384x384 images with LR 3e-4 to 1e-4
+LR*0.1 for presence head
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+BS = 32 (train/valid/test)
+(2h 44m 22s)  
+(Max GPU mem usage : 10900.875 MB)   </t>
   </si>
 </sst>
 </file>
@@ -1385,13 +1807,13 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1442,7 +1864,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1515,12 +1937,24 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1706,15 +2140,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K126"/>
+  <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B124" activeCellId="0" sqref="B124"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A143" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A144" activeCellId="0" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.79"/>
@@ -2689,13 +3123,13 @@
       <c r="B124" s="2" t="n">
         <v>0.862</v>
       </c>
-      <c r="C124" s="18" t="n">
+      <c r="C124" s="13" t="n">
         <v>0.85614</v>
       </c>
-      <c r="D124" s="18" t="n">
+      <c r="D124" s="13" t="n">
         <v>0.84691</v>
       </c>
-      <c r="E124" s="19" t="s">
+      <c r="E124" s="11" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2706,10 +3140,10 @@
       <c r="B125" s="2" t="n">
         <v>0.865</v>
       </c>
-      <c r="C125" s="18" t="n">
+      <c r="C125" s="13" t="n">
         <v>0.8544</v>
       </c>
-      <c r="D125" s="18" t="n">
+      <c r="D125" s="13" t="n">
         <v>0.84696</v>
       </c>
     </row>
@@ -2720,11 +3154,244 @@
       <c r="B126" s="2" t="n">
         <v>0.863</v>
       </c>
-      <c r="C126" s="18" t="n">
+      <c r="C126" s="13" t="n">
         <v>0.84032</v>
       </c>
-      <c r="D126" s="18" t="n">
+      <c r="D126" s="13" t="n">
         <v>0.83256</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="471.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B128" s="2" t="n">
+        <v>0.854</v>
+      </c>
+      <c r="C128" s="2" t="n">
+        <v>0.84982</v>
+      </c>
+      <c r="D128" s="2" t="n">
+        <v>0.84779</v>
+      </c>
+      <c r="E128" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B129" s="2" t="n">
+        <v>0.856</v>
+      </c>
+      <c r="C129" s="2" t="n">
+        <v>0.84748</v>
+      </c>
+      <c r="D129" s="2" t="n">
+        <v>0.84537</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="829.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B131" s="2" t="n">
+        <v>0.844</v>
+      </c>
+      <c r="C131" s="2" t="n">
+        <v>0.83786</v>
+      </c>
+      <c r="D131" s="2" t="n">
+        <v>0.82678</v>
+      </c>
+      <c r="E131" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B132" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="C132" s="2" t="n">
+        <v>0.84301</v>
+      </c>
+      <c r="D132" s="2" t="n">
+        <v>0.8331</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="807.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B134" s="2" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="C134" s="2" t="n">
+        <v>0.84801</v>
+      </c>
+      <c r="D134" s="2" t="n">
+        <v>0.83507</v>
+      </c>
+      <c r="E134" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B135" s="2" t="n">
+        <v>0.8578</v>
+      </c>
+      <c r="C135" s="2" t="n">
+        <v>0.85498</v>
+      </c>
+      <c r="D135" s="2" t="n">
+        <v>0.84632</v>
+      </c>
+      <c r="E135" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B136" s="2" t="n">
+        <v>0.8583</v>
+      </c>
+      <c r="C136" s="2" t="n">
+        <v>0.85388</v>
+      </c>
+      <c r="D136" s="2" t="n">
+        <v>0.84591</v>
+      </c>
+      <c r="E136" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="605.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B138" s="2" t="n">
+        <v>0.844</v>
+      </c>
+      <c r="C138" s="2" t="n">
+        <v>0.8473</v>
+      </c>
+      <c r="D138" s="2" t="n">
+        <v>0.83892</v>
+      </c>
+      <c r="E138" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C139" s="2" t="n">
+        <v>0.8471</v>
+      </c>
+      <c r="D139" s="2" t="n">
+        <v>0.84523</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="617.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B141" s="2" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="C141" s="2" t="n">
+        <v>0.83828</v>
+      </c>
+      <c r="D141" s="2" t="n">
+        <v>0.83337</v>
+      </c>
+      <c r="E141" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C142" s="2" t="n">
+        <v>0.84163</v>
+      </c>
+      <c r="D142" s="2" t="n">
+        <v>0.83464</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="382.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B144" s="2" t="n">
+        <v>0.851</v>
+      </c>
+      <c r="C144" s="2" t="n">
+        <v>0.84871</v>
+      </c>
+      <c r="D144" s="2" t="n">
+        <v>0.84165</v>
+      </c>
+      <c r="E144" s="20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B145" s="0"/>
+      <c r="C145" s="2" t="n">
+        <v>0.8539</v>
+      </c>
+      <c r="D145" s="2" t="n">
+        <v>0.84734</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B146" s="2" t="n">
+        <v>0.856</v>
+      </c>
+      <c r="C146" s="2" t="n">
+        <v>0.8489</v>
+      </c>
+      <c r="D146" s="2" t="n">
+        <v>0.84076</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C147" s="2" t="n">
+        <v>0.85249</v>
+      </c>
+      <c r="D147" s="2" t="n">
+        <v>0.84618</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.1LR for presence head, warmup+cosine_decay LR
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="157">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -1735,8 +1735,40 @@
 (used LOAD_RESIZED = False)
 with grad_accu = 2, BS = 32    
 BS = 32 (train/valid/test)
-(2h 44m 22s)  
+(2h 44m 28s)  
 (Max GPU mem usage : 10900.875 MB)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-L TLo-LB-B TLo-SB-D TLo-SB-L TLo-SB-B TLo-S-D  TLo-S-L  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.641      | 0.468      | 0.575           | 0.146        | 0.139             | 0.761    0.522    0.971    0.696    0.242    0.974    0.639    0.267    0.987    0.581    0.243   | 0.313    0.623    0.545    0.476    0.122    0.487    0.409    0.119    0.423    0.335    0.117   | 0.256  0.069  0.072  | 0.117  0.091  0.210 
+2     | 0.000300  | 0.310      | 0.432      | 0.723           | 0.462        | 0.104             | 0.278    0.342    0.897    0.480    0.077    0.920    0.404    0.084    0.954    0.342    0.082   | 0.313    0.551    0.486    0.447    0.042    0.461    0.400    0.065    0.400    0.318    0.043   | 0.549  0.397  0.366  | 0.120  0.107  0.084 
+3     | 0.000300  | 0.224      | 0.364      | 0.793           | 0.592        | 0.073             | 0.169    0.279    0.668    0.384    0.021    0.847    0.375    0.041    0.858    0.283    0.029   | 0.248    0.480    0.328    0.364    0.012    0.415    0.373    0.031    0.311    0.292    0.012   | 0.687  0.477  0.546  | 0.077  0.088  0.053 
+4     | 0.000290  | 0.178      | 0.311      | 0.816           | 0.634        | 0.062             | 0.124    0.231    0.461    0.321    0.010    0.739    0.354    0.023    0.609    0.230    0.009   | 0.192    0.430    0.290    0.345    0.010    0.379    0.354    0.018    0.222    0.245    0.005   | 0.697  0.553  0.631  | 0.065  0.065  0.056 
+5     | 0.000262  | 0.150      | 0.337      | 0.825           | 0.657        | 0.064             | 0.096    0.204    0.384    0.290    0.008    0.638    0.333    0.016    0.418    0.196    0.004   | 0.244    0.431    0.250    0.355    0.008    0.341    0.363    0.015    0.173    0.255    0.003   | 0.711  0.573  0.661  | 0.063  0.075  0.054 
+6     | 0.000222  | 0.130      | 0.312      | 0.832           | 0.673        | 0.062             | 0.076    0.185    0.340    0.268    0.007    0.563    0.310    0.012    0.321    0.173    0.003   | 0.205    0.418    0.217    0.373    0.008    0.304    0.378    0.012    0.159    0.248    0.003   | 0.727  0.601  0.678  | 0.070  0.067  0.048 
+7     | 0.000178  | 0.113      | 0.300      | 0.835           | 0.688        | 0.067             | 0.057    0.168    0.300    0.243    0.006    0.502    0.288    0.010    0.272    0.155    0.003   | 0.199    0.401    0.225    0.350    0.008    0.306    0.374    0.012    0.147    0.222    0.003   | 0.730  0.601  0.715  | 0.072  0.073  0.055 
+8     | 0.000138  | 0.101      | 0.296      | 0.844           | 0.702        | 0.061             | 0.045    0.157    0.278    0.228    0.005    0.468    0.274    0.009    0.245    0.144    0.002   | 0.201    0.392    0.210    0.350    0.007    0.282    0.369    0.011    0.134    0.213    0.003   | 0.739  0.625  0.731  | 0.061  0.065  0.056 
+9     | 0.000110  | 0.093      | 0.297      | 0.845           | 0.702        | 0.060             | 0.037    0.149    0.261    0.217    0.005    0.438    0.262    0.008    0.222    0.135    0.002   | 0.188    0.406    0.208    0.350    0.007    0.277    0.376    0.011    0.130    0.220    0.003   | 0.743  0.616  0.734  | 0.066  0.070  0.045 
+10    | 0.000100  | 0.086      | 0.315      | 0.838           | 0.691        | 0.064             | 0.030    0.142    0.245    0.208    0.005    0.413    0.251    0.008    0.210    0.129    0.002   | 0.225    0.406    0.205    0.379    0.007    0.274    0.402    0.010    0.131    0.221    0.003   | 0.728  0.614  0.727  | 0.072  0.066  0.054
+Confusion Matrix raw counts
+      LB    SB     S
+TP  2512  1982  1451
+FP   252   257   118
+FN    65    87    75
+TN  4467  4970  5652
+Confusion Matrix normalized per class
+       LB     SB      S
+TP  0.344  0.272  0.199
+FP  0.035  0.035  0.016
+FN  0.009  0.012  0.010
+TN  0.612  0.681  0.775
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.315      | 0.838           | 0.691        | 0.064             | 0.225    0.406    0.205    0.379    0.007    0.274    0.402    0.010    0.131    0.221    0.003   | 0.728  0.614  0.727  | 0.072  0.066  0.054 
+266     | 266     | 0.307      | 0.839           | 0.696        | 0.065             | 0.215    0.400    0.195    0.380    0.008    0.267    0.395    0.011    0.111    0.202    0.002   | 0.725  0.619  0.744  | 0.074  0.067  0.055 
+360     | 310     | 0.339      | 0.819           | 0.619        | 0.048             | 0.241    0.436    0.208    0.318    0.003    0.328    0.366    0.007    0.187    0.370    0.003   | 0.720  0.550  0.609  | 0.058  0.052  0.034 
+276     | 276     | 0.527      | 0.848           | 0.710        | 0.059             | 0.471    0.583    0.308    0.492    0.008    0.339    0.661    0.015    0.206    0.347    0.003   | 0.793  0.613  0.670  | 0.059  0.058  0.062 </t>
   </si>
   <si>
     <t xml:space="preserve">Segformer with mit_b1 encoder 
@@ -1759,8 +1791,394 @@
 (used LOAD_RESIZED = False)
 with grad_accu = 2, BS = 32    
 BS = 32 (train/valid/test)
-(2h 44m 22s)  
+(2h 44m 44s)  
 (Max GPU mem usage : 10900.875 MB)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-L TLo-LB-B TLo-SB-D TLo-SB-L TLo-SB-B TLo-S-D  TLo-S-L  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.710      | 0.565      | 0.530           | 0.153        | 0.218             | 0.875    0.546    0.977    0.738    0.264    0.978    0.674    0.280    0.990    0.594    0.253   | 0.461    0.668    0.549    0.504    0.135    0.488    0.425    0.125    0.425    0.386    0.109   | 0.236  0.137  0.039  | 0.188  0.167  0.298 
+2     | 0.000300  | 0.348      | 0.396      | 0.691           | 0.379        | 0.101             | 0.340    0.357    0.923    0.499    0.103    0.929    0.416    0.097    0.960    0.357    0.095   | 0.241    0.551    0.503    0.440    0.055    0.457    0.386    0.062    0.402    0.315    0.047   | 0.528  0.355  0.177  | 0.108  0.128  0.068 
+3     | 0.000300  | 0.246      | 0.343      | 0.784           | 0.573        | 0.075             | 0.198    0.294    0.743    0.410    0.030    0.861    0.382    0.045    0.878    0.297    0.034   | 0.209    0.477    0.356    0.385    0.015    0.428    0.361    0.034    0.322    0.277    0.012   | 0.658  0.489  0.497  | 0.083  0.100  0.042 
+4     | 0.000290  | 0.188      | 0.302      | 0.812           | 0.638        | 0.072             | 0.137    0.240    0.501    0.334    0.011    0.756    0.362    0.025    0.635    0.238    0.010   | 0.174    0.430    0.294    0.362    0.010    0.374    0.364    0.020    0.217    0.235    0.005   | 0.693  0.547  0.651  | 0.084  0.081  0.052 
+5     | 0.000262  | 0.157      | 0.343      | 0.818           | 0.648        | 0.068             | 0.105    0.208    0.402    0.298    0.008    0.645    0.339    0.016    0.429    0.199    0.005   | 0.242    0.444    0.253    0.369    0.008    0.338    0.392    0.016    0.172    0.250    0.004   | 0.704  0.546  0.664  | 0.066  0.087  0.052 
+6     | 0.000222  | 0.135      | 0.305      | 0.835           | 0.674        | 0.057             | 0.084    0.187    0.348    0.270    0.007    0.570    0.314    0.013    0.330    0.178    0.003   | 0.196    0.414    0.233    0.370    0.008    0.311    0.374    0.012    0.154    0.225    0.003   | 0.718  0.593  0.698  | 0.063  0.064  0.045 
+7     | 0.000178  | 0.120      | 0.296      | 0.834           | 0.685        | 0.066             | 0.067    0.173    0.311    0.251    0.006    0.515    0.295    0.011    0.282    0.159    0.003   | 0.196    0.395    0.231    0.354    0.007    0.305    0.371    0.012    0.151    0.217    0.003   | 0.730  0.609  0.709  | 0.066  0.081  0.052 
+8     | 0.000138  | 0.108      | 0.318      | 0.840           | 0.687        | 0.058             | 0.055    0.161    0.289    0.236    0.006    0.475    0.279    0.009    0.250    0.147    0.002   | 0.225    0.410    0.221    0.362    0.007    0.288    0.386    0.011    0.144    0.217    0.003   | 0.723  0.600  0.716  | 0.056  0.065  0.053 
+9     | 0.000110  | 0.098      | 0.293      | 0.846           | 0.698        | 0.056             | 0.043    0.153    0.270    0.223    0.005    0.446    0.268    0.009    0.228    0.138    0.002   | 0.188    0.399    0.212    0.349    0.007    0.277    0.380    0.011    0.126    0.212    0.003   | 0.737  0.612  0.735  | 0.061  0.065  0.041 
+10    | 0.000100  | 0.092      | 0.314      | 0.844           | 0.700        | 0.061             | 0.038    0.146    0.254    0.214    0.005    0.424    0.258    0.008    0.214    0.131    0.002   | 0.225    0.404    0.200    0.383    0.007    0.269    0.401    0.011    0.126    0.213    0.002   | 0.737  0.623  0.733  | 0.066  0.070  0.046
+Confusion Matrix raw counts
+      LB    SB     S
+TP  2529  1962  1472
+FP   225   218   128
+FN    48   107    54
+TN  4494  5009  5642
+Confusion Matrix normalized per class
+       LB     SB      S
+TP  0.347  0.269  0.202
+FP  0.031  0.030  0.018
+FN  0.007  0.015  0.007
+TN  0.616  0.687  0.773 
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.314      | 0.844           | 0.700        | 0.061             | 0.225    0.404    0.200    0.383    0.007    0.269    0.401    0.011    0.126    0.213    0.002   | 0.737  0.623  0.733  | 0.066  0.070  0.046 
+266     | 266     | 0.300      | 0.845           | 0.705        | 0.062             | 0.206    0.395    0.190    0.384    0.008    0.264    0.394    0.011    0.107    0.192    0.002   | 0.734  0.627  0.756  | 0.069  0.070  0.047 
+360     | 310     | 0.376      | 0.814           | 0.619        | 0.057             | 0.320    0.433    0.211    0.326    0.003    0.322    0.386    0.007    0.175    0.347    0.003   | 0.732  0.556  0.568  | 0.056  0.079  0.036 
+276     | 276     | 0.556      | 0.864           | 0.728        | 0.044             | 0.530    0.581    0.311    0.517    0.008    0.331    0.658    0.015    0.194    0.434    0.003   | 0.805  0.644  0.671  | 0.040  0.056  0.038
+Cutoffs(LB,SB,S) | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+(0.00,0.00,0.00) | 0.314      | 0.843511        | 0.700        | 0.061             | 0.225    0.404    0.200    0.383    0.007    0.269    0.401    0.011    0.126    0.213    0.002   | 0.736  0.623  0.738  | 0.066  0.070  0.046 
+(0.25,0.25,0.25) | 0.314      | 0.843310        | 0.699        | 0.061             | 0.225    0.404    0.200    0.383    0.007    0.269    0.401    0.011    0.126    0.213    0.002   | 0.736  0.623  0.735  | 0.066  0.070  0.046 
+(0.50,0.50,0.50) | 0.314      | 0.843621        | 0.700        | 0.061             | 0.225    0.404    0.200    0.383    0.007    0.269    0.401    0.011    0.126    0.213    0.002   | 0.737  0.623  0.733  | 0.066  0.070  0.046 
+(0.75,0.75,0.75) | 0.314      | 0.844040        | 0.701        | 0.060             | 0.225    0.404    0.200    0.383    0.007    0.269    0.401    0.011    0.126    0.213    0.002   | 0.738  0.624  0.733  | 0.066  0.070  0.045 
+(0.60,0.70,0.70) | 0.314      | 0.844033        | 0.701        | 0.060             | 0.225    0.404    0.200    0.383    0.007    0.269    0.401    0.011    0.126    0.213    0.002   | 0.739  0.624  0.732  | 0.066  0.070  0.046 
+(0.60,0.70,0.80) | 0.314      | 0.844293        | 0.701        | 0.060             | 0.225    0.404    0.200    0.383    0.007    0.269    0.401    0.011    0.126    0.213    0.002   | 0.739  0.624  0.733  | 0.066  0.070  0.045 
+(0.50,0.75,0.75) | 0.314      | 0.844014        | 0.701        | 0.060             | 0.225    0.404    0.200    0.383    0.007    0.269    0.401    0.011    0.126    0.213    0.002   | 0.737  0.624  0.733  | 0.066  0.070  0.045 
+(0.6, 0.7, 0.8)
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.314      | 0.844           | 0.701        | 0.060             | 0.225    0.404    0.200    0.383    0.007    0.269    0.401    0.011    0.126    0.213    0.002   | 0.739  0.624  0.733  | 0.066  0.070  0.045 
+266     | 266     | 0.300      | 0.846           | 0.707        | 0.062             | 0.206    0.395    0.190    0.384    0.008    0.264    0.394    0.011    0.107    0.192    0.002   | 0.735  0.628  0.758  | 0.069  0.070  0.046 
+360     | 310     | 0.376      | 0.812           | 0.615        | 0.057             | 0.320    0.433    0.211    0.326    0.003    0.322    0.386    0.007    0.175    0.347    0.003   | 0.732  0.552  0.555  | 0.056  0.079  0.036 
+276     | 276     | 0.556      | 0.866           | 0.732        | 0.044             | 0.530    0.581    0.311    0.517    0.008    0.331    0.658    0.015    0.194    0.434    0.003   | 0.805  0.650  0.671  | 0.040  0.056  0.038  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cutoff (0.60,0.70,0.80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder 
+with presence head with dropout 0.4
+per class seg loss : 
+dice * 0.1 + lovasz * 0.6 + bce * 0.3
+total_loss = 0.5 * presence_loss + 0.5 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+Presence loss pos_weight = [60/40, 70/30, 75/25]
+On padded images
+With AdamW optim 
+1e-6 weight decay for presence head
+1e-4 weight_decay for other params except 
+                               bias &amp; norm
+On 384x384 images with LR 5e-4 to 3e-4
+LR*0.1 for presence head
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+BS = 32 (train/valid/test)
+(2h 49m 36s)  
+(Max GPU mem usage : 10900.875 MB)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-L TLo-LB-B TLo-SB-D TLo-SB-L TLo-SB-B TLo-S-D  TLo-S-L  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000500  | 0.730      | 0.715      | 0.287           | 0.041        | 0.548             | 0.907    0.553    0.980    0.774    0.269    0.981    0.677    0.274    0.991    0.580    0.241   | 0.682    0.748    0.558    0.610    0.264    0.497    0.454    0.234    0.429    0.446    0.200   | 0.049  0.066  0.000  | 0.312  0.333  1.000 
+2     | 0.000500  | 0.462      | 0.463      | 0.538           | 0.143        | 0.199             | 0.510    0.413    0.958    0.558    0.187    0.955    0.462    0.158    0.979    0.442    0.145   | 0.331    0.596    0.540    0.488    0.126    0.478    0.411    0.102    0.419    0.330    0.096   | 0.157  0.171  0.082  | 0.215  0.160  0.224 
+3     | 0.000500  | 0.328      | 0.457      | 0.599           | 0.251        | 0.169             | 0.308    0.347    0.921    0.495    0.096    0.915    0.401    0.079    0.950    0.341    0.076   | 0.331    0.582    0.520    0.472    0.077    0.463    0.394    0.067    0.401    0.358    0.043   | 0.267  0.280  0.159  | 0.192  0.139  0.174 
+4     | 0.000490  | 0.291      | 0.418      | 0.646           | 0.304        | 0.126             | 0.257    0.324    0.881    0.477    0.062    0.878    0.385    0.053    0.921    0.318    0.047   | 0.277    0.559    0.497    0.468    0.047    0.444    0.376    0.044    0.387    0.331    0.029   | 0.352  0.290  0.238  | 0.159  0.118  0.100 
+5     | 0.000462  | 0.262      | 0.421      | 0.664           | 0.363        | 0.136             | 0.214    0.309    0.838    0.460    0.044    0.841    0.373    0.039    0.885    0.305    0.032   | 0.286    0.556    0.491    0.452    0.042    0.441    0.368    0.039    0.391    0.322    0.031   | 0.434  0.329  0.279  | 0.143  0.107  0.157 
+6     | 0.000422  | 0.236      | 0.390      | 0.726           | 0.453        | 0.092             | 0.178    0.294    0.771    0.435    0.030    0.809    0.367    0.032    0.846    0.298    0.023   | 0.247    0.534    0.427    0.435    0.023    0.422    0.378    0.030    0.363    0.333    0.018   | 0.553  0.391  0.346  | 0.089  0.093  0.095 
+7     | 0.000378  | 0.205      | 0.395      | 0.774           | 0.546        | 0.075             | 0.145    0.266    0.575    0.385    0.014    0.769    0.365    0.025    0.723    0.282    0.013   | 0.280    0.511    0.319    0.404    0.011    0.399    0.385    0.021    0.275    0.333    0.007   | 0.640  0.453  0.472  | 0.084  0.074  0.066 
+8     | 0.000338  | 0.177      | 0.356      | 0.795           | 0.600        | 0.076             | 0.121    0.234    0.454    0.336    0.010    0.717    0.357    0.020    0.514    0.243    0.006   | 0.239    0.472    0.280    0.405    0.010    0.365    0.384    0.016    0.217    0.277    0.005   | 0.662  0.508  0.585  | 0.082  0.077  0.067 
+9     | 0.000310  | 0.155      | 0.314      | 0.809           | 0.631        | 0.073             | 0.101    0.210    0.393    0.305    0.008    0.630    0.343    0.015    0.382    0.206    0.004   | 0.184    0.444    0.263    0.377    0.010    0.346    0.384    0.015    0.178    0.248    0.004   | 0.684  0.530  0.643  | 0.083  0.082  0.054 
+10    | 0.000300  | 0.142      | 0.335      | 0.809           | 0.628        | 0.070             | 0.089    0.196    0.361    0.285    0.007    0.576    0.327    0.013    0.330    0.190    0.003   | 0.218    0.451    0.270    0.383    0.009    0.340    0.387    0.014    0.177    0.252    0.004   | 0.671  0.535  0.645  | 0.076  0.066  0.068
+Confusion Matrix raw counts
+      LB    SB     S
+TP  2301  1790  1354
+FP   102   125   129
+FN   276   279   172
+TN  4617  5102  5641
+Confusion Matrix normalized per class
+       LB     SB      S
+TP  0.315  0.245  0.186
+FP  0.014  0.017  0.018
+FN  0.038  0.038  0.024
+TN  0.633  0.699  0.773
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-L VLo-LB-B VLo-SB-D VLo-SB-L VLo-SB-B VLo-S-D  VLo-S-L  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+-------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.335      | 0.809           | 0.628        | 0.070             | 0.218    0.451    0.270    0.383    0.009    0.340    0.387    0.014    0.177    0.252    0.004   | 0.671  0.535  0.645  | 0.076  0.066  0.068 
+266     | 266     | 0.322      | 0.810           | 0.630        | 0.070             | 0.205    0.439    0.257    0.382    0.009    0.335    0.385    0.014    0.154    0.227    0.004   | 0.666  0.532  0.671  | 0.075  0.066  0.069 
+360     | 310     | 0.392      | 0.796           | 0.575        | 0.056             | 0.326    0.457    0.287    0.323    0.005    0.367    0.327    0.008    0.246    0.426    0.004   | 0.675  0.521  0.462  | 0.064  0.068  0.037 
+276     | 276     | 0.450      | 0.814           | 0.655        | 0.080             | 0.297    0.604    0.421    0.523    0.011    0.416    0.540    0.018    0.295    0.465    0.005   | 0.742  0.610  0.566  | 0.102  0.050  0.089 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segformer with mit_b1 encoder 
+with presence head with dropout 0.4
+per class seg loss : 
+dice * 0.25 +  bce * 0.75
+total_loss = 0.25 * presence_loss + 0.75 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+Presence loss pos_weight = [60/40, 70/30, 75/25]
+On padded images
+With AdamW optim 
+1e-6 weight decay for presence head
+1e-4 weight_decay for other params except 
+                               bias &amp; norm
+On 384x384 images with LR 3e-4 to 1e-4
+LR*0.25 for presence head
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+BS = 32 (train/valid/test)
+(2h 35m 29s)  
+(Max GPU mem usage : 10716.875 MB)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-B TLo-SB-D TLo-SB-B TLo-S-D  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000300  | 0.209      | 0.110      | 0.788           | 0.605        | 0.089             | 0.263    0.192    0.543    0.043    0.745    0.084    0.742    0.078   | 0.164    0.093    0.207    0.012    0.272    0.017    0.167    0.007   | 0.669  0.521  0.601  | 0.089  0.088  0.091 
+2     | 0.000300  | 0.078      | 0.099      | 0.824           | 0.664        | 0.069             | 0.113    0.067    0.222    0.009    0.372    0.013    0.234    0.004   | 0.176    0.073    0.166    0.014    0.218    0.020    0.104    0.004   | 0.703  0.576  0.723  | 0.082  0.070  0.054 
+3     | 0.000300  | 0.062      | 0.095      | 0.832           | 0.678        | 0.066             | 0.087    0.054    0.185    0.008    0.302    0.012    0.165    0.004   | 0.169    0.071    0.163    0.015    0.208    0.018    0.090    0.005   | 0.705  0.592  0.747  | 0.082  0.066  0.049 
+4     | 0.000290  | 0.053      | 0.095      | 0.834           | 0.676        | 0.061             | 0.066    0.048    0.165    0.008    0.269    0.011    0.142    0.003   | 0.179    0.067    0.150    0.014    0.199    0.020    0.088    0.004   | 0.708  0.589  0.748  | 0.069  0.066  0.047 
+5     | 0.000262  | 0.047      | 0.103      | 0.844           | 0.682        | 0.049             | 0.056    0.044    0.153    0.007    0.247    0.010    0.129    0.003   | 0.193    0.074    0.170    0.015    0.221    0.020    0.086    0.004   | 0.707  0.588  0.755  | 0.054  0.058  0.034 
+6     | 0.000222  | 0.042      | 0.107      | 0.842           | 0.689        | 0.055             | 0.046    0.041    0.140    0.006    0.227    0.009    0.116    0.003   | 0.216    0.070    0.155    0.015    0.203    0.019    0.091    0.005   | 0.723  0.611  0.737  | 0.053  0.066  0.047 
+7     | 0.000178  | 0.037      | 0.094      | 0.847           | 0.708        | 0.060             | 0.036    0.038    0.129    0.006    0.212    0.009    0.109    0.003   | 0.178    0.066    0.147    0.014    0.196    0.019    0.077    0.004   | 0.736  0.617  0.773  | 0.071  0.072  0.036 
+8     | 0.000138  | 0.034      | 0.102      | 0.846           | 0.702        | 0.058             | 0.028    0.036    0.121    0.006    0.199    0.008    0.103    0.003   | 0.206    0.067    0.145    0.015    0.197    0.020    0.082    0.004   | 0.731  0.611  0.766  | 0.061  0.066  0.048 
+9     | 0.000110  | 0.030      | 0.100      | 0.851           | 0.713        | 0.057             | 0.020    0.034    0.115    0.005    0.188    0.008    0.098    0.002   | 0.204    0.065    0.143    0.015    0.191    0.020    0.082    0.004   | 0.739  0.628  0.768  | 0.058  0.072  0.040 
+10    | 0.000100  | 0.029      | 0.105      | 0.850           | 0.711        | 0.057             | 0.018    0.033    0.111    0.005    0.183    0.008    0.094    0.002   | 0.227    0.065    0.139    0.015    0.186    0.020    0.084    0.004   | 0.737  0.627  0.764  | 0.066  0.070  0.036
+Confusion Matrix raw counts
+      LB    SB     S
+TP  2507  1915  1463
+FP   231   223    90
+FN    70   154    63
+TN  4488  5004  5680
+Confusion Matrix normalized per class
+       LB     SB      S
+TP  0.344  0.262  0.201
+FP  0.032  0.031  0.012
+FN  0.010  0.021  0.009
+TN  0.615  0.686  0.779
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.105      | 0.850           | 0.711        | 0.057             | 0.227    0.065    0.139    0.015    0.186    0.020    0.084    0.004   | 0.737  0.627  0.764  | 0.066  0.070  0.036 
+266     | 266     | 0.104      | 0.850           | 0.714        | 0.059             | 0.219    0.066    0.139    0.016    0.188    0.020    0.072    0.004   | 0.735  0.631  0.772  | 0.067  0.073  0.037 
+360     | 310     | 0.101      | 0.837           | 0.663        | 0.047             | 0.222    0.061    0.113    0.005    0.218    0.010    0.102    0.004   | 0.719  0.541  0.724  | 0.059  0.048  0.034 
+276     | 276     | 0.175      | 0.870           | 0.742        | 0.045             | 0.470    0.077    0.179    0.013    0.205    0.026    0.105    0.005   | 0.807  0.658  0.708  | 0.055  0.047  0.032 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">warmup&amp;cosdec,0.1LR pres,DL Lo(.5),.25PLo+.75SLo
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Segformer with mit_b1 encoder 
+with presence head with dropout 0.4
+per class seg loss : 
+dice * 0.5 +  bce * 0.5
+total_loss = 0.25 * presence_loss + 0.75 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+Presence loss pos_weight = [60/40, 70/30, 75/25]
+On padded images
+With AdamW optim 
+1e-6 weight decay for presence head
+1e-4 weight_decay for other params except 
+                               bias &amp; norm
+On 384x384 images with 
+LR 1.25e-4, 2.5e-4, 5e-4, cos decay to 3e-4
+LR*0.1 for presence head
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+BS = 32 (train/valid/test)
+(2h 31m 39s)  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Max GPU mem usage : 10716.875 MB)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-B TLo-SB-D TLo-SB-B TLo-S-D  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000125  | 0.355      | 0.195      | 0.793           | 0.589        | 0.071             | 0.214    0.402    0.637    0.072    0.857    0.157    0.909    0.161   | 0.173    0.203    0.224    0.014    0.324    0.026    0.257    0.013   | 0.678  0.493  0.550  | 0.068  0.085  0.060 
+2     | 0.000250  | 0.132      | 0.126      | 0.838           | 0.677        | 0.055             | 0.121    0.136    0.228    0.010    0.393    0.015    0.287    0.006   | 0.141    0.121    0.156    0.015    0.210    0.021    0.100    0.005   | 0.718  0.587  0.718  | 0.066  0.057  0.042 
+3     | 0.000500  | 0.105      | 0.136      | 0.832           | 0.672        | 0.062             | 0.115    0.102    0.188    0.011    0.299    0.015    0.169    0.004   | 0.200    0.115    0.148    0.017    0.206    0.027    0.085    0.005   | 0.718  0.585  0.718  | 0.065  0.062  0.059 
+4     | 0.000490  | 0.089      | 0.116      | 0.841           | 0.692        | 0.060             | 0.091    0.088    0.164    0.010    0.263    0.014    0.136    0.004   | 0.136    0.109    0.146    0.016    0.192    0.025    0.084    0.005   | 0.728  0.612  0.747  | 0.067  0.066  0.048 
+5     | 0.000462  | 0.075      | 0.133      | 0.838           | 0.689        | 0.063             | 0.067    0.078    0.144    0.009    0.232    0.013    0.121    0.004   | 0.186    0.115    0.154    0.018    0.198    0.023    0.091    0.005   | 0.716  0.608  0.732  | 0.074  0.066  0.050 
+6     | 0.000422  | 0.071      | 0.121      | 0.850           | 0.699        | 0.050             | 0.061    0.074    0.137    0.008    0.220    0.012    0.113    0.004   | 0.149    0.111    0.152    0.017    0.191    0.023    0.087    0.005   | 0.718  0.630  0.755  | 0.051  0.061  0.037 
+7     | 0.000378  | 0.064      | 0.112      | 0.855           | 0.712        | 0.050             | 0.051    0.068    0.127    0.008    0.202    0.011    0.103    0.003   | 0.134    0.105    0.144    0.017    0.186    0.022    0.085    0.005   | 0.744  0.631  0.764  | 0.061  0.058  0.032 
+8     | 0.000338  | 0.059      | 0.125      | 0.852           | 0.709        | 0.053             | 0.042    0.064    0.118    0.007    0.191    0.011    0.098    0.003   | 0.177    0.107    0.141    0.017    0.187    0.024    0.085    0.005   | 0.737  0.629  0.747  | 0.060  0.058  0.041 
+9     | 0.000310  | 0.054      | 0.117      | 0.857           | 0.718        | 0.049             | 0.034    0.061    0.112    0.007    0.181    0.010    0.094    0.003   | 0.153    0.104    0.138    0.017    0.183    0.023    0.081    0.005   | 0.746  0.642  0.764  | 0.060  0.057  0.031 
+10    | 0.000300  | 0.055      | 0.112      | 0.853           | 0.721        | 0.058             | 0.038    0.061    0.113    0.007    0.179    0.010    0.095    0.003   | 0.151    0.099    0.135    0.016    0.176    0.023    0.075    0.005   | 0.746  0.646  0.773  | 0.062  0.079  0.033 
+Confusion Matrix raw counts
+      LB    SB     S
+TP  2525  1977  1465
+FP   255   267    93
+FN    52    92    61
+TN  4464  4960  5677
+Confusion Matrix normalized per class
+       LB     SB      S
+TP  0.346  0.271  0.201
+FP  0.035  0.037  0.013
+FN  0.007  0.013  0.008
+TN  0.612  0.680  0.778
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.112      | 0.853           | 0.721        | 0.058             | 0.151    0.099    0.135    0.016    0.176    0.023    0.075    0.005   | 0.746  0.646  0.773  | 0.062  0.079  0.033 
+266     | 266     | 0.111      | 0.853           | 0.722        | 0.060             | 0.145    0.099    0.132    0.017    0.173    0.024    0.064    0.005   | 0.741  0.650  0.782  | 0.064  0.083  0.033 
+360     | 310     | 0.120      | 0.840           | 0.672        | 0.048             | 0.178    0.101    0.108    0.006    0.191    0.012    0.087    0.004   | 0.740  0.563  0.732  | 0.052  0.058  0.035 
+276     | 276     | 0.158      | 0.882           | 0.764        | 0.039             | 0.255    0.125    0.162    0.014    0.191    0.033    0.104    0.007   | 0.831  0.678  0.711  | 0.038  0.048  0.031 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">warmup&amp;cosdec,0.075LR pres,DL Lo(.5),.25PLo+.75SLo
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Segformer with mit_b1 encoder 
+with presence head with dropout 0.4
+per class seg loss : 
+dice * 0.5 +  bce * 0.5
+total_loss = 0.25 * presence_loss + 0.75 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+Presence loss pos_weight = [60/40, 70/30, 75/25]
+On padded images
+With AdamW optim 
+1e-6 weight decay for presence head
+1e-4 weight_decay for other params except 
+                               bias &amp; norm
+On 384x384 images with 
+LR 1.25e-4, 2.5e-4, 5e-4, cos decay to 3e-4
+LR*0.075 for presence head
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+BS = 32 (train/valid/test)
+(2h 32m 10s)  
+(Max GPU mem usage : 10716.875 MB)   
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-B TLo-SB-D TLo-SB-B TLo-S-D  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000125  | 0.354      | 0.197      | 0.791           | 0.579        | 0.068             | 0.214    0.401    0.637    0.072    0.855    0.157    0.905    0.161   | 0.179    0.203    0.230    0.013    0.322    0.026    0.255    0.013   | 0.668  0.493  0.540  | 0.071  0.077  0.055 
+2     | 0.000250  | 0.131      | 0.129      | 0.832           | 0.665        | 0.056             | 0.121    0.135    0.228    0.010    0.390    0.015    0.283    0.005   | 0.144    0.124    0.158    0.016    0.215    0.021    0.106    0.005   | 0.709  0.583  0.693  | 0.068  0.052  0.049 
+3     | 0.000500  | 0.106      | 0.129      | 0.831           | 0.672        | 0.062             | 0.115    0.104    0.190    0.011    0.306    0.015    0.172    0.004   | 0.174    0.115    0.150    0.018    0.201    0.024    0.088    0.005   | 0.708  0.596  0.724  | 0.070  0.062  0.055 
+4     | 0.000490  | 0.086      | 0.113      | 0.843           | 0.704        | 0.064             | 0.084    0.086    0.160    0.010    0.258    0.014    0.133    0.004   | 0.129    0.108    0.142    0.015    0.194    0.022    0.085    0.005   | 0.735  0.615  0.754  | 0.067  0.068  0.057 
+5     | 0.000462  | 0.075      | 0.126      | 0.852           | 0.703        | 0.049             | 0.069    0.078    0.144    0.009    0.232    0.013    0.119    0.004   | 0.165    0.113    0.146    0.018    0.199    0.024    0.086    0.005   | 0.730  0.611  0.759  | 0.060  0.055  0.031 
+6     | 0.000422  | 0.069      | 0.130      | 0.852           | 0.705        | 0.049             | 0.057    0.073    0.135    0.008    0.218    0.012    0.109    0.003   | 0.190    0.111    0.148    0.020    0.187    0.023    0.080    0.005   | 0.721  0.627  0.763  | 0.065  0.052  0.031 
+7     | 0.000378  | 0.065      | 0.118      | 0.846           | 0.711        | 0.063             | 0.051    0.069    0.127    0.008    0.205    0.011    0.107    0.003   | 0.149    0.108    0.148    0.017    0.189    0.021    0.084    0.005   | 0.735  0.631  0.769  | 0.067  0.077  0.046 
+8     | 0.000338  | 0.059      | 0.118      | 0.852           | 0.712        | 0.054             | 0.044    0.065    0.120    0.007    0.192    0.011    0.098    0.003   | 0.155    0.105    0.141    0.016    0.183    0.022    0.080    0.006   | 0.744  0.632  0.757  | 0.057  0.057  0.048 
+9     | 0.000310  | 0.056      | 0.123      | 0.852           | 0.709        | 0.053             | 0.037    0.062    0.114    0.007    0.184    0.010    0.095    0.003   | 0.168    0.108    0.143    0.019    0.190    0.024    0.084    0.005   | 0.735  0.626  0.757  | 0.070  0.054  0.037 
+10    | 0.000300  | 0.054      | 0.122      | 0.857           | 0.724        | 0.055             | 0.034    0.060    0.110    0.007    0.178    0.010    0.093    0.003   | 0.180    0.102    0.140    0.018    0.177    0.024    0.072    0.005   | 0.743  0.646  0.789  | 0.062  0.068  0.034
+Confusion Matrix raw counts
+      LB    SB     S
+TP  2487  1944  1479
+FP   195   213    77
+FN    90   125    47
+TN  4524  5014  5693
+Confusion Matrix normalized per class
+       LB     SB      S
+TP  0.341  0.266  0.203
+FP  0.027  0.029  0.011
+FN  0.012  0.017  0.006
+TN  0.620  0.687  0.780
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.122      | 0.857           | 0.724        | 0.055             | 0.180    0.102    0.140    0.018    0.177    0.024    0.072    0.005   | 0.743  0.646  0.789  | 0.062  0.068  0.034 
+266     | 266     | 0.120      | 0.856           | 0.725        | 0.056             | 0.172    0.102    0.140    0.019    0.177    0.025    0.061    0.005   | 0.738  0.650  0.796  | 0.064  0.071  0.034 
+360     | 310     | 0.124      | 0.851           | 0.691        | 0.043             | 0.203    0.098    0.105    0.006    0.190    0.012    0.081    0.004   | 0.748  0.582  0.769  | 0.055  0.052  0.022 
+276     | 276     | 0.194      | 0.869           | 0.743        | 0.047             | 0.374    0.134    0.182    0.017    0.199    0.036    0.099    0.007   | 0.808  0.657  0.701  | 0.043  0.049  0.049 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">warmup3e-4_1e-4,0.1LR pres,DL Lo(.5),.25PLo+.75SLo
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Segformer with mit_b1 encoder 
+with presence head with dropout 0.4
+per class seg loss : 
+dice * 0.5 +  bce * 0.5
+total_loss = 0.25 * presence_loss + 0.75 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+Presence loss pos_weight = [60/40, 70/30, 75/25]
+On padded images
+With AdamW optim 
+1e-5 weight decay for presence head
+1e-4 weight_decay for other params except 
+                               bias &amp; norm
+On 384x384 images with 
+LR 0.75e-4, 1.5e-4, 3e-4, cos decay to 1e-4
+LR*0.1 for presence head
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+BS = 32 (train/valid/test)
+(2h 31m 39s)  
+(Max GPU mem usage : 10716.875 MB)   </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1770,7 +2188,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1806,14 +2224,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1864,7 +2288,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1933,7 +2357,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1945,16 +2369,32 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2140,15 +2580,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K154"/>
+  <dimension ref="A1:K176"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A143" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A144" activeCellId="0" sqref="A144"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A168" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B168" activeCellId="0" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="50.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.79"/>
@@ -3330,7 +3770,7 @@
         <v>0.83464</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="382.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="583.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="8" t="s">
         <v>139</v>
       </c>
@@ -3343,15 +3783,15 @@
       <c r="D144" s="2" t="n">
         <v>0.84165</v>
       </c>
-      <c r="E144" s="20" t="s">
+      <c r="E144" s="11" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="21" t="s">
+      <c r="A145" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="B145" s="0"/>
+      <c r="B145" s="21"/>
       <c r="C145" s="2" t="n">
         <v>0.8539</v>
       </c>
@@ -3384,14 +3824,246 @@
         <v>0.84618</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="22" t="s">
+    <row r="149" customFormat="false" ht="561.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="8" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="154" customFormat="false" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="22" t="s">
+      <c r="B149" s="2" t="n">
+        <v>0.838</v>
+      </c>
+      <c r="C149" s="2" t="n">
+        <v>0.84362</v>
+      </c>
+      <c r="D149" s="2" t="n">
+        <v>0.82896</v>
+      </c>
+      <c r="E149" s="11" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B150" s="2" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="C150" s="2" t="n">
+        <v>0.83386</v>
+      </c>
+      <c r="D150" s="2" t="n">
+        <v>0.82113</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C151" s="2" t="n">
+        <v>0.84275</v>
+      </c>
+      <c r="D151" s="2" t="n">
+        <v>0.83262</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C152" s="2" t="n">
+        <v>0.83916</v>
+      </c>
+      <c r="D152" s="2" t="n">
+        <v>0.83038</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="941.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B154" s="2" t="n">
+        <v>0.844</v>
+      </c>
+      <c r="C154" s="2" t="n">
+        <v>0.84525</v>
+      </c>
+      <c r="D154" s="2" t="n">
+        <v>0.83194</v>
+      </c>
+      <c r="E154" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B155" s="23" t="n">
+        <v>0.844293</v>
+      </c>
+      <c r="C155" s="21" t="n">
+        <v>0.84543</v>
+      </c>
+      <c r="D155" s="21" t="n">
+        <v>0.83166</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B156" s="2" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="C156" s="2" t="n">
+        <v>0.83671</v>
+      </c>
+      <c r="D156" s="2" t="n">
+        <v>0.82417</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C157" s="2" t="n">
+        <v>0.84467</v>
+      </c>
+      <c r="D157" s="2" t="n">
+        <v>0.83178</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C158" s="2" t="n">
+        <v>0.84101</v>
+      </c>
+      <c r="D158" s="2" t="n">
+        <v>0.82906</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="3"/>
+      <c r="B159" s="21"/>
+      <c r="C159" s="21"/>
+      <c r="D159" s="21"/>
+    </row>
+    <row r="160" customFormat="false" ht="572.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B160" s="21"/>
+      <c r="C160" s="21"/>
+      <c r="D160" s="21"/>
+      <c r="E160" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="561.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B163" s="2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E163" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B164" s="2" t="n">
+        <v>0.851</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="370.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B168" s="2" t="n">
+        <v>0.853</v>
+      </c>
+      <c r="C168" s="2" t="n">
+        <v>0.85246</v>
+      </c>
+      <c r="D168" s="2" t="n">
+        <v>0.8448</v>
+      </c>
+      <c r="E168" s="25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B169" s="2" t="n">
+        <v>0.857</v>
+      </c>
+      <c r="C169" s="2" t="n">
+        <v>0.84705</v>
+      </c>
+      <c r="D169" s="2" t="n">
+        <v>0.83892</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C170" s="26" t="n">
+        <v>0.85845</v>
+      </c>
+      <c r="D170" s="2" t="n">
+        <v>0.8503</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C171" s="2" t="n">
+        <v>0.85755</v>
+      </c>
+      <c r="D171" s="2" t="n">
+        <v>0.84951</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="370.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B173" s="2" t="n">
+        <v>0.857</v>
+      </c>
+      <c r="C173" s="2" t="n">
+        <v>0.84931</v>
+      </c>
+      <c r="D173" s="2" t="n">
+        <v>0.84376</v>
+      </c>
+      <c r="E173" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C174" s="2" t="n">
+        <v>0.8578</v>
+      </c>
+      <c r="D174" s="2" t="n">
+        <v>0.85129</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="24" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
included score for run with LR 3e-4_1e-4
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="158">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -1965,6 +1965,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">warmup&amp;cosdec,0.1LR pres,DL Lo(.5),.25PLo+.75SLo
 </t>
@@ -1999,24 +2000,7 @@
 with grad_accu = 2, BS = 32    
 BS = 32 (train/valid/test)
 (2h 31m 39s)  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Max GPU mem usage : 10716.875 MB)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
+(Max GPU mem usage : 10716.875 MB)   </t>
     </r>
   </si>
   <si>
@@ -2071,15 +2055,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Segformer with mit_b1 encoder 
+Segformer with mit_b1 encoder 
 with presence head with dropout 0.4
 per class seg loss : 
 dice * 0.5 +  bce * 0.5
@@ -2144,6 +2120,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">warmup3e-4_1e-4,0.1LR pres,DL Lo(.5),.25PLo+.75SLo
 </t>
@@ -2153,6 +2130,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
 Segformer with mit_b1 encoder 
@@ -2176,9 +2154,41 @@
 (used LOAD_RESIZED = False)
 with grad_accu = 2, BS = 32    
 BS = 32 (train/valid/test)
-(2h 31m 39s)  
+(2h 34m 13s)  
 (Max GPU mem usage : 10716.875 MB)   </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-B TLo-SB-D TLo-SB-B TLo-S-D  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000075  | 0.405      | 0.266      | 0.746           | 0.489        | 0.083             | 0.215    0.468    0.776    0.104    0.925    0.223    0.962    0.232   | 0.184    0.294    0.297    0.016    0.408    0.060    0.371    0.061   | 0.632  0.393  0.394  | 0.078  0.076  0.096 
+2     | 0.000150  | 0.176      | 0.146      | 0.823           | 0.648        | 0.060             | 0.120    0.195    0.289    0.011    0.538    0.023    0.512    0.016   | 0.184    0.133    0.174    0.015    0.231    0.022    0.124    0.005   | 0.699  0.562  0.676  | 0.067  0.062  0.052 
+3     | 0.000300  | 0.108      | 0.141      | 0.815           | 0.643        | 0.069             | 0.109    0.108    0.195    0.010    0.320    0.014    0.190    0.004   | 0.207    0.119    0.166    0.019    0.211    0.024    0.088    0.005   | 0.674  0.551  0.731  | 0.087  0.067  0.055 
+4     | 0.000290  | 0.084      | 0.111      | 0.845           | 0.698        | 0.058             | 0.078    0.087    0.161    0.009    0.261    0.013    0.135    0.003   | 0.123    0.107    0.150    0.015    0.193    0.020    0.083    0.004   | 0.733  0.617  0.761  | 0.062  0.067  0.044 
+5     | 0.000262  | 0.072      | 0.135      | 0.846           | 0.693        | 0.052             | 0.058    0.077    0.142    0.008    0.229    0.011    0.119    0.003   | 0.200    0.113    0.154    0.016    0.205    0.021    0.084    0.004   | 0.717  0.604  0.759  | 0.055  0.059  0.042 
+6     | 0.000222  | 0.064      | 0.136      | 0.848           | 0.700        | 0.054             | 0.048    0.070    0.129    0.007    0.208    0.011    0.106    0.003   | 0.191    0.117    0.154    0.018    0.203    0.024    0.085    0.005   | 0.723  0.616  0.756  | 0.062  0.054  0.045 
+7     | 0.000178  | 0.058      | 0.114      | 0.847           | 0.715        | 0.065             | 0.037    0.065    0.119    0.007    0.193    0.010    0.101    0.003   | 0.145    0.104    0.140    0.016    0.186    0.021    0.079    0.004   | 0.743  0.631  0.776  | 0.082  0.062  0.051 
+8     | 0.000138  | 0.053      | 0.125      | 0.853           | 0.716        | 0.056             | 0.029    0.061    0.112    0.006    0.181    0.009    0.094    0.003   | 0.189    0.104    0.138    0.017    0.187    0.024    0.077    0.004   | 0.740  0.635  0.769  | 0.067  0.060  0.042 
+9     | 0.000110  | 0.048      | 0.123      | 0.857           | 0.724        | 0.054             | 0.021    0.057    0.105    0.006    0.170    0.009    0.090    0.003   | 0.186    0.102    0.137    0.017    0.182    0.023    0.073    0.004   | 0.746  0.644  0.779  | 0.059  0.061  0.040 
+10    | 0.000100  | 0.047      | 0.128      | 0.852           | 0.717        | 0.058             | 0.021    0.055    0.101    0.006    0.165    0.009    0.086    0.003   | 0.201    0.104    0.136    0.018    0.181    0.025    0.075    0.004   | 0.742  0.640  0.769  | 0.074  0.058  0.041
+Confusion Matrix raw counts
+      LB    SB     S
+TP  2491  1941  1467
+FP   208   206   104
+FN    86   128    59
+TN  4511  5021  5666
+Confusion Matrix normalized per class
+       LB     SB      S
+TP  0.341  0.266  0.201
+FP  0.029  0.028  0.014
+FN  0.012  0.018  0.008
+TN  0.618  0.688  0.777
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.128      | 0.852           | 0.717        | 0.058             | 0.201    0.104    0.136    0.018    0.181    0.025    0.075    0.004   | 0.742  0.640  0.769  | 0.074  0.058  0.041 
+266     | 266     | 0.125      | 0.852           | 0.719        | 0.059             | 0.189    0.104    0.133    0.019    0.179    0.026    0.064    0.004   | 0.740  0.644  0.777  | 0.077  0.060  0.041 
+360     | 310     | 0.138      | 0.839           | 0.672        | 0.049             | 0.249    0.101    0.112    0.007    0.188    0.013    0.084    0.003   | 0.706  0.578  0.744  | 0.063  0.046  0.036 
+276     | 276     | 0.205      | 0.871           | 0.743        | 0.044             | 0.426    0.132    0.175    0.017    0.197    0.033    0.106    0.006   | 0.825  0.672  0.674  | 0.040  0.044  0.048 </t>
   </si>
 </sst>
 </file>
@@ -2188,7 +2198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2222,22 +2232,6 @@
       <name val="Courier New"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2288,7 +2282,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2357,10 +2351,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2383,14 +2373,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -2580,10 +2562,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K176"/>
+  <dimension ref="A1:K179"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A168" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B168" activeCellId="0" sqref="B168"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A176" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A176" activeCellId="0" sqref="A176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3270,7 +3252,7 @@
       <c r="B94" s="2" t="n">
         <v>0.856</v>
       </c>
-      <c r="C94" s="17" t="n">
+      <c r="C94" s="2" t="n">
         <v>0.85739</v>
       </c>
       <c r="D94" s="2" t="n">
@@ -3681,7 +3663,7 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="18" t="s">
+      <c r="A135" s="17" t="s">
         <v>130</v>
       </c>
       <c r="B135" s="2" t="n">
@@ -3698,7 +3680,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="18" t="s">
+      <c r="A136" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B136" s="2" t="n">
@@ -3732,7 +3714,7 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="19" t="s">
+      <c r="A139" s="18" t="s">
         <v>136</v>
       </c>
       <c r="C139" s="2" t="n">
@@ -3760,7 +3742,7 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="19" t="s">
+      <c r="A142" s="18" t="s">
         <v>136</v>
       </c>
       <c r="C142" s="2" t="n">
@@ -3788,10 +3770,10 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="20" t="s">
+      <c r="A145" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B145" s="21"/>
+      <c r="B145" s="20"/>
       <c r="C145" s="2" t="n">
         <v>0.8539</v>
       </c>
@@ -3800,7 +3782,7 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="18" t="s">
+      <c r="A146" s="17" t="s">
         <v>141</v>
       </c>
       <c r="B146" s="2" t="n">
@@ -3814,7 +3796,7 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="18" t="s">
+      <c r="A147" s="17" t="s">
         <v>142</v>
       </c>
       <c r="C147" s="2" t="n">
@@ -3842,7 +3824,7 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="18" t="s">
+      <c r="A150" s="17" t="s">
         <v>141</v>
       </c>
       <c r="B150" s="2" t="n">
@@ -3856,7 +3838,7 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="18" t="s">
+      <c r="A151" s="17" t="s">
         <v>136</v>
       </c>
       <c r="C151" s="2" t="n">
@@ -3867,7 +3849,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="18" t="s">
+      <c r="A152" s="17" t="s">
         <v>142</v>
       </c>
       <c r="C152" s="2" t="n">
@@ -3895,21 +3877,21 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="22" t="s">
+      <c r="A155" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="B155" s="23" t="n">
+      <c r="B155" s="22" t="n">
         <v>0.844293</v>
       </c>
-      <c r="C155" s="21" t="n">
+      <c r="C155" s="20" t="n">
         <v>0.84543</v>
       </c>
-      <c r="D155" s="21" t="n">
+      <c r="D155" s="20" t="n">
         <v>0.83166</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="18" t="s">
+      <c r="A156" s="17" t="s">
         <v>141</v>
       </c>
       <c r="B156" s="2" t="n">
@@ -3923,7 +3905,7 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="18" t="s">
+      <c r="A157" s="17" t="s">
         <v>136</v>
       </c>
       <c r="C157" s="2" t="n">
@@ -3934,7 +3916,7 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="18" t="s">
+      <c r="A158" s="17" t="s">
         <v>142</v>
       </c>
       <c r="C158" s="2" t="n">
@@ -3946,17 +3928,17 @@
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="3"/>
-      <c r="B159" s="21"/>
-      <c r="C159" s="21"/>
-      <c r="D159" s="21"/>
+      <c r="B159" s="20"/>
+      <c r="C159" s="20"/>
+      <c r="D159" s="20"/>
     </row>
     <row r="160" customFormat="false" ht="572.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B160" s="21"/>
-      <c r="C160" s="21"/>
-      <c r="D160" s="21"/>
+      <c r="B160" s="20"/>
+      <c r="C160" s="20"/>
+      <c r="D160" s="20"/>
       <c r="E160" s="11" t="s">
         <v>149</v>
       </c>
@@ -3973,15 +3955,15 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="18" t="s">
+      <c r="A164" s="17" t="s">
         <v>141</v>
       </c>
       <c r="B164" s="2" t="n">
         <v>0.851</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="370.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="24" t="s">
+    <row r="168" customFormat="false" ht="572.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="10" t="s">
         <v>152</v>
       </c>
       <c r="B168" s="2" t="n">
@@ -3993,12 +3975,12 @@
       <c r="D168" s="2" t="n">
         <v>0.8448</v>
       </c>
-      <c r="E168" s="25" t="s">
+      <c r="E168" s="11" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="18" t="s">
+      <c r="A169" s="17" t="s">
         <v>141</v>
       </c>
       <c r="B169" s="2" t="n">
@@ -4012,10 +3994,10 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="18" t="s">
+      <c r="A170" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="C170" s="26" t="n">
+      <c r="C170" s="23" t="n">
         <v>0.85845</v>
       </c>
       <c r="D170" s="2" t="n">
@@ -4023,7 +4005,7 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="18" t="s">
+      <c r="A171" s="17" t="s">
         <v>142</v>
       </c>
       <c r="C171" s="2" t="n">
@@ -4033,7 +4015,7 @@
         <v>0.84951</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="370.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="572.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="10" t="s">
         <v>154</v>
       </c>
@@ -4046,12 +4028,12 @@
       <c r="D173" s="2" t="n">
         <v>0.84376</v>
       </c>
-      <c r="E173" s="25" t="s">
+      <c r="E173" s="11" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="18" t="s">
+      <c r="A174" s="17" t="s">
         <v>136</v>
       </c>
       <c r="C174" s="2" t="n">
@@ -4061,10 +4043,30 @@
         <v>0.85129</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="24" t="s">
+    <row r="176" customFormat="false" ht="572.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="10" t="s">
         <v>156</v>
       </c>
+      <c r="B176" s="2" t="n">
+        <v>0.852</v>
+      </c>
+      <c r="E176" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B177" s="2" t="n">
+        <v>0.857</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="17"/>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
results from 15 epoch mit-b1 and mit-b2
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="180">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -2458,6 +2458,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">9e-4_7e-4
 </t>
@@ -2467,6 +2468,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(9e-4_7e-4 change made to 0.1D + 0.9B)
 Segformer with mit_b1 encoder 
@@ -2490,9 +2492,305 @@
 (used LOAD_RESIZED = False)
 with grad_accu = 2, BS = 32    
 BS = 32 (train/valid/test)
-(2h 35m 24s)  
+(2h 36m 59s)  
 (Max GPU mem usage : 10716.875 MB)   </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-B TLo-SB-D TLo-SB-B TLo-S-D  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000225  | 0.165      | 0.100      | 0.764           | 0.550        | 0.094             | 0.238    0.141    0.713    0.056    0.872    0.104    0.914    0.102   | 0.184    0.072    0.283    0.015    0.349    0.024    0.288    0.016   | 0.633  0.468  0.520  | 0.114  0.084  0.083 
+2     | 0.000450  | 0.069      | 0.083      | 0.799           | 0.613        | 0.077             | 0.137    0.046    0.318    0.010    0.520    0.015    0.442    0.007   | 0.190    0.047    0.202    0.012    0.256    0.016    0.145    0.005   | 0.673  0.529  0.646  | 0.103  0.076  0.052 
+3     | 0.000900  | 0.066      | 0.079      | 0.816           | 0.638        | 0.066             | 0.152    0.037    0.273    0.010    0.422    0.013    0.289    0.006   | 0.179    0.046    0.182    0.012    0.242    0.021    0.109    0.004   | 0.682  0.544  0.680  | 0.071  0.077  0.049 
+4     | 0.000890  | 0.050      | 0.067      | 0.819           | 0.649        | 0.068             | 0.110    0.031    0.231    0.008    0.362    0.012    0.206    0.004   | 0.147    0.041    0.179    0.011    0.225    0.013    0.104    0.004   | 0.683  0.578  0.688  | 0.069  0.064  0.070 
+5     | 0.000862  | 0.044      | 0.079      | 0.826           | 0.654        | 0.059             | 0.092    0.028    0.211    0.008    0.332    0.011    0.190    0.004   | 0.190    0.042    0.179    0.011    0.226    0.015    0.103    0.004   | 0.685  0.566  0.703  | 0.060  0.071  0.047 
+6     | 0.000822  | 0.041      | 0.070      | 0.828           | 0.656        | 0.058             | 0.083    0.027    0.200    0.007    0.316    0.010    0.169    0.004   | 0.148    0.044    0.167    0.013    0.226    0.016    0.101    0.005   | 0.701  0.568  0.704  | 0.070  0.061  0.043 
+7     | 0.000778  | 0.036      | 0.082      | 0.823           | 0.657        | 0.066             | 0.071    0.025    0.187    0.007    0.297    0.010    0.158    0.003   | 0.211    0.039    0.167    0.011    0.213    0.014    0.096    0.004   | 0.701  0.575  0.706  | 0.085  0.073  0.041 
+8     | 0.000738  | 0.035      | 0.071      | 0.830           | 0.666        | 0.061             | 0.065    0.024    0.184    0.007    0.290    0.009    0.153    0.003   | 0.162    0.040    0.169    0.012    0.217    0.014    0.093    0.004   | 0.701  0.583  0.726  | 0.077  0.064  0.042 
+9     | 0.000710  | 0.034      | 0.071      | 0.843           | 0.686        | 0.053             | 0.063    0.024    0.181    0.007    0.289    0.009    0.149    0.003   | 0.171    0.038    0.164    0.011    0.212    0.013    0.086    0.004   | 0.713  0.604  0.745  | 0.059  0.060  0.040 
+10    | 0.000700  | 0.031      | 0.076      | 0.835           | 0.669        | 0.054             | 0.055    0.023    0.171    0.006    0.273    0.009    0.142    0.003   | 0.182    0.041    0.176    0.011    0.226    0.014    0.097    0.004   | 0.702  0.578  0.719  | 0.058  0.062  0.041 
+Confusion Matrix raw counts
+      LB    SB     S
+TP  2360  1806  1467
+FP   127   133   121
+FN   217   263    59
+TN  4592  5094  5649
+Confusion Matrix normalized per class
+       LB     SB      S
+TP  0.323  0.248  0.201
+FP  0.017  0.018  0.017
+FN  0.030  0.036  0.008
+TN  0.629  0.698  0.774
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.076      | 0.835           | 0.669        | 0.054             | 0.182    0.041    0.176    0.011    0.226    0.014    0.097    0.004   | 0.702  0.578  0.719  | 0.058  0.062  0.041 
+266     | 266     | 0.075      | 0.834           | 0.668        | 0.055             | 0.177    0.042    0.170    0.012    0.222    0.014    0.089    0.004   | 0.697  0.582  0.721  | 0.059  0.064  0.042 
+360     | 310     | 0.072      | 0.829           | 0.634        | 0.041             | 0.190    0.032    0.169    0.004    0.281    0.008    0.094    0.002   | 0.682  0.460  0.747  | 0.059  0.044  0.019 
+276     | 276     | 0.102      | 0.865           | 0.737        | 0.050             | 0.278    0.043    0.194    0.008    0.220    0.015    0.136    0.004   | 0.817  0.666  0.640  | 0.042  0.057  0.050 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">15 epoch from stable best model config
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+(15 epoch &amp; final_lr to 2.5e-4 changed from
+warmup&amp;cosdec,0.1LR pres,DL Lo(.5),.25PLo+.75SLo)
+Segformer with mit_b1 encoder 
+with presence head with dropout 0.4
+per class seg loss : 
+dice * 0.5 +  bce * 0.5
+total_loss = 0.25 * presence_loss + 0.75 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+Presence loss pos_weight = [60/40, 70/30, 75/25]
+On padded images
+With AdamW optim 
+1e-6 weight decay for presence head
+1e-4 weight_decay for other params except 
+                               bias &amp; norm
+On 384x384 images with 
+LR 1.25e-4, 2.5e-4, 5e-4, cos decay to 2.5e-4 for 15 epochs
+LR*0.1 for presence head
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+BS = 32 (train/valid/test)
+(3h 44m 18s)  
+(Max GPU mem usage : 10716.875 MB)   </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-B TLo-SB-D TLo-SB-B TLo-S-D  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000125  | 0.352      | 0.189      | 0.794           | 0.593        | 0.071             | 0.213    0.399    0.631    0.071    0.853    0.156    0.902    0.160   | 0.171    0.196    0.218    0.013    0.316    0.025    0.247    0.012   | 0.679  0.497  0.574  | 0.075  0.082  0.057 
+2     | 0.000250  | 0.131      | 0.129      | 0.836           | 0.672        | 0.055             | 0.119    0.135    0.228    0.010    0.391    0.015    0.282    0.005   | 0.156    0.120    0.159    0.015    0.211    0.021    0.098    0.004   | 0.714  0.585  0.718  | 0.069  0.060  0.038 
+3     | 0.000500  | 0.104      | 0.134      | 0.824           | 0.660        | 0.067             | 0.114    0.101    0.185    0.010    0.298    0.015    0.167    0.004   | 0.174    0.120    0.160    0.019    0.203    0.024    0.095    0.005   | 0.694  0.595  0.693  | 0.070  0.067  0.063 
+4     | 0.000496  | 0.087      | 0.116      | 0.843           | 0.691        | 0.056             | 0.086    0.087    0.162    0.010    0.260    0.014    0.136    0.004   | 0.133    0.110    0.147    0.016    0.190    0.023    0.090    0.005   | 0.731  0.607  0.740  | 0.062  0.070  0.036 
+5     | 0.000483  | 0.078      | 0.131      | 0.835           | 0.693        | 0.070             | 0.073    0.079    0.147    0.009    0.235    0.013    0.121    0.004   | 0.182    0.113    0.153    0.020    0.198    0.024    0.088    0.005   | 0.718  0.604  0.748  | 0.091  0.084  0.035 
+6     | 0.000463  | 0.072      | 0.130      | 0.843           | 0.688        | 0.054             | 0.063    0.076    0.139    0.009    0.225    0.012    0.113    0.004   | 0.177    0.114    0.153    0.018    0.195    0.023    0.087    0.005   | 0.714  0.619  0.735  | 0.057  0.061  0.044 
+7     | 0.000438  | 0.066      | 0.129      | 0.845           | 0.699        | 0.057             | 0.053    0.070    0.129    0.008    0.208    0.012    0.107    0.004   | 0.192    0.108    0.147    0.018    0.186    0.024    0.081    0.005   | 0.728  0.619  0.752  | 0.063  0.065  0.042 
+8     | 0.000407  | 0.063      | 0.127      | 0.852           | 0.705        | 0.050             | 0.049    0.068    0.126    0.008    0.201    0.011    0.103    0.003   | 0.179    0.110    0.145    0.017    0.189    0.023    0.081    0.005   | 0.729  0.624  0.756  | 0.058  0.055  0.037 
+9     | 0.000375  | 0.060      | 0.118      | 0.851           | 0.709        | 0.055             | 0.043    0.065    0.120    0.008    0.193    0.011    0.098    0.003   | 0.159    0.105    0.141    0.019    0.188    0.022    0.074    0.005   | 0.732  0.628  0.771  | 0.059  0.058  0.048 
+10    | 0.000343  | 0.056      | 0.117      | 0.854           | 0.717        | 0.054             | 0.038    0.062    0.114    0.007    0.184    0.010    0.095    0.003   | 0.161    0.102    0.143    0.017    0.176    0.025    0.071    0.005   | 0.735  0.647  0.783  | 0.058  0.068  0.036 
+11    | 0.000313  | 0.053      | 0.122      | 0.855           | 0.718        | 0.054             | 0.034    0.060    0.109    0.007    0.175    0.010    0.092    0.003   | 0.182    0.103    0.135    0.017    0.184    0.023    0.078    0.006   | 0.747  0.635  0.771  | 0.052  0.075  0.035 
+12    | 0.000287  | 0.049      | 0.123      | 0.859           | 0.720        | 0.049             | 0.029    0.056    0.103    0.006    0.166    0.009    0.086    0.003   | 0.175    0.106    0.149    0.019    0.182    0.024    0.074    0.005   | 0.741  0.647  0.774  | 0.051  0.062  0.034 
+13    | 0.000267  | 0.049      | 0.122      | 0.858           | 0.723        | 0.051             | 0.028    0.056    0.101    0.006    0.164    0.009    0.084    0.003   | 0.184    0.102    0.136    0.020    0.170    0.025    0.074    0.005   | 0.743  0.650  0.778  | 0.060  0.056  0.039 
+14    | 0.000254  | 0.046      | 0.130      | 0.853           | 0.711        | 0.052             | 0.022    0.054    0.098    0.006    0.157    0.009    0.084    0.003   | 0.195    0.109    0.147    0.019    0.186    0.026    0.080    0.006   | 0.727  0.636  0.771  | 0.053  0.063  0.039 
+15    | 0.000250  | 0.046      | 0.125      | 0.852           | 0.713        | 0.056             | 0.025    0.053    0.098    0.006    0.157    0.009    0.084    0.003   | 0.186    0.104    0.137    0.019    0.179    0.025    0.078    0.005   | 0.739  0.634  0.765  | 0.061  0.071  0.034 
+Confusion Matrix raw counts
+      LB    SB     S
+TP  2484  1966  1427
+FP   231   246    73
+FN    93   103    99
+TN  4488  4981  5697
+Confusion Matrix normalized per class
+       LB     SB      S
+TP  0.340  0.269  0.196
+FP  0.032  0.034  0.010
+FN  0.013  0.014  0.014
+TN  0.615  0.683  0.781
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.125      | 0.852           | 0.713        | 0.056             | 0.186    0.104    0.137    0.019    0.179    0.025    0.078    0.005   | 0.739  0.634  0.765  | 0.061  0.071  0.034 
+266     | 266     | 0.120      | 0.852           | 0.716        | 0.057             | 0.172    0.103    0.134    0.020    0.175    0.026    0.065    0.005   | 0.735  0.639  0.782  | 0.063  0.074  0.034 
+360     | 310     | 0.154      | 0.830           | 0.655        | 0.053             | 0.289    0.109    0.110    0.007    0.207    0.014    0.097    0.004   | 0.731  0.551  0.657  | 0.063  0.053  0.043 
+276     | 276     | 0.185      | 0.871           | 0.742        | 0.043             | 0.348    0.130    0.168    0.016    0.194    0.034    0.098    0.007   | 0.813  0.656  0.704  | 0.040  0.056  0.031 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA Epoch 12</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">15 epoch same LR from stable best model config
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+(15 epoch changed from
+warmup&amp;cosdec,0.1LR pres,DL Lo(.5),.25PLo+.75SLo)
+Segformer with mit_b1 encoder 
+with presence head with dropout 0.4
+per class seg loss : 
+dice * 0.5 +  bce * 0.5
+total_loss = 0.25 * presence_loss + 0.75 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+Presence loss pos_weight = [60/40, 70/30, 75/25]
+On padded images
+With AdamW optim 
+1e-6 weight decay for presence head
+1e-4 weight_decay for other params except 
+                               bias &amp; norm
+On 384x384 images with 
+LR 1.25e-4, 2.5e-4, 5e-4, cos decay to 3e-4 for 15 epochs
+LR*0.1 for presence head
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+BS = 32 (train/valid/test)
+(3h 42m 36s)  
+(Max GPU mem usage : 10716.875 MB)   </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-B TLo-SB-D TLo-SB-B TLo-S-D  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000125  | 0.351      | 0.190      | 0.800           | 0.592        | 0.061             | 0.209    0.399    0.629    0.070    0.854    0.156    0.902    0.159   | 0.161    0.200    0.226    0.013    0.322    0.026    0.249    0.012   | 0.674  0.495  0.574  | 0.063  0.068  0.052 
+2     | 0.000250  | 0.130      | 0.135      | 0.831           | 0.661        | 0.056             | 0.119    0.134    0.226    0.010    0.389    0.015    0.282    0.005   | 0.172    0.123    0.165    0.017    0.210    0.022    0.097    0.004   | 0.698  0.575  0.720  | 0.075  0.055  0.037 
+3     | 0.000500  | 0.106      | 0.126      | 0.836           | 0.684        | 0.064             | 0.116    0.103    0.189    0.011    0.301    0.015    0.173    0.004   | 0.167    0.113    0.149    0.016    0.197    0.024    0.087    0.005   | 0.718  0.602  0.751  | 0.073  0.067  0.051 
+4     | 0.000497  | 0.086      | 0.119      | 0.841           | 0.690        | 0.059             | 0.085    0.086    0.160    0.010    0.258    0.014    0.132    0.004   | 0.145    0.110    0.143    0.015    0.191    0.022    0.091    0.006   | 0.726  0.613  0.727  | 0.063  0.061  0.054 
+5     | 0.000487  | 0.076      | 0.131      | 0.836           | 0.689        | 0.066             | 0.070    0.078    0.145    0.009    0.232    0.013    0.120    0.004   | 0.192    0.111    0.146    0.019    0.195    0.028    0.084    0.005   | 0.720  0.604  0.749  | 0.067  0.078  0.053 
+6     | 0.000471  | 0.073      | 0.121      | 0.848           | 0.693        | 0.049             | 0.066    0.075    0.140    0.009    0.223    0.012    0.114    0.004   | 0.151    0.111    0.150    0.018    0.192    0.022    0.083    0.005   | 0.711  0.626  0.756  | 0.059  0.052  0.034 
+7     | 0.000450  | 0.067      | 0.127      | 0.840           | 0.692        | 0.061             | 0.053    0.071    0.131    0.008    0.210    0.012    0.107    0.003   | 0.188    0.107    0.141    0.017    0.187    0.024    0.077    0.005   | 0.721  0.611  0.760  | 0.075  0.072  0.037 
+8     | 0.000426  | 0.064      | 0.124      | 0.854           | 0.709        | 0.050             | 0.051    0.069    0.128    0.008    0.205    0.011    0.105    0.003   | 0.165    0.110    0.153    0.017    0.190    0.021    0.084    0.005   | 0.727  0.635  0.757  | 0.051  0.062  0.037 
+9     | 0.000400  | 0.060      | 0.119      | 0.856           | 0.720        | 0.053             | 0.046    0.065    0.120    0.007    0.193    0.011    0.099    0.003   | 0.158    0.106    0.141    0.017    0.188    0.023    0.076    0.005   | 0.745  0.637  0.769  | 0.060  0.057  0.043 
+10    | 0.000374  | 0.057      | 0.119      | 0.849           | 0.711        | 0.060             | 0.039    0.063    0.116    0.007    0.186    0.010    0.096    0.003   | 0.161    0.106    0.142    0.017    0.183    0.022    0.083    0.005   | 0.730  0.638  0.766  | 0.073  0.078  0.028 
+11    | 0.000350  | 0.054      | 0.130      | 0.852           | 0.710        | 0.053             | 0.035    0.060    0.109    0.007    0.177    0.010    0.092    0.003   | 0.209    0.104    0.140    0.018    0.176    0.023    0.082    0.005   | 0.735  0.638  0.756  | 0.059  0.062  0.038 
+12    | 0.000329  | 0.050      | 0.135      | 0.850           | 0.705        | 0.054             | 0.031    0.057    0.103    0.006    0.168    0.010    0.088    0.003   | 0.199    0.113    0.159    0.022    0.190    0.026    0.078    0.005   | 0.725  0.635  0.766  | 0.053  0.061  0.046 
+13    | 0.000313  | 0.049      | 0.121      | 0.855           | 0.723        | 0.057             | 0.028    0.056    0.102    0.007    0.164    0.009    0.086    0.003   | 0.181    0.101    0.132    0.019    0.173    0.027    0.076    0.006   | 0.747  0.656  0.765  | 0.055  0.063  0.054 
+14    | 0.000303  | 0.048      | 0.123      | 0.856           | 0.725        | 0.057             | 0.026    0.055    0.101    0.007    0.161    0.009    0.087    0.003   | 0.187    0.101    0.132    0.018    0.179    0.025    0.074    0.006   | 0.747  0.646  0.775  | 0.061  0.067  0.045 
+15    | 0.000300  | 0.048      | 0.127      | 0.860           | 0.730        | 0.053             | 0.028    0.055    0.100    0.006    0.160    0.009    0.087    0.003   | 0.199    0.103    0.137    0.019    0.179    0.024    0.081    0.005   | 0.751  0.659  0.776  | 0.058  0.071  0.029 
+Confusion Matrix raw counts
+      LB    SB     S
+TP  2474  1940  1430
+FP   168   168    58
+FN   103   129    96
+TN  4551  5059  5712
+Confusion Matrix normalized per class
+       LB     SB      S
+TP  0.339  0.266  0.196
+FP  0.023  0.023  0.008
+FN  0.014  0.018  0.013
+TN  0.624  0.693  0.783
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.127      | 0.860           | 0.730        | 0.053             | 0.199    0.103    0.137    0.019    0.179    0.024    0.081    0.005   | 0.751  0.659  0.776  | 0.058  0.071  0.029 
+266     | 266     | 0.125      | 0.861           | 0.734        | 0.055             | 0.191    0.103    0.131    0.020    0.173    0.025    0.070    0.005   | 0.750  0.664  0.787  | 0.060  0.075  0.029 
+360     | 310     | 0.139      | 0.840           | 0.659        | 0.039             | 0.246    0.104    0.131    0.007    0.201    0.014    0.084    0.004   | 0.699  0.571  0.727  | 0.047  0.049  0.023 
+276     | 276     | 0.175      | 0.881           | 0.761        | 0.039             | 0.311    0.130    0.163    0.017    0.188    0.033    0.104    0.008   | 0.831  0.685  0.685  | 0.045  0.042  0.028 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mitb2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+(mitb2 change from
+'15 epoch same LR from stable best model config’)
+Segformer with mit_b2 encoder 
+with presence head with dropout 0.4
+per class seg loss : 
+dice * 0.5 +  bce * 0.5
+total_loss = 0.25 * presence_loss + 0.75 * seg_loss
+(seg_loss is presence gated avg of 
+per class seg loss)
+presence_gate = 
+       Presence_true.mean(dim=0) + 1e-3
+Presence loss pos_weight = [60/40, 70/30, 75/25]
+On padded images
+With AdamW optim 
+1e-6 weight decay for presence head
+1e-4 weight_decay for other params except 
+                               bias &amp; norm
+On 384x384 images with 
+LR 1.25e-4, 2.5e-4, 5e-4, cos decay to 3e-4 for 15 epochs
+LR*0.1 for presence head
+(used LOAD_RESIZED = False)
+with grad_accu = 2, BS = 32    
+BS = 32 (train/valid/test)
+(5h 1m 10s)  
+(Max GPU mem usage : 14396.875 MB)   </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch | LR        | Train Loss | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | TLo-Pres TLo-Seg  TLo-LB-D TLo-LB-B TLo-SB-D TLo-SB-B TLo-S-D  TLo-S-B | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+1     | 0.000125  | 0.364      | 0.177      | 0.811           | 0.621        | 0.062             | 0.201    0.418    0.775    0.155    0.846    0.146    0.810    0.096   | 0.149    0.186    0.277    0.016    0.302    0.025    0.170    0.005   | 0.671  0.520  0.668  | 0.072  0.069  0.046 
+2     | 0.000250  | 0.120      | 0.142      | 0.822           | 0.653        | 0.065             | 0.108    0.124    0.244    0.010    0.357    0.015    0.205    0.004   | 0.202    0.122    0.170    0.019    0.211    0.022    0.104    0.005   | 0.694  0.567  0.729  | 0.090  0.075  0.031 
+3     | 0.000500  | 0.098      | 0.129      | 0.839           | 0.677        | 0.054             | 0.106    0.095    0.180    0.010    0.280    0.014    0.146    0.004   | 0.193    0.107    0.146    0.014    0.194    0.022    0.080    0.005   | 0.710  0.595  0.732  | 0.058  0.059  0.044 
+4     | 0.000497  | 0.082      | 0.121      | 0.842           | 0.692        | 0.058             | 0.082    0.082    0.155    0.009    0.243    0.013    0.119    0.004   | 0.139    0.115    0.154    0.016    0.201    0.022    0.084    0.005   | 0.725  0.605  0.751  | 0.057  0.062  0.057 
+5     | 0.000487  | 0.071      | 0.143      | 0.831           | 0.672        | 0.062             | 0.064    0.074    0.139    0.008    0.219    0.012    0.111    0.004   | 0.238    0.112    0.154    0.021    0.200    0.030    0.087    0.006   | 0.698  0.587  0.757  | 0.079  0.073  0.035 
+6     | 0.000471  | 0.069      | 0.124      | 0.842           | 0.700        | 0.063             | 0.060    0.072    0.137    0.008    0.215    0.012    0.104    0.004   | 0.185    0.104    0.136    0.016    0.183    0.024    0.086    0.005   | 0.736  0.627  0.748  | 0.067  0.068  0.055 
+7     | 0.000450  | 0.062      | 0.115      | 0.858           | 0.712        | 0.045             | 0.051    0.065    0.122    0.007    0.194    0.011    0.096    0.003   | 0.145    0.105    0.145    0.016    0.190    0.023    0.074    0.005   | 0.731  0.625  0.786  | 0.051  0.057  0.028 
+8     | 0.000426  | 0.058      | 0.123      | 0.854           | 0.713        | 0.052             | 0.044    0.063    0.118    0.007    0.186    0.011    0.096    0.003   | 0.177    0.105    0.141    0.016    0.181    0.026    0.078    0.006   | 0.736  0.645  0.747  | 0.061  0.059  0.038 
+9     | 0.000400  | 0.058      | 0.128      | 0.842           | 0.693        | 0.060             | 0.042    0.063    0.117    0.007    0.186    0.011    0.093    0.003   | 0.200    0.104    0.137    0.017    0.181    0.023    0.086    0.005   | 0.732  0.621  0.745  | 0.067  0.063  0.049 
+10    | 0.000374  | 0.054      | 0.119      | 0.850           | 0.710        | 0.057             | 0.036    0.060    0.110    0.007    0.177    0.010    0.091    0.003   | 0.174    0.101    0.137    0.017    0.181    0.024    0.074    0.006   | 0.733  0.632  0.781  | 0.067  0.070  0.035 
+11    | 0.000350  | 0.050      | 0.116      | 0.861           | 0.723        | 0.047             | 0.031    0.057    0.104    0.007    0.166    0.010    0.085    0.003   | 0.156    0.103    0.133    0.017    0.182    0.024    0.082    0.006   | 0.750  0.642  0.768  | 0.068  0.052  0.022 
+12    | 0.000329  | 0.048      | 0.115      | 0.857           | 0.729        | 0.057             | 0.028    0.055    0.102    0.006    0.161    0.010    0.083    0.003   | 0.155    0.101    0.130    0.017    0.183    0.026    0.074    0.006   | 0.753  0.648  0.780  | 0.061  0.074  0.036 
+13    | 0.000313  | 0.048      | 0.117      | 0.860           | 0.730        | 0.052             | 0.028    0.055    0.101    0.006    0.160    0.009    0.082    0.003   | 0.163    0.101    0.136    0.019    0.179    0.026    0.071    0.005   | 0.751  0.653  0.784  | 0.058  0.066  0.032 
+14    | 0.000303  | 0.046      | 0.136      | 0.843           | 0.705        | 0.065             | 0.026    0.053    0.098    0.006    0.156    0.009    0.082    0.003   | 0.233    0.103    0.136    0.019    0.179    0.027    0.074    0.007   | 0.733  0.632  0.770  | 0.073  0.072  0.050 
+15    | 0.000300  | 0.045      | 0.123      | 0.855           | 0.725        | 0.059             | 0.022    0.052    0.096    0.006    0.154    0.009    0.080    0.003   | 0.182    0.103    0.134    0.020    0.185    0.027    0.074    0.006   | 0.746  0.639  0.792  | 0.074  0.059  0.043 
+Confusion Matrix raw counts
+      LB    SB     S
+TP  2500  1994  1452
+FP   216   263    65
+FN    77    75    74
+TN  4503  4964  5705
+Confusion Matrix normalized per class
+       LB     SB      S
+TP  0.343  0.273  0.199
+FP  0.030  0.036  0.009
+FN  0.011  0.010  0.010
+TN  0.617  0.680  0.782
+Slice_W | Slice_H | Valid Loss | Combined Metric | Dice Overall | Hausdorff Overall | VLo-Pres VLo-Seg  VLo-LB-D VLo-LB-B VLo-SB-D VLo-SB-B VLo-S-D  VLo-S-B | D-LB   D-SB   D-S    | H-LB   H-SB   H-S   
+----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------
+-1      | -1      | 0.123      | 0.855           | 0.725        | 0.059             | 0.182    0.103    0.134    0.020    0.185    0.027    0.074    0.006   | 0.746  0.639  0.792  | 0.074  0.059  0.043 
+266     | 266     | 0.122      | 0.854           | 0.724        | 0.060             | 0.176    0.104    0.132    0.021    0.184    0.029    0.063    0.006   | 0.741  0.640  0.796  | 0.073  0.061  0.046 
+360     | 310     | 0.116      | 0.856           | 0.705        | 0.043             | 0.188    0.092    0.097    0.007    0.208    0.013    0.062    0.003   | 0.736  0.592  0.788  | 0.057  0.055  0.017 
+276     | 276     | 0.163      | 0.874           | 0.775        | 0.060             | 0.301    0.118    0.148    0.014    0.170    0.031    0.099    0.008   | 0.839  0.702  0.729  | 0.113  0.039  0.028 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMA Epoch 11</t>
   </si>
 </sst>
 </file>
@@ -2502,7 +2800,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2541,17 +2839,6 @@
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2602,7 +2889,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2695,7 +2982,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2703,8 +2990,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2890,10 +3181,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K193"/>
+  <dimension ref="A1:K208"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A185" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A191" activeCellId="0" sqref="A191"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A203" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A211" activeCellId="0" sqref="A211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4510,14 +4801,14 @@
       <c r="B186" s="14" t="n">
         <v>0.858467</v>
       </c>
-      <c r="C186" s="23" t="n">
+      <c r="C186" s="2" t="n">
         <v>0.8606</v>
       </c>
       <c r="D186" s="2" t="n">
         <v>0.85173</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="370.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="561.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="10" t="s">
         <v>164</v>
       </c>
@@ -4530,7 +4821,7 @@
       <c r="D188" s="2" t="n">
         <v>0.83834</v>
       </c>
-      <c r="E188" s="24" t="s">
+      <c r="E188" s="11" t="s">
         <v>165</v>
       </c>
     </row>
@@ -4570,9 +4861,149 @@
         <v>0.83963</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="370.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="25" t="s">
+    <row r="193" customFormat="false" ht="561.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="10" t="s">
         <v>168</v>
+      </c>
+      <c r="B193" s="2" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="E193" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="673.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B196" s="2" t="n">
+        <v>0.852</v>
+      </c>
+      <c r="C196" s="2" t="n">
+        <v>0.85213</v>
+      </c>
+      <c r="D196" s="2" t="n">
+        <v>0.84335</v>
+      </c>
+      <c r="E196" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B197" s="2" t="n">
+        <v>0.859</v>
+      </c>
+      <c r="C197" s="2" t="n">
+        <v>0.84739</v>
+      </c>
+      <c r="D197" s="2" t="n">
+        <v>0.83395</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C198" s="23" t="n">
+        <v>0.86286</v>
+      </c>
+      <c r="D198" s="2" t="n">
+        <v>0.85721</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C199" s="2" t="n">
+        <v>0.86225</v>
+      </c>
+      <c r="D199" s="2" t="n">
+        <v>0.85397</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="415.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B202" s="2" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="C202" s="2" t="n">
+        <v>0.8518</v>
+      </c>
+      <c r="D202" s="2" t="n">
+        <v>0.84582</v>
+      </c>
+      <c r="E202" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C203" s="2" t="n">
+        <v>0.86222</v>
+      </c>
+      <c r="D203" s="2" t="n">
+        <v>0.85247</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="415.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B205" s="2" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="C205" s="2" t="n">
+        <v>0.85644</v>
+      </c>
+      <c r="D205" s="2" t="n">
+        <v>0.84595</v>
+      </c>
+      <c r="E205" s="24" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B206" s="2" t="n">
+        <v>0.861</v>
+      </c>
+      <c r="C206" s="2" t="n">
+        <v>0.85413</v>
+      </c>
+      <c r="D206" s="2" t="n">
+        <v>0.84303</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C207" s="26" t="n">
+        <v>0.86445</v>
+      </c>
+      <c r="D207" s="2" t="n">
+        <v>0.85588</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="C208" s="2" t="n">
+        <v>0.86303</v>
+      </c>
+      <c r="D208" s="2" t="n">
+        <v>0.85492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>